<commit_message>
Updates in the world model, including process emissions
</commit_message>
<xml_diff>
--- a/models/14sectors_cat/climate.xlsx
+++ b/models/14sectors_cat/climate.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="9945" tabRatio="500"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="9945" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Global" sheetId="1" r:id="rId1"/>
@@ -166,6 +166,7 @@
     <definedName name="initial_SF6_conc" localSheetId="1">World!$C$46</definedName>
     <definedName name="land_thickness" localSheetId="1">World!$G$23</definedName>
     <definedName name="last_historical_RF_year" localSheetId="1">World!$C$90</definedName>
+    <definedName name="last_year_process_emissions" localSheetId="1">World!$AD$202</definedName>
     <definedName name="layer_depth" localSheetId="1">World!$C$17:$C$20</definedName>
     <definedName name="mineral_aerosols_and_land_RF" localSheetId="1">World!$C$91</definedName>
     <definedName name="mixed_layer_depth" localSheetId="1">World!$C$15</definedName>
@@ -192,6 +193,7 @@
     <definedName name="preindustrial_HFC_conc" localSheetId="1">World!$C$61</definedName>
     <definedName name="preindustrial_PFC_conc" localSheetId="1">World!$C$44</definedName>
     <definedName name="preindustrial_SF6_conc" localSheetId="1">World!$C$48</definedName>
+    <definedName name="process_emissions_intensity" localSheetId="1">World!$C$203:$AD$203</definedName>
     <definedName name="ref_buffer_factor" localSheetId="1">World!$C$12</definedName>
     <definedName name="reference_CH4_time_constant" localSheetId="1">World!$C$35</definedName>
     <definedName name="reference_CO2_radiative_forcing" localSheetId="1">World!$G$18</definedName>
@@ -222,6 +224,7 @@
     <definedName name="year_emissions" localSheetId="3">Catalonia!$D$1:$P$1</definedName>
     <definedName name="year_emissions" localSheetId="2">Europe!$D$1:$P$1</definedName>
     <definedName name="year_emissions" localSheetId="1">World!$D$94:$P$94</definedName>
+    <definedName name="years_process_emissions" localSheetId="1">World!$C$202:$AD$202</definedName>
   </definedNames>
   <calcPr calcId="125725" iterateDelta="1E-4"/>
   <extLst>
@@ -1449,7 +1452,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="734" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="739" uniqueCount="219">
   <si>
     <t>Global Warming Potentials</t>
   </si>
@@ -2094,6 +2097,18 @@
   </si>
   <si>
     <t>solid sorbent</t>
+  </si>
+  <si>
+    <t>Historic carbon intensity process emissions</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Process emission intensity</t>
+  </si>
+  <si>
+    <t>GtCO2/T$</t>
   </si>
 </sst>
 </file>
@@ -3394,6 +3409,8 @@
     <xf numFmtId="9" fontId="9" fillId="0" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3402,6 +3419,33 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="16" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3412,14 +3456,32 @@
     <xf numFmtId="0" fontId="3" fillId="16" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3436,65 +3498,18 @@
     <xf numFmtId="0" fontId="2" fillId="12" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
@@ -3608,7 +3623,7 @@
         <xdr:cNvPr id="2" name="CustomShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3981,8 +3996,8 @@
   </sheetPr>
   <dimension ref="A1:FI57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="H49" sqref="H49"/>
+    <sheetView topLeftCell="A40" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A60" sqref="A60:XFD62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -3997,11 +4012,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:165">
-      <c r="A1" s="192" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="192"/>
-      <c r="C1" s="192"/>
+      <c r="A1" s="194" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="194"/>
+      <c r="C1" s="194"/>
       <c r="E1" s="1"/>
       <c r="F1" s="2"/>
       <c r="G1" s="3"/>
@@ -4572,11 +4587,11 @@
       </c>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="193" t="s">
+      <c r="A17" s="195" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="193"/>
-      <c r="C17" s="193"/>
+      <c r="B17" s="195"/>
+      <c r="C17" s="195"/>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="17" t="s">
@@ -4950,12 +4965,12 @@
       </c>
     </row>
     <row r="48" spans="1:4">
-      <c r="A48" s="194" t="s">
+      <c r="A48" s="196" t="s">
         <v>184</v>
       </c>
-      <c r="B48" s="194"/>
-      <c r="C48" s="194"/>
-      <c r="D48" s="194"/>
+      <c r="B48" s="196"/>
+      <c r="C48" s="196"/>
+      <c r="D48" s="196"/>
     </row>
     <row r="49" spans="1:7">
       <c r="A49" s="17"/>
@@ -5001,16 +5016,16 @@
       <c r="G52" s="187"/>
     </row>
     <row r="54" spans="1:7">
-      <c r="A54" s="225" t="s">
+      <c r="A54" s="197" t="s">
         <v>208</v>
       </c>
-      <c r="B54" s="225"/>
-      <c r="C54" s="225"/>
-      <c r="D54" s="225"/>
+      <c r="B54" s="197"/>
+      <c r="C54" s="197"/>
+      <c r="D54" s="197"/>
     </row>
     <row r="55" spans="1:7">
-      <c r="A55" s="226"/>
-      <c r="B55" s="226"/>
+      <c r="A55" s="193"/>
+      <c r="B55" s="193"/>
       <c r="C55" s="19" t="s">
         <v>206</v>
       </c>
@@ -5064,10 +5079,10 @@
   <sheetPr>
     <tabColor rgb="FF9DC3E6"/>
   </sheetPr>
-  <dimension ref="A1:AJ199"/>
+  <dimension ref="A1:AJ203"/>
   <sheetViews>
-    <sheetView topLeftCell="A154" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E175" sqref="E175"/>
+    <sheetView tabSelected="1" topLeftCell="O178" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="AD202" sqref="AD202"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -5091,16 +5106,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="198" t="s">
+      <c r="A1" s="223" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="198"/>
-      <c r="C1" s="198"/>
-      <c r="E1" s="198" t="s">
+      <c r="B1" s="223"/>
+      <c r="C1" s="223"/>
+      <c r="E1" s="223" t="s">
         <v>49</v>
       </c>
-      <c r="F1" s="198"/>
-      <c r="G1" s="198"/>
+      <c r="F1" s="223"/>
+      <c r="G1" s="223"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="27" t="s">
@@ -5172,10 +5187,10 @@
       <c r="C5" s="35">
         <v>85.177099999999996</v>
       </c>
-      <c r="E5" s="199" t="s">
+      <c r="E5" s="224" t="s">
         <v>62</v>
       </c>
-      <c r="F5" s="199"/>
+      <c r="F5" s="224"/>
       <c r="G5" s="36"/>
     </row>
     <row r="6" spans="1:11">
@@ -5276,10 +5291,10 @@
       <c r="C10" s="42">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="E10" s="199" t="s">
+      <c r="E10" s="224" t="s">
         <v>73</v>
       </c>
-      <c r="F10" s="199"/>
+      <c r="F10" s="224"/>
       <c r="G10" s="43"/>
     </row>
     <row r="11" spans="1:11">
@@ -5374,10 +5389,10 @@
       </c>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="200" t="s">
+      <c r="A16" s="225" t="s">
         <v>82</v>
       </c>
-      <c r="B16" s="200"/>
+      <c r="B16" s="225"/>
       <c r="C16" s="50"/>
     </row>
     <row r="17" spans="1:8">
@@ -5390,11 +5405,11 @@
       <c r="C17" s="41">
         <v>300</v>
       </c>
-      <c r="E17" s="201" t="s">
+      <c r="E17" s="218" t="s">
         <v>83</v>
       </c>
-      <c r="F17" s="201"/>
-      <c r="G17" s="201"/>
+      <c r="F17" s="218"/>
+      <c r="G17" s="218"/>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="27" t="s">
@@ -5570,12 +5585,12 @@
       </c>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="202" t="s">
+      <c r="A29" s="219" t="s">
         <v>104</v>
       </c>
-      <c r="B29" s="202"/>
-      <c r="C29" s="202"/>
-      <c r="D29" s="202"/>
+      <c r="B29" s="219"/>
+      <c r="C29" s="219"/>
+      <c r="D29" s="219"/>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="67" t="s">
@@ -5587,7 +5602,7 @@
       <c r="C30" s="68">
         <v>1726</v>
       </c>
-      <c r="D30" s="203" t="s">
+      <c r="D30" s="220" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5601,7 +5616,7 @@
       <c r="C31" s="70">
         <v>2213</v>
       </c>
-      <c r="D31" s="203"/>
+      <c r="D31" s="220"/>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="69" t="s">
@@ -5613,7 +5628,7 @@
       <c r="C32" s="70">
         <v>50</v>
       </c>
-      <c r="D32" s="203"/>
+      <c r="D32" s="220"/>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="71" t="s">
@@ -5625,7 +5640,7 @@
       <c r="C33" s="72">
         <v>0</v>
       </c>
-      <c r="D33" s="203"/>
+      <c r="D33" s="220"/>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="69" t="s">
@@ -5637,7 +5652,7 @@
       <c r="C34" s="70">
         <v>1</v>
       </c>
-      <c r="D34" s="203"/>
+      <c r="D34" s="220"/>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="69" t="s">
@@ -5649,7 +5664,7 @@
       <c r="C35" s="73">
         <v>8.5</v>
       </c>
-      <c r="D35" s="203"/>
+      <c r="D35" s="220"/>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="69" t="s">
@@ -5661,7 +5676,7 @@
       <c r="C36" s="73">
         <v>0.88</v>
       </c>
-      <c r="D36" s="203"/>
+      <c r="D36" s="220"/>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="69" t="s">
@@ -5673,7 +5688,7 @@
       <c r="C37" s="73">
         <v>0.08</v>
       </c>
-      <c r="D37" s="203"/>
+      <c r="D37" s="220"/>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="74" t="s">
@@ -5685,7 +5700,7 @@
       <c r="C38" s="76">
         <v>1</v>
       </c>
-      <c r="D38" s="203"/>
+      <c r="D38" s="220"/>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="67" t="s">
@@ -5697,7 +5712,7 @@
       <c r="C39" s="77">
         <v>11</v>
       </c>
-      <c r="D39" s="204" t="s">
+      <c r="D39" s="221" t="s">
         <v>5</v>
       </c>
     </row>
@@ -5711,7 +5726,7 @@
       <c r="C40" s="78">
         <v>312.3</v>
       </c>
-      <c r="D40" s="204"/>
+      <c r="D40" s="221"/>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="74" t="s">
@@ -5723,7 +5738,7 @@
       <c r="C41" s="76">
         <v>117</v>
       </c>
-      <c r="D41" s="204"/>
+      <c r="D41" s="221"/>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="67" t="s">
@@ -5735,7 +5750,7 @@
       <c r="C42" s="77">
         <v>76</v>
       </c>
-      <c r="D42" s="205" t="s">
+      <c r="D42" s="222" t="s">
         <v>125</v>
       </c>
     </row>
@@ -5749,7 +5764,7 @@
       <c r="C43" s="70">
         <v>50000</v>
       </c>
-      <c r="D43" s="205"/>
+      <c r="D43" s="222"/>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="69" t="s">
@@ -5761,7 +5776,7 @@
       <c r="C44" s="70">
         <v>40</v>
       </c>
-      <c r="D44" s="205"/>
+      <c r="D44" s="222"/>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="74" t="s">
@@ -5773,7 +5788,7 @@
       <c r="C45" s="79">
         <v>0.09</v>
       </c>
-      <c r="D45" s="205"/>
+      <c r="D45" s="222"/>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="67" t="s">
@@ -5785,7 +5800,7 @@
       <c r="C46" s="80">
         <v>3.47</v>
       </c>
-      <c r="D46" s="206" t="s">
+      <c r="D46" s="214" t="s">
         <v>7</v>
       </c>
     </row>
@@ -5799,7 +5814,7 @@
       <c r="C47" s="70">
         <v>3200</v>
       </c>
-      <c r="D47" s="206"/>
+      <c r="D47" s="214"/>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="69" t="s">
@@ -5811,7 +5826,7 @@
       <c r="C48" s="70">
         <v>0</v>
       </c>
-      <c r="D48" s="206"/>
+      <c r="D48" s="214"/>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="81" t="s">
@@ -5823,7 +5838,7 @@
       <c r="C49" s="83">
         <v>0.56999999999999995</v>
       </c>
-      <c r="D49" s="206"/>
+      <c r="D49" s="214"/>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="84" t="s">
@@ -5991,11 +6006,11 @@
       </c>
     </row>
     <row r="64" spans="1:4">
-      <c r="A64" s="207" t="s">
+      <c r="A64" s="215" t="s">
         <v>140</v>
       </c>
-      <c r="B64" s="207"/>
-      <c r="C64" s="207"/>
+      <c r="B64" s="215"/>
+      <c r="C64" s="215"/>
     </row>
     <row r="65" spans="1:36">
       <c r="A65" s="69" t="s">
@@ -6454,7 +6469,7 @@
       <c r="A85" s="51" t="s">
         <v>158</v>
       </c>
-      <c r="B85" s="208" t="s">
+      <c r="B85" s="216" t="s">
         <v>85</v>
       </c>
       <c r="C85" s="108">
@@ -6492,7 +6507,7 @@
       <c r="A86" s="51" t="s">
         <v>159</v>
       </c>
-      <c r="B86" s="208"/>
+      <c r="B86" s="216"/>
       <c r="C86" s="108">
         <v>-0.71328999999999998</v>
       </c>
@@ -6528,7 +6543,7 @@
       <c r="A87" s="51" t="s">
         <v>160</v>
       </c>
-      <c r="B87" s="208"/>
+      <c r="B87" s="216"/>
       <c r="C87" s="108">
         <v>-0.75124999999999997</v>
       </c>
@@ -6564,7 +6579,7 @@
       <c r="A88" s="51" t="s">
         <v>161</v>
       </c>
-      <c r="B88" s="208"/>
+      <c r="B88" s="216"/>
       <c r="C88" s="108">
         <v>-0.69615000000000005</v>
       </c>
@@ -6665,7 +6680,7 @@
       </c>
     </row>
     <row r="95" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A95" s="209" t="s">
+      <c r="A95" s="217" t="s">
         <v>165</v>
       </c>
       <c r="B95" s="210" t="s">
@@ -6715,7 +6730,7 @@
       </c>
     </row>
     <row r="96" spans="1:16">
-      <c r="A96" s="209"/>
+      <c r="A96" s="217"/>
       <c r="B96" s="210"/>
       <c r="C96" s="19" t="s">
         <v>167</v>
@@ -6761,7 +6776,7 @@
       </c>
     </row>
     <row r="97" spans="1:16">
-      <c r="A97" s="209"/>
+      <c r="A97" s="217"/>
       <c r="B97" s="210"/>
       <c r="C97" s="19" t="s">
         <v>168</v>
@@ -6807,7 +6822,7 @@
       </c>
     </row>
     <row r="98" spans="1:16">
-      <c r="A98" s="209"/>
+      <c r="A98" s="217"/>
       <c r="B98" s="210"/>
       <c r="C98" s="123" t="s">
         <v>169</v>
@@ -6853,7 +6868,7 @@
       </c>
     </row>
     <row r="99" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A99" s="211" t="s">
+      <c r="A99" s="209" t="s">
         <v>170</v>
       </c>
       <c r="B99" s="210" t="s">
@@ -6906,7 +6921,7 @@
       </c>
     </row>
     <row r="100" spans="1:16">
-      <c r="A100" s="211"/>
+      <c r="A100" s="209"/>
       <c r="B100" s="210"/>
       <c r="C100" s="19" t="s">
         <v>167</v>
@@ -6955,7 +6970,7 @@
       </c>
     </row>
     <row r="101" spans="1:16">
-      <c r="A101" s="211"/>
+      <c r="A101" s="209"/>
       <c r="B101" s="210"/>
       <c r="C101" s="19" t="s">
         <v>168</v>
@@ -7004,7 +7019,7 @@
       </c>
     </row>
     <row r="102" spans="1:16">
-      <c r="A102" s="211"/>
+      <c r="A102" s="209"/>
       <c r="B102" s="210"/>
       <c r="C102" s="123" t="s">
         <v>169</v>
@@ -7053,10 +7068,10 @@
       </c>
     </row>
     <row r="103" spans="1:16">
-      <c r="A103" s="212" t="s">
+      <c r="A103" s="211" t="s">
         <v>172</v>
       </c>
-      <c r="B103" s="213" t="s">
+      <c r="B103" s="212" t="s">
         <v>173</v>
       </c>
       <c r="C103" s="115" t="s">
@@ -7103,8 +7118,8 @@
       </c>
     </row>
     <row r="104" spans="1:16">
-      <c r="A104" s="212"/>
-      <c r="B104" s="213"/>
+      <c r="A104" s="211"/>
+      <c r="B104" s="212"/>
       <c r="C104" s="19" t="s">
         <v>167</v>
       </c>
@@ -7149,8 +7164,8 @@
       </c>
     </row>
     <row r="105" spans="1:16">
-      <c r="A105" s="212"/>
-      <c r="B105" s="213"/>
+      <c r="A105" s="211"/>
+      <c r="B105" s="212"/>
       <c r="C105" s="19" t="s">
         <v>168</v>
       </c>
@@ -7195,8 +7210,8 @@
       </c>
     </row>
     <row r="106" spans="1:16">
-      <c r="A106" s="212"/>
-      <c r="B106" s="213"/>
+      <c r="A106" s="211"/>
+      <c r="B106" s="212"/>
       <c r="C106" s="144" t="s">
         <v>169</v>
       </c>
@@ -7241,10 +7256,10 @@
       </c>
     </row>
     <row r="107" spans="1:16">
-      <c r="A107" s="211" t="s">
+      <c r="A107" s="209" t="s">
         <v>174</v>
       </c>
-      <c r="B107" s="214" t="s">
+      <c r="B107" s="213" t="s">
         <v>173</v>
       </c>
       <c r="C107" s="115" t="s">
@@ -7291,8 +7306,8 @@
       </c>
     </row>
     <row r="108" spans="1:16">
-      <c r="A108" s="211"/>
-      <c r="B108" s="214"/>
+      <c r="A108" s="209"/>
+      <c r="B108" s="213"/>
       <c r="C108" s="149" t="s">
         <v>167</v>
       </c>
@@ -7337,8 +7352,8 @@
       </c>
     </row>
     <row r="109" spans="1:16">
-      <c r="A109" s="211"/>
-      <c r="B109" s="214"/>
+      <c r="A109" s="209"/>
+      <c r="B109" s="213"/>
       <c r="C109" s="149" t="s">
         <v>168</v>
       </c>
@@ -7383,8 +7398,8 @@
       </c>
     </row>
     <row r="110" spans="1:16">
-      <c r="A110" s="211"/>
-      <c r="B110" s="214"/>
+      <c r="A110" s="209"/>
+      <c r="B110" s="213"/>
       <c r="C110" s="150" t="s">
         <v>169</v>
       </c>
@@ -7449,10 +7464,10 @@
       <c r="P111" s="155"/>
     </row>
     <row r="112" spans="1:16">
-      <c r="A112" s="215" t="s">
+      <c r="A112" s="200" t="s">
         <v>8</v>
       </c>
-      <c r="B112" s="216" t="s">
+      <c r="B112" s="201" t="s">
         <v>173</v>
       </c>
       <c r="C112" s="19" t="s">
@@ -7499,8 +7514,8 @@
       </c>
     </row>
     <row r="113" spans="1:16">
-      <c r="A113" s="215"/>
-      <c r="B113" s="216"/>
+      <c r="A113" s="200"/>
+      <c r="B113" s="201"/>
       <c r="C113" s="19" t="s">
         <v>167</v>
       </c>
@@ -7545,8 +7560,8 @@
       </c>
     </row>
     <row r="114" spans="1:16">
-      <c r="A114" s="215"/>
-      <c r="B114" s="216"/>
+      <c r="A114" s="200"/>
+      <c r="B114" s="201"/>
       <c r="C114" s="19" t="s">
         <v>168</v>
       </c>
@@ -7591,8 +7606,8 @@
       </c>
     </row>
     <row r="115" spans="1:16">
-      <c r="A115" s="215"/>
-      <c r="B115" s="216"/>
+      <c r="A115" s="200"/>
+      <c r="B115" s="201"/>
       <c r="C115" s="19" t="s">
         <v>169</v>
       </c>
@@ -7637,10 +7652,10 @@
       </c>
     </row>
     <row r="116" spans="1:16">
-      <c r="A116" s="215" t="s">
+      <c r="A116" s="200" t="s">
         <v>9</v>
       </c>
-      <c r="B116" s="216" t="s">
+      <c r="B116" s="201" t="s">
         <v>173</v>
       </c>
       <c r="C116" s="157" t="s">
@@ -7687,8 +7702,8 @@
       </c>
     </row>
     <row r="117" spans="1:16">
-      <c r="A117" s="215"/>
-      <c r="B117" s="216"/>
+      <c r="A117" s="200"/>
+      <c r="B117" s="201"/>
       <c r="C117" s="19" t="s">
         <v>167</v>
       </c>
@@ -7733,8 +7748,8 @@
       </c>
     </row>
     <row r="118" spans="1:16">
-      <c r="A118" s="215"/>
-      <c r="B118" s="216"/>
+      <c r="A118" s="200"/>
+      <c r="B118" s="201"/>
       <c r="C118" s="19" t="s">
         <v>168</v>
       </c>
@@ -7779,8 +7794,8 @@
       </c>
     </row>
     <row r="119" spans="1:16">
-      <c r="A119" s="215"/>
-      <c r="B119" s="216"/>
+      <c r="A119" s="200"/>
+      <c r="B119" s="201"/>
       <c r="C119" s="19" t="s">
         <v>169</v>
       </c>
@@ -7825,10 +7840,10 @@
       </c>
     </row>
     <row r="120" spans="1:16">
-      <c r="A120" s="215" t="s">
+      <c r="A120" s="200" t="s">
         <v>10</v>
       </c>
-      <c r="B120" s="216" t="s">
+      <c r="B120" s="201" t="s">
         <v>173</v>
       </c>
       <c r="C120" s="19" t="s">
@@ -7875,8 +7890,8 @@
       </c>
     </row>
     <row r="121" spans="1:16">
-      <c r="A121" s="215"/>
-      <c r="B121" s="216"/>
+      <c r="A121" s="200"/>
+      <c r="B121" s="201"/>
       <c r="C121" s="19" t="s">
         <v>167</v>
       </c>
@@ -7921,8 +7936,8 @@
       </c>
     </row>
     <row r="122" spans="1:16">
-      <c r="A122" s="215"/>
-      <c r="B122" s="216"/>
+      <c r="A122" s="200"/>
+      <c r="B122" s="201"/>
       <c r="C122" s="19" t="s">
         <v>168</v>
       </c>
@@ -7967,8 +7982,8 @@
       </c>
     </row>
     <row r="123" spans="1:16">
-      <c r="A123" s="215"/>
-      <c r="B123" s="216"/>
+      <c r="A123" s="200"/>
+      <c r="B123" s="201"/>
       <c r="C123" s="19" t="s">
         <v>169</v>
       </c>
@@ -8013,10 +8028,10 @@
       </c>
     </row>
     <row r="124" spans="1:16">
-      <c r="A124" s="215" t="s">
+      <c r="A124" s="200" t="s">
         <v>11</v>
       </c>
-      <c r="B124" s="216" t="s">
+      <c r="B124" s="201" t="s">
         <v>173</v>
       </c>
       <c r="C124" s="19" t="s">
@@ -8063,8 +8078,8 @@
       </c>
     </row>
     <row r="125" spans="1:16">
-      <c r="A125" s="215"/>
-      <c r="B125" s="216"/>
+      <c r="A125" s="200"/>
+      <c r="B125" s="201"/>
       <c r="C125" s="19" t="s">
         <v>167</v>
       </c>
@@ -8109,8 +8124,8 @@
       </c>
     </row>
     <row r="126" spans="1:16">
-      <c r="A126" s="215"/>
-      <c r="B126" s="216"/>
+      <c r="A126" s="200"/>
+      <c r="B126" s="201"/>
       <c r="C126" s="19" t="s">
         <v>168</v>
       </c>
@@ -8155,8 +8170,8 @@
       </c>
     </row>
     <row r="127" spans="1:16">
-      <c r="A127" s="215"/>
-      <c r="B127" s="216"/>
+      <c r="A127" s="200"/>
+      <c r="B127" s="201"/>
       <c r="C127" s="19" t="s">
         <v>169</v>
       </c>
@@ -8201,10 +8216,10 @@
       </c>
     </row>
     <row r="128" spans="1:16">
-      <c r="A128" s="215" t="s">
+      <c r="A128" s="200" t="s">
         <v>12</v>
       </c>
-      <c r="B128" s="216" t="s">
+      <c r="B128" s="201" t="s">
         <v>173</v>
       </c>
       <c r="C128" s="19" t="s">
@@ -8251,8 +8266,8 @@
       </c>
     </row>
     <row r="129" spans="1:16">
-      <c r="A129" s="215"/>
-      <c r="B129" s="216"/>
+      <c r="A129" s="200"/>
+      <c r="B129" s="201"/>
       <c r="C129" s="19" t="s">
         <v>167</v>
       </c>
@@ -8297,8 +8312,8 @@
       </c>
     </row>
     <row r="130" spans="1:16">
-      <c r="A130" s="215"/>
-      <c r="B130" s="216"/>
+      <c r="A130" s="200"/>
+      <c r="B130" s="201"/>
       <c r="C130" s="19" t="s">
         <v>168</v>
       </c>
@@ -8343,8 +8358,8 @@
       </c>
     </row>
     <row r="131" spans="1:16">
-      <c r="A131" s="215"/>
-      <c r="B131" s="216"/>
+      <c r="A131" s="200"/>
+      <c r="B131" s="201"/>
       <c r="C131" s="19" t="s">
         <v>169</v>
       </c>
@@ -8389,10 +8404,10 @@
       </c>
     </row>
     <row r="132" spans="1:16">
-      <c r="A132" s="215" t="s">
+      <c r="A132" s="200" t="s">
         <v>13</v>
       </c>
-      <c r="B132" s="216" t="s">
+      <c r="B132" s="201" t="s">
         <v>173</v>
       </c>
       <c r="C132" s="19" t="s">
@@ -8439,8 +8454,8 @@
       </c>
     </row>
     <row r="133" spans="1:16">
-      <c r="A133" s="215"/>
-      <c r="B133" s="216"/>
+      <c r="A133" s="200"/>
+      <c r="B133" s="201"/>
       <c r="C133" s="19" t="s">
         <v>167</v>
       </c>
@@ -8485,8 +8500,8 @@
       </c>
     </row>
     <row r="134" spans="1:16">
-      <c r="A134" s="215"/>
-      <c r="B134" s="216"/>
+      <c r="A134" s="200"/>
+      <c r="B134" s="201"/>
       <c r="C134" s="19" t="s">
         <v>168</v>
       </c>
@@ -8531,8 +8546,8 @@
       </c>
     </row>
     <row r="135" spans="1:16">
-      <c r="A135" s="215"/>
-      <c r="B135" s="216"/>
+      <c r="A135" s="200"/>
+      <c r="B135" s="201"/>
       <c r="C135" s="19" t="s">
         <v>169</v>
       </c>
@@ -8577,10 +8592,10 @@
       </c>
     </row>
     <row r="136" spans="1:16">
-      <c r="A136" s="215" t="s">
+      <c r="A136" s="200" t="s">
         <v>14</v>
       </c>
-      <c r="B136" s="216" t="s">
+      <c r="B136" s="201" t="s">
         <v>173</v>
       </c>
       <c r="C136" s="19" t="s">
@@ -8627,8 +8642,8 @@
       </c>
     </row>
     <row r="137" spans="1:16">
-      <c r="A137" s="215"/>
-      <c r="B137" s="216"/>
+      <c r="A137" s="200"/>
+      <c r="B137" s="201"/>
       <c r="C137" s="19" t="s">
         <v>167</v>
       </c>
@@ -8673,8 +8688,8 @@
       </c>
     </row>
     <row r="138" spans="1:16">
-      <c r="A138" s="215"/>
-      <c r="B138" s="216"/>
+      <c r="A138" s="200"/>
+      <c r="B138" s="201"/>
       <c r="C138" s="19" t="s">
         <v>168</v>
       </c>
@@ -8719,8 +8734,8 @@
       </c>
     </row>
     <row r="139" spans="1:16">
-      <c r="A139" s="215"/>
-      <c r="B139" s="216"/>
+      <c r="A139" s="200"/>
+      <c r="B139" s="201"/>
       <c r="C139" s="19" t="s">
         <v>169</v>
       </c>
@@ -8765,10 +8780,10 @@
       </c>
     </row>
     <row r="140" spans="1:16">
-      <c r="A140" s="219" t="s">
+      <c r="A140" s="202" t="s">
         <v>15</v>
       </c>
-      <c r="B140" s="216" t="s">
+      <c r="B140" s="201" t="s">
         <v>173</v>
       </c>
       <c r="C140" s="19" t="s">
@@ -8815,8 +8830,8 @@
       </c>
     </row>
     <row r="141" spans="1:16">
-      <c r="A141" s="219"/>
-      <c r="B141" s="216"/>
+      <c r="A141" s="202"/>
+      <c r="B141" s="201"/>
       <c r="C141" s="19" t="s">
         <v>167</v>
       </c>
@@ -8861,8 +8876,8 @@
       </c>
     </row>
     <row r="142" spans="1:16">
-      <c r="A142" s="219"/>
-      <c r="B142" s="216"/>
+      <c r="A142" s="202"/>
+      <c r="B142" s="201"/>
       <c r="C142" s="19" t="s">
         <v>168</v>
       </c>
@@ -8907,8 +8922,8 @@
       </c>
     </row>
     <row r="143" spans="1:16">
-      <c r="A143" s="219"/>
-      <c r="B143" s="216"/>
+      <c r="A143" s="202"/>
+      <c r="B143" s="201"/>
       <c r="C143" s="19" t="s">
         <v>169</v>
       </c>
@@ -8953,10 +8968,10 @@
       </c>
     </row>
     <row r="144" spans="1:16">
-      <c r="A144" s="220" t="s">
+      <c r="A144" s="203" t="s">
         <v>16</v>
       </c>
-      <c r="B144" s="221" t="s">
+      <c r="B144" s="204" t="s">
         <v>173</v>
       </c>
       <c r="C144" s="19" t="s">
@@ -9003,8 +9018,8 @@
       </c>
     </row>
     <row r="145" spans="1:16">
-      <c r="A145" s="220"/>
-      <c r="B145" s="221"/>
+      <c r="A145" s="203"/>
+      <c r="B145" s="204"/>
       <c r="C145" s="19" t="s">
         <v>167</v>
       </c>
@@ -9049,8 +9064,8 @@
       </c>
     </row>
     <row r="146" spans="1:16">
-      <c r="A146" s="220"/>
-      <c r="B146" s="221"/>
+      <c r="A146" s="203"/>
+      <c r="B146" s="204"/>
       <c r="C146" s="19" t="s">
         <v>168</v>
       </c>
@@ -9095,8 +9110,8 @@
       </c>
     </row>
     <row r="147" spans="1:16">
-      <c r="A147" s="220"/>
-      <c r="B147" s="221"/>
+      <c r="A147" s="203"/>
+      <c r="B147" s="204"/>
       <c r="C147" s="123" t="s">
         <v>169</v>
       </c>
@@ -9141,7 +9156,7 @@
       </c>
     </row>
     <row r="149" spans="1:16">
-      <c r="C149" s="224"/>
+      <c r="C149" s="192"/>
     </row>
     <row r="151" spans="1:16">
       <c r="A151" s="188" t="s">
@@ -9188,7 +9203,7 @@
       </c>
     </row>
     <row r="152" spans="1:16">
-      <c r="A152" s="217" t="s">
+      <c r="A152" s="198" t="s">
         <v>196</v>
       </c>
       <c r="B152" s="17" t="s">
@@ -9232,7 +9247,7 @@
       </c>
     </row>
     <row r="153" spans="1:16">
-      <c r="A153" s="218"/>
+      <c r="A153" s="199"/>
       <c r="B153" s="17" t="s">
         <v>194</v>
       </c>
@@ -9274,7 +9289,7 @@
       </c>
     </row>
     <row r="154" spans="1:16">
-      <c r="A154" s="222"/>
+      <c r="A154" s="205"/>
       <c r="B154" s="17" t="s">
         <v>195</v>
       </c>
@@ -9316,7 +9331,7 @@
       </c>
     </row>
     <row r="155" spans="1:16">
-      <c r="A155" s="195" t="s">
+      <c r="A155" s="206" t="s">
         <v>197</v>
       </c>
       <c r="B155" s="17" t="s">
@@ -9360,7 +9375,7 @@
       </c>
     </row>
     <row r="156" spans="1:16">
-      <c r="A156" s="196"/>
+      <c r="A156" s="207"/>
       <c r="B156" s="17" t="s">
         <v>194</v>
       </c>
@@ -9402,7 +9417,7 @@
       </c>
     </row>
     <row r="157" spans="1:16">
-      <c r="A157" s="197"/>
+      <c r="A157" s="208"/>
       <c r="B157" s="17" t="s">
         <v>195</v>
       </c>
@@ -9444,7 +9459,7 @@
       </c>
     </row>
     <row r="158" spans="1:16">
-      <c r="A158" s="195" t="s">
+      <c r="A158" s="206" t="s">
         <v>186</v>
       </c>
       <c r="B158" s="17" t="s">
@@ -9500,7 +9515,7 @@
       </c>
     </row>
     <row r="159" spans="1:16">
-      <c r="A159" s="196"/>
+      <c r="A159" s="207"/>
       <c r="B159" s="17" t="s">
         <v>194</v>
       </c>
@@ -9542,7 +9557,7 @@
       </c>
     </row>
     <row r="160" spans="1:16">
-      <c r="A160" s="197"/>
+      <c r="A160" s="208"/>
       <c r="B160" s="17" t="s">
         <v>195</v>
       </c>
@@ -9584,7 +9599,7 @@
       </c>
     </row>
     <row r="161" spans="1:14">
-      <c r="A161" s="195" t="s">
+      <c r="A161" s="206" t="s">
         <v>187</v>
       </c>
       <c r="B161" s="17" t="s">
@@ -9628,7 +9643,7 @@
       </c>
     </row>
     <row r="162" spans="1:14">
-      <c r="A162" s="196"/>
+      <c r="A162" s="207"/>
       <c r="B162" s="17" t="s">
         <v>194</v>
       </c>
@@ -9670,7 +9685,7 @@
       </c>
     </row>
     <row r="163" spans="1:14">
-      <c r="A163" s="197"/>
+      <c r="A163" s="208"/>
       <c r="B163" s="17" t="s">
         <v>195</v>
       </c>
@@ -9712,7 +9727,7 @@
       </c>
     </row>
     <row r="164" spans="1:14">
-      <c r="A164" s="195" t="s">
+      <c r="A164" s="206" t="s">
         <v>188</v>
       </c>
       <c r="B164" s="17" t="s">
@@ -9756,7 +9771,7 @@
       </c>
     </row>
     <row r="165" spans="1:14">
-      <c r="A165" s="196"/>
+      <c r="A165" s="207"/>
       <c r="B165" s="17" t="s">
         <v>194</v>
       </c>
@@ -9798,7 +9813,7 @@
       </c>
     </row>
     <row r="166" spans="1:14">
-      <c r="A166" s="197"/>
+      <c r="A166" s="208"/>
       <c r="B166" s="17" t="s">
         <v>195</v>
       </c>
@@ -9840,7 +9855,7 @@
       </c>
     </row>
     <row r="167" spans="1:14">
-      <c r="A167" s="195" t="s">
+      <c r="A167" s="206" t="s">
         <v>189</v>
       </c>
       <c r="B167" s="17" t="s">
@@ -9884,7 +9899,7 @@
       </c>
     </row>
     <row r="168" spans="1:14">
-      <c r="A168" s="196"/>
+      <c r="A168" s="207"/>
       <c r="B168" s="17" t="s">
         <v>194</v>
       </c>
@@ -9926,7 +9941,7 @@
       </c>
     </row>
     <row r="169" spans="1:14">
-      <c r="A169" s="197"/>
+      <c r="A169" s="208"/>
       <c r="B169" s="17" t="s">
         <v>195</v>
       </c>
@@ -9968,7 +9983,7 @@
       </c>
     </row>
     <row r="170" spans="1:14">
-      <c r="A170" s="195" t="s">
+      <c r="A170" s="206" t="s">
         <v>190</v>
       </c>
       <c r="B170" s="17" t="s">
@@ -10012,7 +10027,7 @@
       </c>
     </row>
     <row r="171" spans="1:14">
-      <c r="A171" s="196"/>
+      <c r="A171" s="207"/>
       <c r="B171" s="17" t="s">
         <v>194</v>
       </c>
@@ -10054,7 +10069,7 @@
       </c>
     </row>
     <row r="172" spans="1:14">
-      <c r="A172" s="197"/>
+      <c r="A172" s="208"/>
       <c r="B172" s="17" t="s">
         <v>195</v>
       </c>
@@ -10096,7 +10111,7 @@
       </c>
     </row>
     <row r="173" spans="1:14">
-      <c r="A173" s="195" t="s">
+      <c r="A173" s="206" t="s">
         <v>191</v>
       </c>
       <c r="B173" s="17" t="s">
@@ -10140,7 +10155,7 @@
       </c>
     </row>
     <row r="174" spans="1:14">
-      <c r="A174" s="196"/>
+      <c r="A174" s="207"/>
       <c r="B174" s="17" t="s">
         <v>194</v>
       </c>
@@ -10182,7 +10197,7 @@
       </c>
     </row>
     <row r="175" spans="1:14">
-      <c r="A175" s="197"/>
+      <c r="A175" s="208"/>
       <c r="B175" s="17" t="s">
         <v>195</v>
       </c>
@@ -10224,7 +10239,7 @@
       </c>
     </row>
     <row r="176" spans="1:14">
-      <c r="A176" s="195" t="s">
+      <c r="A176" s="206" t="s">
         <v>198</v>
       </c>
       <c r="B176" s="17" t="s">
@@ -10268,7 +10283,7 @@
       </c>
     </row>
     <row r="177" spans="1:14">
-      <c r="A177" s="196"/>
+      <c r="A177" s="207"/>
       <c r="B177" s="17" t="s">
         <v>194</v>
       </c>
@@ -10310,7 +10325,7 @@
       </c>
     </row>
     <row r="178" spans="1:14">
-      <c r="A178" s="197"/>
+      <c r="A178" s="208"/>
       <c r="B178" s="17" t="s">
         <v>195</v>
       </c>
@@ -10352,7 +10367,7 @@
       </c>
     </row>
     <row r="179" spans="1:14">
-      <c r="A179" s="195" t="s">
+      <c r="A179" s="206" t="s">
         <v>199</v>
       </c>
       <c r="B179" s="17" t="s">
@@ -10396,7 +10411,7 @@
       </c>
     </row>
     <row r="180" spans="1:14">
-      <c r="A180" s="196"/>
+      <c r="A180" s="207"/>
       <c r="B180" s="17" t="s">
         <v>194</v>
       </c>
@@ -10438,7 +10453,7 @@
       </c>
     </row>
     <row r="181" spans="1:14">
-      <c r="A181" s="197"/>
+      <c r="A181" s="208"/>
       <c r="B181" s="17" t="s">
         <v>195</v>
       </c>
@@ -10480,7 +10495,7 @@
       </c>
     </row>
     <row r="182" spans="1:14">
-      <c r="A182" s="195" t="s">
+      <c r="A182" s="206" t="s">
         <v>200</v>
       </c>
       <c r="B182" s="17" t="s">
@@ -10524,7 +10539,7 @@
       </c>
     </row>
     <row r="183" spans="1:14">
-      <c r="A183" s="196"/>
+      <c r="A183" s="207"/>
       <c r="B183" s="17" t="s">
         <v>194</v>
       </c>
@@ -10566,7 +10581,7 @@
       </c>
     </row>
     <row r="184" spans="1:14">
-      <c r="A184" s="197"/>
+      <c r="A184" s="208"/>
       <c r="B184" s="17" t="s">
         <v>195</v>
       </c>
@@ -10608,7 +10623,7 @@
       </c>
     </row>
     <row r="185" spans="1:14">
-      <c r="A185" s="195" t="s">
+      <c r="A185" s="206" t="s">
         <v>201</v>
       </c>
       <c r="B185" s="17" t="s">
@@ -10652,7 +10667,7 @@
       </c>
     </row>
     <row r="186" spans="1:14">
-      <c r="A186" s="196"/>
+      <c r="A186" s="207"/>
       <c r="B186" s="17" t="s">
         <v>194</v>
       </c>
@@ -10694,7 +10709,7 @@
       </c>
     </row>
     <row r="187" spans="1:14">
-      <c r="A187" s="197"/>
+      <c r="A187" s="208"/>
       <c r="B187" s="17" t="s">
         <v>195</v>
       </c>
@@ -10736,7 +10751,7 @@
       </c>
     </row>
     <row r="188" spans="1:14">
-      <c r="A188" s="195" t="s">
+      <c r="A188" s="206" t="s">
         <v>202</v>
       </c>
       <c r="B188" s="17" t="s">
@@ -10780,7 +10795,7 @@
       </c>
     </row>
     <row r="189" spans="1:14">
-      <c r="A189" s="196"/>
+      <c r="A189" s="207"/>
       <c r="B189" s="17" t="s">
         <v>194</v>
       </c>
@@ -10822,7 +10837,7 @@
       </c>
     </row>
     <row r="190" spans="1:14">
-      <c r="A190" s="197"/>
+      <c r="A190" s="208"/>
       <c r="B190" s="17" t="s">
         <v>195</v>
       </c>
@@ -10864,7 +10879,7 @@
       </c>
     </row>
     <row r="191" spans="1:14">
-      <c r="A191" s="195" t="s">
+      <c r="A191" s="206" t="s">
         <v>203</v>
       </c>
       <c r="B191" s="17" t="s">
@@ -10908,7 +10923,7 @@
       </c>
     </row>
     <row r="192" spans="1:14">
-      <c r="A192" s="196"/>
+      <c r="A192" s="207"/>
       <c r="B192" s="17" t="s">
         <v>194</v>
       </c>
@@ -10949,8 +10964,8 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="193" spans="1:14">
-      <c r="A193" s="197"/>
+    <row r="193" spans="1:30">
+      <c r="A193" s="208"/>
       <c r="B193" s="17" t="s">
         <v>195</v>
       </c>
@@ -10991,8 +11006,8 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="194" spans="1:14">
-      <c r="A194" s="195" t="s">
+    <row r="194" spans="1:30">
+      <c r="A194" s="206" t="s">
         <v>204</v>
       </c>
       <c r="B194" s="17" t="s">
@@ -11035,8 +11050,8 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="195" spans="1:14">
-      <c r="A195" s="196"/>
+    <row r="195" spans="1:30">
+      <c r="A195" s="207"/>
       <c r="B195" s="17" t="s">
         <v>194</v>
       </c>
@@ -11077,8 +11092,8 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="196" spans="1:14">
-      <c r="A196" s="197"/>
+    <row r="196" spans="1:30">
+      <c r="A196" s="208"/>
       <c r="B196" s="17" t="s">
         <v>195</v>
       </c>
@@ -11119,7 +11134,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="197" spans="1:14">
+    <row r="197" spans="1:30">
       <c r="A197" s="188" t="s">
         <v>211</v>
       </c>
@@ -11163,8 +11178,8 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="198" spans="1:14">
-      <c r="A198" s="217" t="s">
+    <row r="198" spans="1:30">
+      <c r="A198" s="198" t="s">
         <v>212</v>
       </c>
       <c r="B198" s="17" t="s">
@@ -11207,8 +11222,8 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="199" spans="1:14">
-      <c r="A199" s="218"/>
+    <row r="199" spans="1:30">
+      <c r="A199" s="199"/>
       <c r="B199" s="17" t="s">
         <v>214</v>
       </c>
@@ -11249,8 +11264,266 @@
         <v>0.5</v>
       </c>
     </row>
+    <row r="201" spans="1:30">
+      <c r="A201" s="197" t="s">
+        <v>215</v>
+      </c>
+      <c r="B201" s="197"/>
+      <c r="C201" s="197"/>
+      <c r="D201" s="197"/>
+      <c r="E201" s="197"/>
+      <c r="F201" s="197"/>
+      <c r="G201" s="197"/>
+      <c r="H201" s="197"/>
+      <c r="I201" s="197"/>
+      <c r="J201" s="197"/>
+      <c r="K201" s="197"/>
+      <c r="L201" s="197"/>
+      <c r="M201" s="197"/>
+      <c r="N201" s="197"/>
+      <c r="O201" s="197"/>
+      <c r="P201" s="197"/>
+      <c r="Q201" s="197"/>
+      <c r="R201" s="197"/>
+      <c r="S201" s="197"/>
+      <c r="T201" s="197"/>
+      <c r="U201" s="197"/>
+      <c r="V201" s="197"/>
+      <c r="W201" s="197"/>
+      <c r="X201" s="197"/>
+      <c r="Y201" s="197"/>
+      <c r="Z201" s="197"/>
+      <c r="AA201" s="197"/>
+      <c r="AB201" s="197"/>
+      <c r="AC201" s="197"/>
+      <c r="AD201" s="197"/>
+    </row>
+    <row r="202" spans="1:30">
+      <c r="A202" s="17" t="s">
+        <v>216</v>
+      </c>
+      <c r="B202" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C202" s="19">
+        <v>1995</v>
+      </c>
+      <c r="D202" s="19">
+        <v>1996</v>
+      </c>
+      <c r="E202" s="19">
+        <v>1997</v>
+      </c>
+      <c r="F202" s="19">
+        <v>1998</v>
+      </c>
+      <c r="G202" s="19">
+        <v>1999</v>
+      </c>
+      <c r="H202" s="19">
+        <v>2000</v>
+      </c>
+      <c r="I202" s="19">
+        <v>2001</v>
+      </c>
+      <c r="J202" s="19">
+        <v>2002</v>
+      </c>
+      <c r="K202" s="19">
+        <v>2003</v>
+      </c>
+      <c r="L202" s="19">
+        <v>2004</v>
+      </c>
+      <c r="M202" s="19">
+        <v>2005</v>
+      </c>
+      <c r="N202" s="19">
+        <v>2006</v>
+      </c>
+      <c r="O202" s="19">
+        <v>2007</v>
+      </c>
+      <c r="P202" s="19">
+        <v>2008</v>
+      </c>
+      <c r="Q202" s="19">
+        <v>2009</v>
+      </c>
+      <c r="R202" s="19">
+        <v>2010</v>
+      </c>
+      <c r="S202" s="19">
+        <v>2011</v>
+      </c>
+      <c r="T202" s="19">
+        <v>2012</v>
+      </c>
+      <c r="U202" s="19">
+        <v>2013</v>
+      </c>
+      <c r="V202" s="19">
+        <v>2014</v>
+      </c>
+      <c r="W202" s="19">
+        <v>2015</v>
+      </c>
+      <c r="X202" s="19">
+        <v>2016</v>
+      </c>
+      <c r="Y202" s="19">
+        <v>2017</v>
+      </c>
+      <c r="Z202" s="19">
+        <v>2018</v>
+      </c>
+      <c r="AA202" s="19">
+        <v>2019</v>
+      </c>
+      <c r="AB202" s="19">
+        <v>2020</v>
+      </c>
+      <c r="AC202" s="19">
+        <v>2021</v>
+      </c>
+      <c r="AD202" s="19">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="203" spans="1:30">
+      <c r="A203" s="17" t="s">
+        <v>217</v>
+      </c>
+      <c r="B203" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="C203" s="19">
+        <v>0.197862902023071</v>
+      </c>
+      <c r="D203" s="19">
+        <v>0.19705245774944699</v>
+      </c>
+      <c r="E203" s="19">
+        <v>0.195862164585204</v>
+      </c>
+      <c r="F203" s="19">
+        <v>0.201506494990219</v>
+      </c>
+      <c r="G203" s="19">
+        <v>0.20239331346144401</v>
+      </c>
+      <c r="H203" s="19">
+        <v>0.19184050965229399</v>
+      </c>
+      <c r="I203" s="19">
+        <v>0.19816391062786801</v>
+      </c>
+      <c r="J203" s="19">
+        <v>0.20784587230133</v>
+      </c>
+      <c r="K203" s="19">
+        <v>0.20742275052980599</v>
+      </c>
+      <c r="L203" s="19">
+        <v>0.199178611956073</v>
+      </c>
+      <c r="M203" s="19">
+        <v>0.191773175691209</v>
+      </c>
+      <c r="N203" s="19">
+        <v>0.18843581838972301</v>
+      </c>
+      <c r="O203" s="19">
+        <v>0.18492183987135299</v>
+      </c>
+      <c r="P203" s="19">
+        <v>0.17476484558917099</v>
+      </c>
+      <c r="Q203" s="19">
+        <v>0.18473705831690901</v>
+      </c>
+      <c r="R203" s="19">
+        <v>0.18654754004049501</v>
+      </c>
+      <c r="S203" s="19">
+        <v>0.189454834248799</v>
+      </c>
+      <c r="T203" s="19">
+        <v>0.18970988362343699</v>
+      </c>
+      <c r="U203" s="19">
+        <v>0.191084988644315</v>
+      </c>
+      <c r="V203" s="19">
+        <v>0.195502781940076</v>
+      </c>
+      <c r="W203" s="19">
+        <v>0.18767352366145501</v>
+      </c>
+      <c r="X203" s="19">
+        <v>0.18955666805548799</v>
+      </c>
+      <c r="Y203" s="19">
+        <v>0.18919126608338799</v>
+      </c>
+      <c r="Z203" s="19">
+        <v>0.19123080280548899</v>
+      </c>
+      <c r="AA203" s="19">
+        <v>0.20390796789551899</v>
+      </c>
+      <c r="AB203" s="19">
+        <v>0.192958485556329</v>
+      </c>
+      <c r="AC203" s="19">
+        <v>0.195589643486903</v>
+      </c>
+      <c r="AD203" s="19">
+        <v>0.185678435467685</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="55">
+  <mergeCells count="56">
+    <mergeCell ref="A201:AD201"/>
+    <mergeCell ref="A194:A196"/>
+    <mergeCell ref="A179:A181"/>
+    <mergeCell ref="A182:A184"/>
+    <mergeCell ref="A185:A187"/>
+    <mergeCell ref="A188:A190"/>
+    <mergeCell ref="A191:A193"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="A29:D29"/>
+    <mergeCell ref="D30:D38"/>
+    <mergeCell ref="D39:D41"/>
+    <mergeCell ref="D42:D45"/>
+    <mergeCell ref="D46:D49"/>
+    <mergeCell ref="A64:C64"/>
+    <mergeCell ref="B85:B88"/>
+    <mergeCell ref="A95:A98"/>
+    <mergeCell ref="B95:B98"/>
+    <mergeCell ref="A99:A102"/>
+    <mergeCell ref="B99:B102"/>
+    <mergeCell ref="A103:A106"/>
+    <mergeCell ref="B103:B106"/>
+    <mergeCell ref="A107:A110"/>
+    <mergeCell ref="B107:B110"/>
+    <mergeCell ref="A112:A115"/>
+    <mergeCell ref="B112:B115"/>
+    <mergeCell ref="A116:A119"/>
+    <mergeCell ref="B116:B119"/>
+    <mergeCell ref="A120:A123"/>
+    <mergeCell ref="B120:B123"/>
+    <mergeCell ref="A124:A127"/>
+    <mergeCell ref="B124:B127"/>
+    <mergeCell ref="A128:A131"/>
+    <mergeCell ref="B128:B131"/>
+    <mergeCell ref="A132:A135"/>
+    <mergeCell ref="B132:B135"/>
     <mergeCell ref="A198:A199"/>
     <mergeCell ref="A136:A139"/>
     <mergeCell ref="B136:B139"/>
@@ -11267,45 +11540,6 @@
     <mergeCell ref="A170:A172"/>
     <mergeCell ref="A173:A175"/>
     <mergeCell ref="A176:A178"/>
-    <mergeCell ref="A124:A127"/>
-    <mergeCell ref="B124:B127"/>
-    <mergeCell ref="A128:A131"/>
-    <mergeCell ref="B128:B131"/>
-    <mergeCell ref="A132:A135"/>
-    <mergeCell ref="B132:B135"/>
-    <mergeCell ref="A112:A115"/>
-    <mergeCell ref="B112:B115"/>
-    <mergeCell ref="A116:A119"/>
-    <mergeCell ref="B116:B119"/>
-    <mergeCell ref="A120:A123"/>
-    <mergeCell ref="B120:B123"/>
-    <mergeCell ref="A99:A102"/>
-    <mergeCell ref="B99:B102"/>
-    <mergeCell ref="A103:A106"/>
-    <mergeCell ref="B103:B106"/>
-    <mergeCell ref="A107:A110"/>
-    <mergeCell ref="B107:B110"/>
-    <mergeCell ref="D46:D49"/>
-    <mergeCell ref="A64:C64"/>
-    <mergeCell ref="B85:B88"/>
-    <mergeCell ref="A95:A98"/>
-    <mergeCell ref="B95:B98"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="A29:D29"/>
-    <mergeCell ref="D30:D38"/>
-    <mergeCell ref="D39:D41"/>
-    <mergeCell ref="D42:D45"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A194:A196"/>
-    <mergeCell ref="A179:A181"/>
-    <mergeCell ref="A182:A184"/>
-    <mergeCell ref="A185:A187"/>
-    <mergeCell ref="A188:A190"/>
-    <mergeCell ref="A191:A193"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -11382,7 +11616,7 @@
       </c>
     </row>
     <row r="2" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A2" s="209" t="s">
+      <c r="A2" s="217" t="s">
         <v>165</v>
       </c>
       <c r="B2" s="210" t="s">
@@ -11432,7 +11666,7 @@
       </c>
     </row>
     <row r="3" spans="1:16">
-      <c r="A3" s="209"/>
+      <c r="A3" s="217"/>
       <c r="B3" s="210"/>
       <c r="C3" s="19" t="s">
         <v>167</v>
@@ -11478,7 +11712,7 @@
       </c>
     </row>
     <row r="4" spans="1:16">
-      <c r="A4" s="209"/>
+      <c r="A4" s="217"/>
       <c r="B4" s="210"/>
       <c r="C4" s="19" t="s">
         <v>168</v>
@@ -11524,7 +11758,7 @@
       </c>
     </row>
     <row r="5" spans="1:16">
-      <c r="A5" s="209"/>
+      <c r="A5" s="217"/>
       <c r="B5" s="210"/>
       <c r="C5" s="123" t="s">
         <v>169</v>
@@ -11570,7 +11804,7 @@
       </c>
     </row>
     <row r="6" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A6" s="211" t="s">
+      <c r="A6" s="209" t="s">
         <v>170</v>
       </c>
       <c r="B6" s="210" t="s">
@@ -11620,7 +11854,7 @@
       </c>
     </row>
     <row r="7" spans="1:16">
-      <c r="A7" s="211"/>
+      <c r="A7" s="209"/>
       <c r="B7" s="210"/>
       <c r="C7" s="19" t="s">
         <v>167</v>
@@ -11666,7 +11900,7 @@
       </c>
     </row>
     <row r="8" spans="1:16">
-      <c r="A8" s="211"/>
+      <c r="A8" s="209"/>
       <c r="B8" s="210"/>
       <c r="C8" s="19" t="s">
         <v>168</v>
@@ -11712,7 +11946,7 @@
       </c>
     </row>
     <row r="9" spans="1:16">
-      <c r="A9" s="211"/>
+      <c r="A9" s="209"/>
       <c r="B9" s="210"/>
       <c r="C9" s="123" t="s">
         <v>169</v>
@@ -11758,10 +11992,10 @@
       </c>
     </row>
     <row r="10" spans="1:16">
-      <c r="A10" s="212" t="s">
+      <c r="A10" s="211" t="s">
         <v>172</v>
       </c>
-      <c r="B10" s="213" t="s">
+      <c r="B10" s="212" t="s">
         <v>173</v>
       </c>
       <c r="C10" s="115" t="s">
@@ -11808,8 +12042,8 @@
       </c>
     </row>
     <row r="11" spans="1:16">
-      <c r="A11" s="212"/>
-      <c r="B11" s="213"/>
+      <c r="A11" s="211"/>
+      <c r="B11" s="212"/>
       <c r="C11" s="19" t="s">
         <v>167</v>
       </c>
@@ -11854,8 +12088,8 @@
       </c>
     </row>
     <row r="12" spans="1:16">
-      <c r="A12" s="212"/>
-      <c r="B12" s="213"/>
+      <c r="A12" s="211"/>
+      <c r="B12" s="212"/>
       <c r="C12" s="19" t="s">
         <v>168</v>
       </c>
@@ -11900,8 +12134,8 @@
       </c>
     </row>
     <row r="13" spans="1:16">
-      <c r="A13" s="212"/>
-      <c r="B13" s="213"/>
+      <c r="A13" s="211"/>
+      <c r="B13" s="212"/>
       <c r="C13" s="144" t="s">
         <v>169</v>
       </c>
@@ -11946,10 +12180,10 @@
       </c>
     </row>
     <row r="14" spans="1:16">
-      <c r="A14" s="211" t="s">
+      <c r="A14" s="209" t="s">
         <v>174</v>
       </c>
-      <c r="B14" s="214" t="s">
+      <c r="B14" s="213" t="s">
         <v>173</v>
       </c>
       <c r="C14" s="115" t="s">
@@ -11996,8 +12230,8 @@
       </c>
     </row>
     <row r="15" spans="1:16">
-      <c r="A15" s="211"/>
-      <c r="B15" s="214"/>
+      <c r="A15" s="209"/>
+      <c r="B15" s="213"/>
       <c r="C15" s="149" t="s">
         <v>167</v>
       </c>
@@ -12042,8 +12276,8 @@
       </c>
     </row>
     <row r="16" spans="1:16">
-      <c r="A16" s="211"/>
-      <c r="B16" s="214"/>
+      <c r="A16" s="209"/>
+      <c r="B16" s="213"/>
       <c r="C16" s="149" t="s">
         <v>168</v>
       </c>
@@ -12088,8 +12322,8 @@
       </c>
     </row>
     <row r="17" spans="1:16">
-      <c r="A17" s="211"/>
-      <c r="B17" s="214"/>
+      <c r="A17" s="209"/>
+      <c r="B17" s="213"/>
       <c r="C17" s="150" t="s">
         <v>169</v>
       </c>
@@ -12154,10 +12388,10 @@
       <c r="P18" s="155"/>
     </row>
     <row r="19" spans="1:16">
-      <c r="A19" s="215" t="s">
+      <c r="A19" s="200" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="216" t="s">
+      <c r="B19" s="201" t="s">
         <v>173</v>
       </c>
       <c r="C19" s="19" t="s">
@@ -12204,8 +12438,8 @@
       </c>
     </row>
     <row r="20" spans="1:16">
-      <c r="A20" s="215"/>
-      <c r="B20" s="216"/>
+      <c r="A20" s="200"/>
+      <c r="B20" s="201"/>
       <c r="C20" s="19" t="s">
         <v>167</v>
       </c>
@@ -12250,8 +12484,8 @@
       </c>
     </row>
     <row r="21" spans="1:16">
-      <c r="A21" s="215"/>
-      <c r="B21" s="216"/>
+      <c r="A21" s="200"/>
+      <c r="B21" s="201"/>
       <c r="C21" s="19" t="s">
         <v>168</v>
       </c>
@@ -12296,8 +12530,8 @@
       </c>
     </row>
     <row r="22" spans="1:16">
-      <c r="A22" s="215"/>
-      <c r="B22" s="216"/>
+      <c r="A22" s="200"/>
+      <c r="B22" s="201"/>
       <c r="C22" s="19" t="s">
         <v>169</v>
       </c>
@@ -12342,10 +12576,10 @@
       </c>
     </row>
     <row r="23" spans="1:16">
-      <c r="A23" s="215" t="s">
+      <c r="A23" s="200" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="216" t="s">
+      <c r="B23" s="201" t="s">
         <v>173</v>
       </c>
       <c r="C23" s="157" t="s">
@@ -12392,8 +12626,8 @@
       </c>
     </row>
     <row r="24" spans="1:16">
-      <c r="A24" s="215"/>
-      <c r="B24" s="216"/>
+      <c r="A24" s="200"/>
+      <c r="B24" s="201"/>
       <c r="C24" s="19" t="s">
         <v>167</v>
       </c>
@@ -12438,8 +12672,8 @@
       </c>
     </row>
     <row r="25" spans="1:16">
-      <c r="A25" s="215"/>
-      <c r="B25" s="216"/>
+      <c r="A25" s="200"/>
+      <c r="B25" s="201"/>
       <c r="C25" s="19" t="s">
         <v>168</v>
       </c>
@@ -12484,8 +12718,8 @@
       </c>
     </row>
     <row r="26" spans="1:16">
-      <c r="A26" s="215"/>
-      <c r="B26" s="216"/>
+      <c r="A26" s="200"/>
+      <c r="B26" s="201"/>
       <c r="C26" s="19" t="s">
         <v>169</v>
       </c>
@@ -12530,10 +12764,10 @@
       </c>
     </row>
     <row r="27" spans="1:16">
-      <c r="A27" s="215" t="s">
+      <c r="A27" s="200" t="s">
         <v>10</v>
       </c>
-      <c r="B27" s="216" t="s">
+      <c r="B27" s="201" t="s">
         <v>173</v>
       </c>
       <c r="C27" s="19" t="s">
@@ -12580,8 +12814,8 @@
       </c>
     </row>
     <row r="28" spans="1:16">
-      <c r="A28" s="215"/>
-      <c r="B28" s="216"/>
+      <c r="A28" s="200"/>
+      <c r="B28" s="201"/>
       <c r="C28" s="19" t="s">
         <v>167</v>
       </c>
@@ -12626,8 +12860,8 @@
       </c>
     </row>
     <row r="29" spans="1:16">
-      <c r="A29" s="215"/>
-      <c r="B29" s="216"/>
+      <c r="A29" s="200"/>
+      <c r="B29" s="201"/>
       <c r="C29" s="19" t="s">
         <v>168</v>
       </c>
@@ -12672,8 +12906,8 @@
       </c>
     </row>
     <row r="30" spans="1:16">
-      <c r="A30" s="215"/>
-      <c r="B30" s="216"/>
+      <c r="A30" s="200"/>
+      <c r="B30" s="201"/>
       <c r="C30" s="19" t="s">
         <v>169</v>
       </c>
@@ -12718,10 +12952,10 @@
       </c>
     </row>
     <row r="31" spans="1:16">
-      <c r="A31" s="215" t="s">
+      <c r="A31" s="200" t="s">
         <v>11</v>
       </c>
-      <c r="B31" s="216" t="s">
+      <c r="B31" s="201" t="s">
         <v>173</v>
       </c>
       <c r="C31" s="19" t="s">
@@ -12768,8 +13002,8 @@
       </c>
     </row>
     <row r="32" spans="1:16">
-      <c r="A32" s="215"/>
-      <c r="B32" s="216"/>
+      <c r="A32" s="200"/>
+      <c r="B32" s="201"/>
       <c r="C32" s="19" t="s">
         <v>167</v>
       </c>
@@ -12814,8 +13048,8 @@
       </c>
     </row>
     <row r="33" spans="1:16">
-      <c r="A33" s="215"/>
-      <c r="B33" s="216"/>
+      <c r="A33" s="200"/>
+      <c r="B33" s="201"/>
       <c r="C33" s="19" t="s">
         <v>168</v>
       </c>
@@ -12860,8 +13094,8 @@
       </c>
     </row>
     <row r="34" spans="1:16">
-      <c r="A34" s="215"/>
-      <c r="B34" s="216"/>
+      <c r="A34" s="200"/>
+      <c r="B34" s="201"/>
       <c r="C34" s="19" t="s">
         <v>169</v>
       </c>
@@ -12906,10 +13140,10 @@
       </c>
     </row>
     <row r="35" spans="1:16">
-      <c r="A35" s="215" t="s">
+      <c r="A35" s="200" t="s">
         <v>12</v>
       </c>
-      <c r="B35" s="216" t="s">
+      <c r="B35" s="201" t="s">
         <v>173</v>
       </c>
       <c r="C35" s="19" t="s">
@@ -12956,8 +13190,8 @@
       </c>
     </row>
     <row r="36" spans="1:16">
-      <c r="A36" s="215"/>
-      <c r="B36" s="216"/>
+      <c r="A36" s="200"/>
+      <c r="B36" s="201"/>
       <c r="C36" s="19" t="s">
         <v>167</v>
       </c>
@@ -13002,8 +13236,8 @@
       </c>
     </row>
     <row r="37" spans="1:16">
-      <c r="A37" s="215"/>
-      <c r="B37" s="216"/>
+      <c r="A37" s="200"/>
+      <c r="B37" s="201"/>
       <c r="C37" s="19" t="s">
         <v>168</v>
       </c>
@@ -13048,8 +13282,8 @@
       </c>
     </row>
     <row r="38" spans="1:16">
-      <c r="A38" s="215"/>
-      <c r="B38" s="216"/>
+      <c r="A38" s="200"/>
+      <c r="B38" s="201"/>
       <c r="C38" s="19" t="s">
         <v>169</v>
       </c>
@@ -13094,10 +13328,10 @@
       </c>
     </row>
     <row r="39" spans="1:16">
-      <c r="A39" s="215" t="s">
+      <c r="A39" s="200" t="s">
         <v>13</v>
       </c>
-      <c r="B39" s="216" t="s">
+      <c r="B39" s="201" t="s">
         <v>173</v>
       </c>
       <c r="C39" s="19" t="s">
@@ -13144,8 +13378,8 @@
       </c>
     </row>
     <row r="40" spans="1:16">
-      <c r="A40" s="215"/>
-      <c r="B40" s="216"/>
+      <c r="A40" s="200"/>
+      <c r="B40" s="201"/>
       <c r="C40" s="19" t="s">
         <v>167</v>
       </c>
@@ -13190,8 +13424,8 @@
       </c>
     </row>
     <row r="41" spans="1:16">
-      <c r="A41" s="215"/>
-      <c r="B41" s="216"/>
+      <c r="A41" s="200"/>
+      <c r="B41" s="201"/>
       <c r="C41" s="19" t="s">
         <v>168</v>
       </c>
@@ -13236,8 +13470,8 @@
       </c>
     </row>
     <row r="42" spans="1:16">
-      <c r="A42" s="215"/>
-      <c r="B42" s="216"/>
+      <c r="A42" s="200"/>
+      <c r="B42" s="201"/>
       <c r="C42" s="19" t="s">
         <v>169</v>
       </c>
@@ -13282,10 +13516,10 @@
       </c>
     </row>
     <row r="43" spans="1:16">
-      <c r="A43" s="215" t="s">
+      <c r="A43" s="200" t="s">
         <v>14</v>
       </c>
-      <c r="B43" s="216" t="s">
+      <c r="B43" s="201" t="s">
         <v>173</v>
       </c>
       <c r="C43" s="19" t="s">
@@ -13332,8 +13566,8 @@
       </c>
     </row>
     <row r="44" spans="1:16">
-      <c r="A44" s="215"/>
-      <c r="B44" s="216"/>
+      <c r="A44" s="200"/>
+      <c r="B44" s="201"/>
       <c r="C44" s="19" t="s">
         <v>167</v>
       </c>
@@ -13378,8 +13612,8 @@
       </c>
     </row>
     <row r="45" spans="1:16">
-      <c r="A45" s="215"/>
-      <c r="B45" s="216"/>
+      <c r="A45" s="200"/>
+      <c r="B45" s="201"/>
       <c r="C45" s="19" t="s">
         <v>168</v>
       </c>
@@ -13424,8 +13658,8 @@
       </c>
     </row>
     <row r="46" spans="1:16">
-      <c r="A46" s="215"/>
-      <c r="B46" s="216"/>
+      <c r="A46" s="200"/>
+      <c r="B46" s="201"/>
       <c r="C46" s="19" t="s">
         <v>169</v>
       </c>
@@ -13470,10 +13704,10 @@
       </c>
     </row>
     <row r="47" spans="1:16">
-      <c r="A47" s="219" t="s">
+      <c r="A47" s="202" t="s">
         <v>15</v>
       </c>
-      <c r="B47" s="216" t="s">
+      <c r="B47" s="201" t="s">
         <v>173</v>
       </c>
       <c r="C47" s="19" t="s">
@@ -13520,8 +13754,8 @@
       </c>
     </row>
     <row r="48" spans="1:16">
-      <c r="A48" s="219"/>
-      <c r="B48" s="216"/>
+      <c r="A48" s="202"/>
+      <c r="B48" s="201"/>
       <c r="C48" s="19" t="s">
         <v>167</v>
       </c>
@@ -13566,8 +13800,8 @@
       </c>
     </row>
     <row r="49" spans="1:16">
-      <c r="A49" s="219"/>
-      <c r="B49" s="216"/>
+      <c r="A49" s="202"/>
+      <c r="B49" s="201"/>
       <c r="C49" s="19" t="s">
         <v>168</v>
       </c>
@@ -13612,8 +13846,8 @@
       </c>
     </row>
     <row r="50" spans="1:16">
-      <c r="A50" s="219"/>
-      <c r="B50" s="216"/>
+      <c r="A50" s="202"/>
+      <c r="B50" s="201"/>
       <c r="C50" s="19" t="s">
         <v>169</v>
       </c>
@@ -13658,10 +13892,10 @@
       </c>
     </row>
     <row r="51" spans="1:16">
-      <c r="A51" s="220" t="s">
+      <c r="A51" s="203" t="s">
         <v>16</v>
       </c>
-      <c r="B51" s="221" t="s">
+      <c r="B51" s="204" t="s">
         <v>173</v>
       </c>
       <c r="C51" s="19" t="s">
@@ -13708,8 +13942,8 @@
       </c>
     </row>
     <row r="52" spans="1:16">
-      <c r="A52" s="220"/>
-      <c r="B52" s="221"/>
+      <c r="A52" s="203"/>
+      <c r="B52" s="204"/>
       <c r="C52" s="19" t="s">
         <v>167</v>
       </c>
@@ -13754,8 +13988,8 @@
       </c>
     </row>
     <row r="53" spans="1:16">
-      <c r="A53" s="220"/>
-      <c r="B53" s="221"/>
+      <c r="A53" s="203"/>
+      <c r="B53" s="204"/>
       <c r="C53" s="19" t="s">
         <v>168</v>
       </c>
@@ -13800,8 +14034,8 @@
       </c>
     </row>
     <row r="54" spans="1:16">
-      <c r="A54" s="220"/>
-      <c r="B54" s="221"/>
+      <c r="A54" s="203"/>
+      <c r="B54" s="204"/>
       <c r="C54" s="123" t="s">
         <v>169</v>
       </c>
@@ -13890,7 +14124,7 @@
       </c>
     </row>
     <row r="59" spans="1:16">
-      <c r="A59" s="217" t="s">
+      <c r="A59" s="198" t="s">
         <v>196</v>
       </c>
       <c r="B59" s="17" t="s">
@@ -13934,7 +14168,7 @@
       </c>
     </row>
     <row r="60" spans="1:16">
-      <c r="A60" s="218"/>
+      <c r="A60" s="199"/>
       <c r="B60" s="17" t="s">
         <v>194</v>
       </c>
@@ -13976,7 +14210,7 @@
       </c>
     </row>
     <row r="61" spans="1:16">
-      <c r="A61" s="222"/>
+      <c r="A61" s="205"/>
       <c r="B61" s="17" t="s">
         <v>195</v>
       </c>
@@ -14018,7 +14252,7 @@
       </c>
     </row>
     <row r="62" spans="1:16">
-      <c r="A62" s="217" t="s">
+      <c r="A62" s="198" t="s">
         <v>197</v>
       </c>
       <c r="B62" s="17" t="s">
@@ -14062,7 +14296,7 @@
       </c>
     </row>
     <row r="63" spans="1:16">
-      <c r="A63" s="218"/>
+      <c r="A63" s="199"/>
       <c r="B63" s="17" t="s">
         <v>194</v>
       </c>
@@ -14104,7 +14338,7 @@
       </c>
     </row>
     <row r="64" spans="1:16">
-      <c r="A64" s="222"/>
+      <c r="A64" s="205"/>
       <c r="B64" s="17" t="s">
         <v>195</v>
       </c>
@@ -14146,7 +14380,7 @@
       </c>
     </row>
     <row r="65" spans="1:14">
-      <c r="A65" s="217" t="s">
+      <c r="A65" s="198" t="s">
         <v>186</v>
       </c>
       <c r="B65" s="17" t="s">
@@ -14202,7 +14436,7 @@
       </c>
     </row>
     <row r="66" spans="1:14">
-      <c r="A66" s="218"/>
+      <c r="A66" s="199"/>
       <c r="B66" s="17" t="s">
         <v>194</v>
       </c>
@@ -14244,7 +14478,7 @@
       </c>
     </row>
     <row r="67" spans="1:14">
-      <c r="A67" s="222"/>
+      <c r="A67" s="205"/>
       <c r="B67" s="17" t="s">
         <v>195</v>
       </c>
@@ -14286,7 +14520,7 @@
       </c>
     </row>
     <row r="68" spans="1:14">
-      <c r="A68" s="217" t="s">
+      <c r="A68" s="198" t="s">
         <v>187</v>
       </c>
       <c r="B68" s="17" t="s">
@@ -14330,7 +14564,7 @@
       </c>
     </row>
     <row r="69" spans="1:14">
-      <c r="A69" s="218"/>
+      <c r="A69" s="199"/>
       <c r="B69" s="17" t="s">
         <v>194</v>
       </c>
@@ -14372,7 +14606,7 @@
       </c>
     </row>
     <row r="70" spans="1:14">
-      <c r="A70" s="222"/>
+      <c r="A70" s="205"/>
       <c r="B70" s="17" t="s">
         <v>195</v>
       </c>
@@ -14414,7 +14648,7 @@
       </c>
     </row>
     <row r="71" spans="1:14">
-      <c r="A71" s="217" t="s">
+      <c r="A71" s="198" t="s">
         <v>188</v>
       </c>
       <c r="B71" s="17" t="s">
@@ -14458,7 +14692,7 @@
       </c>
     </row>
     <row r="72" spans="1:14">
-      <c r="A72" s="218"/>
+      <c r="A72" s="199"/>
       <c r="B72" s="17" t="s">
         <v>194</v>
       </c>
@@ -14500,7 +14734,7 @@
       </c>
     </row>
     <row r="73" spans="1:14">
-      <c r="A73" s="222"/>
+      <c r="A73" s="205"/>
       <c r="B73" s="17" t="s">
         <v>195</v>
       </c>
@@ -14542,7 +14776,7 @@
       </c>
     </row>
     <row r="74" spans="1:14">
-      <c r="A74" s="217" t="s">
+      <c r="A74" s="198" t="s">
         <v>189</v>
       </c>
       <c r="B74" s="17" t="s">
@@ -14586,7 +14820,7 @@
       </c>
     </row>
     <row r="75" spans="1:14">
-      <c r="A75" s="218"/>
+      <c r="A75" s="199"/>
       <c r="B75" s="17" t="s">
         <v>194</v>
       </c>
@@ -14628,7 +14862,7 @@
       </c>
     </row>
     <row r="76" spans="1:14">
-      <c r="A76" s="222"/>
+      <c r="A76" s="205"/>
       <c r="B76" s="17" t="s">
         <v>195</v>
       </c>
@@ -14670,7 +14904,7 @@
       </c>
     </row>
     <row r="77" spans="1:14">
-      <c r="A77" s="217" t="s">
+      <c r="A77" s="198" t="s">
         <v>190</v>
       </c>
       <c r="B77" s="17" t="s">
@@ -14714,7 +14948,7 @@
       </c>
     </row>
     <row r="78" spans="1:14">
-      <c r="A78" s="218"/>
+      <c r="A78" s="199"/>
       <c r="B78" s="17" t="s">
         <v>194</v>
       </c>
@@ -14756,7 +14990,7 @@
       </c>
     </row>
     <row r="79" spans="1:14">
-      <c r="A79" s="222"/>
+      <c r="A79" s="205"/>
       <c r="B79" s="17" t="s">
         <v>195</v>
       </c>
@@ -14798,7 +15032,7 @@
       </c>
     </row>
     <row r="80" spans="1:14">
-      <c r="A80" s="217" t="s">
+      <c r="A80" s="198" t="s">
         <v>191</v>
       </c>
       <c r="B80" s="17" t="s">
@@ -14842,7 +15076,7 @@
       </c>
     </row>
     <row r="81" spans="1:14">
-      <c r="A81" s="218"/>
+      <c r="A81" s="199"/>
       <c r="B81" s="17" t="s">
         <v>194</v>
       </c>
@@ -14884,7 +15118,7 @@
       </c>
     </row>
     <row r="82" spans="1:14">
-      <c r="A82" s="222"/>
+      <c r="A82" s="205"/>
       <c r="B82" s="17" t="s">
         <v>195</v>
       </c>
@@ -14926,7 +15160,7 @@
       </c>
     </row>
     <row r="83" spans="1:14">
-      <c r="A83" s="217" t="s">
+      <c r="A83" s="198" t="s">
         <v>198</v>
       </c>
       <c r="B83" s="17" t="s">
@@ -14970,7 +15204,7 @@
       </c>
     </row>
     <row r="84" spans="1:14">
-      <c r="A84" s="218"/>
+      <c r="A84" s="199"/>
       <c r="B84" s="17" t="s">
         <v>194</v>
       </c>
@@ -15012,7 +15246,7 @@
       </c>
     </row>
     <row r="85" spans="1:14">
-      <c r="A85" s="222"/>
+      <c r="A85" s="205"/>
       <c r="B85" s="17" t="s">
         <v>195</v>
       </c>
@@ -15054,7 +15288,7 @@
       </c>
     </row>
     <row r="86" spans="1:14">
-      <c r="A86" s="217" t="s">
+      <c r="A86" s="198" t="s">
         <v>199</v>
       </c>
       <c r="B86" s="17" t="s">
@@ -15098,7 +15332,7 @@
       </c>
     </row>
     <row r="87" spans="1:14">
-      <c r="A87" s="218"/>
+      <c r="A87" s="199"/>
       <c r="B87" s="17" t="s">
         <v>194</v>
       </c>
@@ -15140,7 +15374,7 @@
       </c>
     </row>
     <row r="88" spans="1:14">
-      <c r="A88" s="222"/>
+      <c r="A88" s="205"/>
       <c r="B88" s="17" t="s">
         <v>195</v>
       </c>
@@ -15182,7 +15416,7 @@
       </c>
     </row>
     <row r="89" spans="1:14">
-      <c r="A89" s="217" t="s">
+      <c r="A89" s="198" t="s">
         <v>200</v>
       </c>
       <c r="B89" s="17" t="s">
@@ -15226,7 +15460,7 @@
       </c>
     </row>
     <row r="90" spans="1:14">
-      <c r="A90" s="218"/>
+      <c r="A90" s="199"/>
       <c r="B90" s="17" t="s">
         <v>194</v>
       </c>
@@ -15268,7 +15502,7 @@
       </c>
     </row>
     <row r="91" spans="1:14">
-      <c r="A91" s="222"/>
+      <c r="A91" s="205"/>
       <c r="B91" s="17" t="s">
         <v>195</v>
       </c>
@@ -15310,7 +15544,7 @@
       </c>
     </row>
     <row r="92" spans="1:14">
-      <c r="A92" s="217" t="s">
+      <c r="A92" s="198" t="s">
         <v>201</v>
       </c>
       <c r="B92" s="17" t="s">
@@ -15354,7 +15588,7 @@
       </c>
     </row>
     <row r="93" spans="1:14">
-      <c r="A93" s="218"/>
+      <c r="A93" s="199"/>
       <c r="B93" s="17" t="s">
         <v>194</v>
       </c>
@@ -15396,7 +15630,7 @@
       </c>
     </row>
     <row r="94" spans="1:14">
-      <c r="A94" s="222"/>
+      <c r="A94" s="205"/>
       <c r="B94" s="17" t="s">
         <v>195</v>
       </c>
@@ -15438,7 +15672,7 @@
       </c>
     </row>
     <row r="95" spans="1:14">
-      <c r="A95" s="217" t="s">
+      <c r="A95" s="198" t="s">
         <v>202</v>
       </c>
       <c r="B95" s="17" t="s">
@@ -15482,7 +15716,7 @@
       </c>
     </row>
     <row r="96" spans="1:14">
-      <c r="A96" s="218"/>
+      <c r="A96" s="199"/>
       <c r="B96" s="17" t="s">
         <v>194</v>
       </c>
@@ -15524,7 +15758,7 @@
       </c>
     </row>
     <row r="97" spans="1:14">
-      <c r="A97" s="222"/>
+      <c r="A97" s="205"/>
       <c r="B97" s="17" t="s">
         <v>195</v>
       </c>
@@ -15566,7 +15800,7 @@
       </c>
     </row>
     <row r="98" spans="1:14">
-      <c r="A98" s="217" t="s">
+      <c r="A98" s="198" t="s">
         <v>203</v>
       </c>
       <c r="B98" s="17" t="s">
@@ -15610,7 +15844,7 @@
       </c>
     </row>
     <row r="99" spans="1:14">
-      <c r="A99" s="218"/>
+      <c r="A99" s="199"/>
       <c r="B99" s="17" t="s">
         <v>194</v>
       </c>
@@ -15652,7 +15886,7 @@
       </c>
     </row>
     <row r="100" spans="1:14">
-      <c r="A100" s="222"/>
+      <c r="A100" s="205"/>
       <c r="B100" s="17" t="s">
         <v>195</v>
       </c>
@@ -15694,7 +15928,7 @@
       </c>
     </row>
     <row r="101" spans="1:14">
-      <c r="A101" s="217" t="s">
+      <c r="A101" s="198" t="s">
         <v>204</v>
       </c>
       <c r="B101" s="17" t="s">
@@ -15738,7 +15972,7 @@
       </c>
     </row>
     <row r="102" spans="1:14">
-      <c r="A102" s="218"/>
+      <c r="A102" s="199"/>
       <c r="B102" s="17" t="s">
         <v>194</v>
       </c>
@@ -15780,7 +16014,7 @@
       </c>
     </row>
     <row r="103" spans="1:14">
-      <c r="A103" s="222"/>
+      <c r="A103" s="205"/>
       <c r="B103" s="17" t="s">
         <v>195</v>
       </c>
@@ -15866,7 +16100,7 @@
       </c>
     </row>
     <row r="105" spans="1:14">
-      <c r="A105" s="217" t="s">
+      <c r="A105" s="198" t="s">
         <v>212</v>
       </c>
       <c r="B105" s="17" t="s">
@@ -15910,7 +16144,7 @@
       </c>
     </row>
     <row r="106" spans="1:14">
-      <c r="A106" s="218"/>
+      <c r="A106" s="199"/>
       <c r="B106" s="17" t="s">
         <v>214</v>
       </c>
@@ -15953,6 +16187,32 @@
     </row>
   </sheetData>
   <mergeCells count="42">
+    <mergeCell ref="A98:A100"/>
+    <mergeCell ref="A101:A103"/>
+    <mergeCell ref="A77:A79"/>
+    <mergeCell ref="A80:A82"/>
+    <mergeCell ref="A83:A85"/>
+    <mergeCell ref="A86:A88"/>
+    <mergeCell ref="A89:A91"/>
+    <mergeCell ref="A92:A94"/>
+    <mergeCell ref="A95:A97"/>
+    <mergeCell ref="A27:A30"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="A31:A34"/>
+    <mergeCell ref="A59:A61"/>
+    <mergeCell ref="A62:A64"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="A23:A26"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="B10:B13"/>
     <mergeCell ref="A105:A106"/>
     <mergeCell ref="B31:B34"/>
     <mergeCell ref="A35:A38"/>
@@ -15969,32 +16229,6 @@
     <mergeCell ref="A65:A67"/>
     <mergeCell ref="A68:A70"/>
     <mergeCell ref="A71:A73"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="A14:A17"/>
-    <mergeCell ref="B14:B17"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="A23:A26"/>
-    <mergeCell ref="B23:B26"/>
-    <mergeCell ref="A27:A30"/>
-    <mergeCell ref="B27:B30"/>
-    <mergeCell ref="A31:A34"/>
-    <mergeCell ref="A59:A61"/>
-    <mergeCell ref="A62:A64"/>
-    <mergeCell ref="A98:A100"/>
-    <mergeCell ref="A101:A103"/>
-    <mergeCell ref="A77:A79"/>
-    <mergeCell ref="A80:A82"/>
-    <mergeCell ref="A83:A85"/>
-    <mergeCell ref="A86:A88"/>
-    <mergeCell ref="A89:A91"/>
-    <mergeCell ref="A92:A94"/>
-    <mergeCell ref="A95:A97"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -16070,7 +16304,7 @@
       </c>
     </row>
     <row r="2" spans="1:16" ht="13.5" customHeight="1">
-      <c r="A2" s="209" t="s">
+      <c r="A2" s="217" t="s">
         <v>165</v>
       </c>
       <c r="B2" s="210" t="s">
@@ -16120,7 +16354,7 @@
       </c>
     </row>
     <row r="3" spans="1:16">
-      <c r="A3" s="209"/>
+      <c r="A3" s="217"/>
       <c r="B3" s="210"/>
       <c r="C3" s="19" t="s">
         <v>167</v>
@@ -16166,7 +16400,7 @@
       </c>
     </row>
     <row r="4" spans="1:16">
-      <c r="A4" s="209"/>
+      <c r="A4" s="217"/>
       <c r="B4" s="210"/>
       <c r="C4" s="19" t="s">
         <v>168</v>
@@ -16212,7 +16446,7 @@
       </c>
     </row>
     <row r="5" spans="1:16">
-      <c r="A5" s="209"/>
+      <c r="A5" s="217"/>
       <c r="B5" s="210"/>
       <c r="C5" s="123" t="s">
         <v>169</v>
@@ -16258,7 +16492,7 @@
       </c>
     </row>
     <row r="6" spans="1:16" ht="13.5" customHeight="1">
-      <c r="A6" s="211" t="s">
+      <c r="A6" s="209" t="s">
         <v>170</v>
       </c>
       <c r="B6" s="210" t="s">
@@ -16308,7 +16542,7 @@
       </c>
     </row>
     <row r="7" spans="1:16">
-      <c r="A7" s="211"/>
+      <c r="A7" s="209"/>
       <c r="B7" s="210"/>
       <c r="C7" s="19" t="s">
         <v>167</v>
@@ -16354,7 +16588,7 @@
       </c>
     </row>
     <row r="8" spans="1:16">
-      <c r="A8" s="211"/>
+      <c r="A8" s="209"/>
       <c r="B8" s="210"/>
       <c r="C8" s="19" t="s">
         <v>168</v>
@@ -16400,7 +16634,7 @@
       </c>
     </row>
     <row r="9" spans="1:16">
-      <c r="A9" s="211"/>
+      <c r="A9" s="209"/>
       <c r="B9" s="210"/>
       <c r="C9" s="123" t="s">
         <v>169</v>
@@ -16446,10 +16680,10 @@
       </c>
     </row>
     <row r="10" spans="1:16">
-      <c r="A10" s="212" t="s">
+      <c r="A10" s="211" t="s">
         <v>172</v>
       </c>
-      <c r="B10" s="213" t="s">
+      <c r="B10" s="212" t="s">
         <v>173</v>
       </c>
       <c r="C10" s="115" t="s">
@@ -16496,8 +16730,8 @@
       </c>
     </row>
     <row r="11" spans="1:16">
-      <c r="A11" s="212"/>
-      <c r="B11" s="213"/>
+      <c r="A11" s="211"/>
+      <c r="B11" s="212"/>
       <c r="C11" s="19" t="s">
         <v>167</v>
       </c>
@@ -16542,8 +16776,8 @@
       </c>
     </row>
     <row r="12" spans="1:16">
-      <c r="A12" s="212"/>
-      <c r="B12" s="213"/>
+      <c r="A12" s="211"/>
+      <c r="B12" s="212"/>
       <c r="C12" s="19" t="s">
         <v>168</v>
       </c>
@@ -16588,8 +16822,8 @@
       </c>
     </row>
     <row r="13" spans="1:16">
-      <c r="A13" s="212"/>
-      <c r="B13" s="213"/>
+      <c r="A13" s="211"/>
+      <c r="B13" s="212"/>
       <c r="C13" s="144" t="s">
         <v>169</v>
       </c>
@@ -16634,10 +16868,10 @@
       </c>
     </row>
     <row r="14" spans="1:16">
-      <c r="A14" s="211" t="s">
+      <c r="A14" s="209" t="s">
         <v>174</v>
       </c>
-      <c r="B14" s="214" t="s">
+      <c r="B14" s="213" t="s">
         <v>173</v>
       </c>
       <c r="C14" s="115" t="s">
@@ -16685,8 +16919,8 @@
       </c>
     </row>
     <row r="15" spans="1:16">
-      <c r="A15" s="211"/>
-      <c r="B15" s="214"/>
+      <c r="A15" s="209"/>
+      <c r="B15" s="213"/>
       <c r="C15" s="149" t="s">
         <v>167</v>
       </c>
@@ -16732,8 +16966,8 @@
       </c>
     </row>
     <row r="16" spans="1:16">
-      <c r="A16" s="211"/>
-      <c r="B16" s="214"/>
+      <c r="A16" s="209"/>
+      <c r="B16" s="213"/>
       <c r="C16" s="149" t="s">
         <v>168</v>
       </c>
@@ -16779,8 +17013,8 @@
       </c>
     </row>
     <row r="17" spans="1:16">
-      <c r="A17" s="211"/>
-      <c r="B17" s="214"/>
+      <c r="A17" s="209"/>
+      <c r="B17" s="213"/>
       <c r="C17" s="150" t="s">
         <v>169</v>
       </c>
@@ -16846,10 +17080,10 @@
       <c r="P18" s="155"/>
     </row>
     <row r="19" spans="1:16">
-      <c r="A19" s="215" t="s">
+      <c r="A19" s="200" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="216" t="s">
+      <c r="B19" s="201" t="s">
         <v>173</v>
       </c>
       <c r="C19" s="19" t="s">
@@ -16896,8 +17130,8 @@
       </c>
     </row>
     <row r="20" spans="1:16">
-      <c r="A20" s="215"/>
-      <c r="B20" s="216"/>
+      <c r="A20" s="200"/>
+      <c r="B20" s="201"/>
       <c r="C20" s="19" t="s">
         <v>167</v>
       </c>
@@ -16942,8 +17176,8 @@
       </c>
     </row>
     <row r="21" spans="1:16">
-      <c r="A21" s="215"/>
-      <c r="B21" s="216"/>
+      <c r="A21" s="200"/>
+      <c r="B21" s="201"/>
       <c r="C21" s="19" t="s">
         <v>168</v>
       </c>
@@ -16988,8 +17222,8 @@
       </c>
     </row>
     <row r="22" spans="1:16">
-      <c r="A22" s="215"/>
-      <c r="B22" s="216"/>
+      <c r="A22" s="200"/>
+      <c r="B22" s="201"/>
       <c r="C22" s="19" t="s">
         <v>169</v>
       </c>
@@ -17034,10 +17268,10 @@
       </c>
     </row>
     <row r="23" spans="1:16">
-      <c r="A23" s="215" t="s">
+      <c r="A23" s="200" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="216" t="s">
+      <c r="B23" s="201" t="s">
         <v>173</v>
       </c>
       <c r="C23" s="157" t="s">
@@ -17084,8 +17318,8 @@
       </c>
     </row>
     <row r="24" spans="1:16">
-      <c r="A24" s="215"/>
-      <c r="B24" s="216"/>
+      <c r="A24" s="200"/>
+      <c r="B24" s="201"/>
       <c r="C24" s="19" t="s">
         <v>167</v>
       </c>
@@ -17130,8 +17364,8 @@
       </c>
     </row>
     <row r="25" spans="1:16">
-      <c r="A25" s="215"/>
-      <c r="B25" s="216"/>
+      <c r="A25" s="200"/>
+      <c r="B25" s="201"/>
       <c r="C25" s="19" t="s">
         <v>168</v>
       </c>
@@ -17176,8 +17410,8 @@
       </c>
     </row>
     <row r="26" spans="1:16">
-      <c r="A26" s="215"/>
-      <c r="B26" s="216"/>
+      <c r="A26" s="200"/>
+      <c r="B26" s="201"/>
       <c r="C26" s="19" t="s">
         <v>169</v>
       </c>
@@ -17222,10 +17456,10 @@
       </c>
     </row>
     <row r="27" spans="1:16">
-      <c r="A27" s="215" t="s">
+      <c r="A27" s="200" t="s">
         <v>10</v>
       </c>
-      <c r="B27" s="216" t="s">
+      <c r="B27" s="201" t="s">
         <v>173</v>
       </c>
       <c r="C27" s="19" t="s">
@@ -17272,8 +17506,8 @@
       </c>
     </row>
     <row r="28" spans="1:16">
-      <c r="A28" s="215"/>
-      <c r="B28" s="216"/>
+      <c r="A28" s="200"/>
+      <c r="B28" s="201"/>
       <c r="C28" s="19" t="s">
         <v>167</v>
       </c>
@@ -17318,8 +17552,8 @@
       </c>
     </row>
     <row r="29" spans="1:16">
-      <c r="A29" s="215"/>
-      <c r="B29" s="216"/>
+      <c r="A29" s="200"/>
+      <c r="B29" s="201"/>
       <c r="C29" s="19" t="s">
         <v>168</v>
       </c>
@@ -17364,8 +17598,8 @@
       </c>
     </row>
     <row r="30" spans="1:16">
-      <c r="A30" s="215"/>
-      <c r="B30" s="216"/>
+      <c r="A30" s="200"/>
+      <c r="B30" s="201"/>
       <c r="C30" s="19" t="s">
         <v>169</v>
       </c>
@@ -17410,10 +17644,10 @@
       </c>
     </row>
     <row r="31" spans="1:16">
-      <c r="A31" s="215" t="s">
+      <c r="A31" s="200" t="s">
         <v>11</v>
       </c>
-      <c r="B31" s="216" t="s">
+      <c r="B31" s="201" t="s">
         <v>173</v>
       </c>
       <c r="C31" s="19" t="s">
@@ -17460,8 +17694,8 @@
       </c>
     </row>
     <row r="32" spans="1:16">
-      <c r="A32" s="215"/>
-      <c r="B32" s="216"/>
+      <c r="A32" s="200"/>
+      <c r="B32" s="201"/>
       <c r="C32" s="19" t="s">
         <v>167</v>
       </c>
@@ -17506,8 +17740,8 @@
       </c>
     </row>
     <row r="33" spans="1:16">
-      <c r="A33" s="215"/>
-      <c r="B33" s="216"/>
+      <c r="A33" s="200"/>
+      <c r="B33" s="201"/>
       <c r="C33" s="19" t="s">
         <v>168</v>
       </c>
@@ -17552,8 +17786,8 @@
       </c>
     </row>
     <row r="34" spans="1:16">
-      <c r="A34" s="215"/>
-      <c r="B34" s="216"/>
+      <c r="A34" s="200"/>
+      <c r="B34" s="201"/>
       <c r="C34" s="19" t="s">
         <v>169</v>
       </c>
@@ -17598,10 +17832,10 @@
       </c>
     </row>
     <row r="35" spans="1:16">
-      <c r="A35" s="215" t="s">
+      <c r="A35" s="200" t="s">
         <v>12</v>
       </c>
-      <c r="B35" s="216" t="s">
+      <c r="B35" s="201" t="s">
         <v>173</v>
       </c>
       <c r="C35" s="19" t="s">
@@ -17648,8 +17882,8 @@
       </c>
     </row>
     <row r="36" spans="1:16">
-      <c r="A36" s="215"/>
-      <c r="B36" s="216"/>
+      <c r="A36" s="200"/>
+      <c r="B36" s="201"/>
       <c r="C36" s="19" t="s">
         <v>167</v>
       </c>
@@ -17694,8 +17928,8 @@
       </c>
     </row>
     <row r="37" spans="1:16">
-      <c r="A37" s="215"/>
-      <c r="B37" s="216"/>
+      <c r="A37" s="200"/>
+      <c r="B37" s="201"/>
       <c r="C37" s="19" t="s">
         <v>168</v>
       </c>
@@ -17740,8 +17974,8 @@
       </c>
     </row>
     <row r="38" spans="1:16">
-      <c r="A38" s="215"/>
-      <c r="B38" s="216"/>
+      <c r="A38" s="200"/>
+      <c r="B38" s="201"/>
       <c r="C38" s="19" t="s">
         <v>169</v>
       </c>
@@ -17786,10 +18020,10 @@
       </c>
     </row>
     <row r="39" spans="1:16">
-      <c r="A39" s="215" t="s">
+      <c r="A39" s="200" t="s">
         <v>13</v>
       </c>
-      <c r="B39" s="216" t="s">
+      <c r="B39" s="201" t="s">
         <v>173</v>
       </c>
       <c r="C39" s="19" t="s">
@@ -17836,8 +18070,8 @@
       </c>
     </row>
     <row r="40" spans="1:16">
-      <c r="A40" s="215"/>
-      <c r="B40" s="216"/>
+      <c r="A40" s="200"/>
+      <c r="B40" s="201"/>
       <c r="C40" s="19" t="s">
         <v>167</v>
       </c>
@@ -17882,8 +18116,8 @@
       </c>
     </row>
     <row r="41" spans="1:16">
-      <c r="A41" s="215"/>
-      <c r="B41" s="216"/>
+      <c r="A41" s="200"/>
+      <c r="B41" s="201"/>
       <c r="C41" s="19" t="s">
         <v>168</v>
       </c>
@@ -17928,8 +18162,8 @@
       </c>
     </row>
     <row r="42" spans="1:16">
-      <c r="A42" s="215"/>
-      <c r="B42" s="216"/>
+      <c r="A42" s="200"/>
+      <c r="B42" s="201"/>
       <c r="C42" s="19" t="s">
         <v>169</v>
       </c>
@@ -17974,10 +18208,10 @@
       </c>
     </row>
     <row r="43" spans="1:16">
-      <c r="A43" s="215" t="s">
+      <c r="A43" s="200" t="s">
         <v>14</v>
       </c>
-      <c r="B43" s="216" t="s">
+      <c r="B43" s="201" t="s">
         <v>173</v>
       </c>
       <c r="C43" s="19" t="s">
@@ -18024,8 +18258,8 @@
       </c>
     </row>
     <row r="44" spans="1:16">
-      <c r="A44" s="215"/>
-      <c r="B44" s="216"/>
+      <c r="A44" s="200"/>
+      <c r="B44" s="201"/>
       <c r="C44" s="19" t="s">
         <v>167</v>
       </c>
@@ -18070,8 +18304,8 @@
       </c>
     </row>
     <row r="45" spans="1:16">
-      <c r="A45" s="215"/>
-      <c r="B45" s="216"/>
+      <c r="A45" s="200"/>
+      <c r="B45" s="201"/>
       <c r="C45" s="19" t="s">
         <v>168</v>
       </c>
@@ -18116,8 +18350,8 @@
       </c>
     </row>
     <row r="46" spans="1:16">
-      <c r="A46" s="215"/>
-      <c r="B46" s="216"/>
+      <c r="A46" s="200"/>
+      <c r="B46" s="201"/>
       <c r="C46" s="19" t="s">
         <v>169</v>
       </c>
@@ -18162,10 +18396,10 @@
       </c>
     </row>
     <row r="47" spans="1:16">
-      <c r="A47" s="219" t="s">
+      <c r="A47" s="202" t="s">
         <v>15</v>
       </c>
-      <c r="B47" s="216" t="s">
+      <c r="B47" s="201" t="s">
         <v>173</v>
       </c>
       <c r="C47" s="19" t="s">
@@ -18212,8 +18446,8 @@
       </c>
     </row>
     <row r="48" spans="1:16">
-      <c r="A48" s="219"/>
-      <c r="B48" s="216"/>
+      <c r="A48" s="202"/>
+      <c r="B48" s="201"/>
       <c r="C48" s="19" t="s">
         <v>167</v>
       </c>
@@ -18258,8 +18492,8 @@
       </c>
     </row>
     <row r="49" spans="1:23">
-      <c r="A49" s="219"/>
-      <c r="B49" s="216"/>
+      <c r="A49" s="202"/>
+      <c r="B49" s="201"/>
       <c r="C49" s="19" t="s">
         <v>168</v>
       </c>
@@ -18304,8 +18538,8 @@
       </c>
     </row>
     <row r="50" spans="1:23">
-      <c r="A50" s="219"/>
-      <c r="B50" s="216"/>
+      <c r="A50" s="202"/>
+      <c r="B50" s="201"/>
       <c r="C50" s="19" t="s">
         <v>169</v>
       </c>
@@ -18350,10 +18584,10 @@
       </c>
     </row>
     <row r="51" spans="1:23">
-      <c r="A51" s="220" t="s">
+      <c r="A51" s="203" t="s">
         <v>16</v>
       </c>
-      <c r="B51" s="221" t="s">
+      <c r="B51" s="204" t="s">
         <v>173</v>
       </c>
       <c r="C51" s="19" t="s">
@@ -18400,8 +18634,8 @@
       </c>
     </row>
     <row r="52" spans="1:23">
-      <c r="A52" s="220"/>
-      <c r="B52" s="221"/>
+      <c r="A52" s="203"/>
+      <c r="B52" s="204"/>
       <c r="C52" s="19" t="s">
         <v>167</v>
       </c>
@@ -18446,8 +18680,8 @@
       </c>
     </row>
     <row r="53" spans="1:23">
-      <c r="A53" s="220"/>
-      <c r="B53" s="221"/>
+      <c r="A53" s="203"/>
+      <c r="B53" s="204"/>
       <c r="C53" s="19" t="s">
         <v>168</v>
       </c>
@@ -18492,8 +18726,8 @@
       </c>
     </row>
     <row r="54" spans="1:23">
-      <c r="A54" s="220"/>
-      <c r="B54" s="221"/>
+      <c r="A54" s="203"/>
+      <c r="B54" s="204"/>
       <c r="C54" s="123" t="s">
         <v>169</v>
       </c>
@@ -18538,10 +18772,10 @@
       </c>
     </row>
     <row r="58" spans="1:23">
-      <c r="A58" s="223" t="s">
+      <c r="A58" s="226" t="s">
         <v>176</v>
       </c>
-      <c r="B58" s="223"/>
+      <c r="B58" s="226"/>
       <c r="C58" s="19">
         <v>1995</v>
       </c>
@@ -18864,7 +19098,7 @@
       </c>
     </row>
     <row r="65" spans="1:14">
-      <c r="A65" s="217" t="s">
+      <c r="A65" s="198" t="s">
         <v>196</v>
       </c>
       <c r="B65" s="17" t="s">
@@ -18908,7 +19142,7 @@
       </c>
     </row>
     <row r="66" spans="1:14">
-      <c r="A66" s="218"/>
+      <c r="A66" s="199"/>
       <c r="B66" s="17" t="s">
         <v>194</v>
       </c>
@@ -18950,7 +19184,7 @@
       </c>
     </row>
     <row r="67" spans="1:14">
-      <c r="A67" s="222"/>
+      <c r="A67" s="205"/>
       <c r="B67" s="17" t="s">
         <v>195</v>
       </c>
@@ -18992,7 +19226,7 @@
       </c>
     </row>
     <row r="68" spans="1:14">
-      <c r="A68" s="217" t="s">
+      <c r="A68" s="198" t="s">
         <v>197</v>
       </c>
       <c r="B68" s="17" t="s">
@@ -19036,7 +19270,7 @@
       </c>
     </row>
     <row r="69" spans="1:14">
-      <c r="A69" s="218"/>
+      <c r="A69" s="199"/>
       <c r="B69" s="17" t="s">
         <v>194</v>
       </c>
@@ -19078,7 +19312,7 @@
       </c>
     </row>
     <row r="70" spans="1:14">
-      <c r="A70" s="222"/>
+      <c r="A70" s="205"/>
       <c r="B70" s="17" t="s">
         <v>195</v>
       </c>
@@ -19120,7 +19354,7 @@
       </c>
     </row>
     <row r="71" spans="1:14">
-      <c r="A71" s="217" t="s">
+      <c r="A71" s="198" t="s">
         <v>186</v>
       </c>
       <c r="B71" s="17" t="s">
@@ -19164,7 +19398,7 @@
       </c>
     </row>
     <row r="72" spans="1:14">
-      <c r="A72" s="218"/>
+      <c r="A72" s="199"/>
       <c r="B72" s="17" t="s">
         <v>194</v>
       </c>
@@ -19206,7 +19440,7 @@
       </c>
     </row>
     <row r="73" spans="1:14">
-      <c r="A73" s="222"/>
+      <c r="A73" s="205"/>
       <c r="B73" s="17" t="s">
         <v>195</v>
       </c>
@@ -19248,7 +19482,7 @@
       </c>
     </row>
     <row r="74" spans="1:14">
-      <c r="A74" s="217" t="s">
+      <c r="A74" s="198" t="s">
         <v>187</v>
       </c>
       <c r="B74" s="17" t="s">
@@ -19292,7 +19526,7 @@
       </c>
     </row>
     <row r="75" spans="1:14">
-      <c r="A75" s="218"/>
+      <c r="A75" s="199"/>
       <c r="B75" s="17" t="s">
         <v>194</v>
       </c>
@@ -19334,7 +19568,7 @@
       </c>
     </row>
     <row r="76" spans="1:14">
-      <c r="A76" s="222"/>
+      <c r="A76" s="205"/>
       <c r="B76" s="17" t="s">
         <v>195</v>
       </c>
@@ -19376,7 +19610,7 @@
       </c>
     </row>
     <row r="77" spans="1:14">
-      <c r="A77" s="217" t="s">
+      <c r="A77" s="198" t="s">
         <v>188</v>
       </c>
       <c r="B77" s="17" t="s">
@@ -19420,7 +19654,7 @@
       </c>
     </row>
     <row r="78" spans="1:14">
-      <c r="A78" s="218"/>
+      <c r="A78" s="199"/>
       <c r="B78" s="17" t="s">
         <v>194</v>
       </c>
@@ -19462,7 +19696,7 @@
       </c>
     </row>
     <row r="79" spans="1:14">
-      <c r="A79" s="222"/>
+      <c r="A79" s="205"/>
       <c r="B79" s="17" t="s">
         <v>195</v>
       </c>
@@ -19504,7 +19738,7 @@
       </c>
     </row>
     <row r="80" spans="1:14">
-      <c r="A80" s="217" t="s">
+      <c r="A80" s="198" t="s">
         <v>189</v>
       </c>
       <c r="B80" s="17" t="s">
@@ -19548,7 +19782,7 @@
       </c>
     </row>
     <row r="81" spans="1:14">
-      <c r="A81" s="218"/>
+      <c r="A81" s="199"/>
       <c r="B81" s="17" t="s">
         <v>194</v>
       </c>
@@ -19590,7 +19824,7 @@
       </c>
     </row>
     <row r="82" spans="1:14">
-      <c r="A82" s="222"/>
+      <c r="A82" s="205"/>
       <c r="B82" s="17" t="s">
         <v>195</v>
       </c>
@@ -19632,7 +19866,7 @@
       </c>
     </row>
     <row r="83" spans="1:14">
-      <c r="A83" s="217" t="s">
+      <c r="A83" s="198" t="s">
         <v>190</v>
       </c>
       <c r="B83" s="17" t="s">
@@ -19676,7 +19910,7 @@
       </c>
     </row>
     <row r="84" spans="1:14">
-      <c r="A84" s="218"/>
+      <c r="A84" s="199"/>
       <c r="B84" s="17" t="s">
         <v>194</v>
       </c>
@@ -19718,7 +19952,7 @@
       </c>
     </row>
     <row r="85" spans="1:14">
-      <c r="A85" s="222"/>
+      <c r="A85" s="205"/>
       <c r="B85" s="17" t="s">
         <v>195</v>
       </c>
@@ -19760,7 +19994,7 @@
       </c>
     </row>
     <row r="86" spans="1:14">
-      <c r="A86" s="217" t="s">
+      <c r="A86" s="198" t="s">
         <v>191</v>
       </c>
       <c r="B86" s="17" t="s">
@@ -19804,7 +20038,7 @@
       </c>
     </row>
     <row r="87" spans="1:14">
-      <c r="A87" s="218"/>
+      <c r="A87" s="199"/>
       <c r="B87" s="17" t="s">
         <v>194</v>
       </c>
@@ -19846,7 +20080,7 @@
       </c>
     </row>
     <row r="88" spans="1:14">
-      <c r="A88" s="222"/>
+      <c r="A88" s="205"/>
       <c r="B88" s="17" t="s">
         <v>195</v>
       </c>
@@ -19888,7 +20122,7 @@
       </c>
     </row>
     <row r="89" spans="1:14">
-      <c r="A89" s="217" t="s">
+      <c r="A89" s="198" t="s">
         <v>198</v>
       </c>
       <c r="B89" s="17" t="s">
@@ -19932,7 +20166,7 @@
       </c>
     </row>
     <row r="90" spans="1:14">
-      <c r="A90" s="218"/>
+      <c r="A90" s="199"/>
       <c r="B90" s="17" t="s">
         <v>194</v>
       </c>
@@ -19974,7 +20208,7 @@
       </c>
     </row>
     <row r="91" spans="1:14">
-      <c r="A91" s="222"/>
+      <c r="A91" s="205"/>
       <c r="B91" s="17" t="s">
         <v>195</v>
       </c>
@@ -20016,7 +20250,7 @@
       </c>
     </row>
     <row r="92" spans="1:14">
-      <c r="A92" s="217" t="s">
+      <c r="A92" s="198" t="s">
         <v>199</v>
       </c>
       <c r="B92" s="17" t="s">
@@ -20060,7 +20294,7 @@
       </c>
     </row>
     <row r="93" spans="1:14">
-      <c r="A93" s="218"/>
+      <c r="A93" s="199"/>
       <c r="B93" s="17" t="s">
         <v>194</v>
       </c>
@@ -20102,7 +20336,7 @@
       </c>
     </row>
     <row r="94" spans="1:14" ht="16.5" customHeight="1">
-      <c r="A94" s="222"/>
+      <c r="A94" s="205"/>
       <c r="B94" s="17" t="s">
         <v>195</v>
       </c>
@@ -20144,7 +20378,7 @@
       </c>
     </row>
     <row r="95" spans="1:14">
-      <c r="A95" s="217" t="s">
+      <c r="A95" s="198" t="s">
         <v>200</v>
       </c>
       <c r="B95" s="17" t="s">
@@ -20188,7 +20422,7 @@
       </c>
     </row>
     <row r="96" spans="1:14">
-      <c r="A96" s="218"/>
+      <c r="A96" s="199"/>
       <c r="B96" s="17" t="s">
         <v>194</v>
       </c>
@@ -20230,7 +20464,7 @@
       </c>
     </row>
     <row r="97" spans="1:14">
-      <c r="A97" s="222"/>
+      <c r="A97" s="205"/>
       <c r="B97" s="17" t="s">
         <v>195</v>
       </c>
@@ -20272,7 +20506,7 @@
       </c>
     </row>
     <row r="98" spans="1:14">
-      <c r="A98" s="217" t="s">
+      <c r="A98" s="198" t="s">
         <v>201</v>
       </c>
       <c r="B98" s="17" t="s">
@@ -20316,7 +20550,7 @@
       </c>
     </row>
     <row r="99" spans="1:14">
-      <c r="A99" s="218"/>
+      <c r="A99" s="199"/>
       <c r="B99" s="17" t="s">
         <v>194</v>
       </c>
@@ -20358,7 +20592,7 @@
       </c>
     </row>
     <row r="100" spans="1:14">
-      <c r="A100" s="222"/>
+      <c r="A100" s="205"/>
       <c r="B100" s="17" t="s">
         <v>195</v>
       </c>
@@ -20400,7 +20634,7 @@
       </c>
     </row>
     <row r="101" spans="1:14">
-      <c r="A101" s="217" t="s">
+      <c r="A101" s="198" t="s">
         <v>202</v>
       </c>
       <c r="B101" s="17" t="s">
@@ -20444,7 +20678,7 @@
       </c>
     </row>
     <row r="102" spans="1:14">
-      <c r="A102" s="218"/>
+      <c r="A102" s="199"/>
       <c r="B102" s="17" t="s">
         <v>194</v>
       </c>
@@ -20486,7 +20720,7 @@
       </c>
     </row>
     <row r="103" spans="1:14">
-      <c r="A103" s="222"/>
+      <c r="A103" s="205"/>
       <c r="B103" s="17" t="s">
         <v>195</v>
       </c>
@@ -20528,7 +20762,7 @@
       </c>
     </row>
     <row r="104" spans="1:14">
-      <c r="A104" s="217" t="s">
+      <c r="A104" s="198" t="s">
         <v>203</v>
       </c>
       <c r="B104" s="17" t="s">
@@ -20572,7 +20806,7 @@
       </c>
     </row>
     <row r="105" spans="1:14">
-      <c r="A105" s="218"/>
+      <c r="A105" s="199"/>
       <c r="B105" s="17" t="s">
         <v>194</v>
       </c>
@@ -20614,7 +20848,7 @@
       </c>
     </row>
     <row r="106" spans="1:14">
-      <c r="A106" s="222"/>
+      <c r="A106" s="205"/>
       <c r="B106" s="17" t="s">
         <v>195</v>
       </c>
@@ -20656,7 +20890,7 @@
       </c>
     </row>
     <row r="107" spans="1:14">
-      <c r="A107" s="217" t="s">
+      <c r="A107" s="198" t="s">
         <v>204</v>
       </c>
       <c r="B107" s="17" t="s">
@@ -20700,7 +20934,7 @@
       </c>
     </row>
     <row r="108" spans="1:14">
-      <c r="A108" s="218"/>
+      <c r="A108" s="199"/>
       <c r="B108" s="17" t="s">
         <v>194</v>
       </c>
@@ -20742,7 +20976,7 @@
       </c>
     </row>
     <row r="109" spans="1:14">
-      <c r="A109" s="222"/>
+      <c r="A109" s="205"/>
       <c r="B109" s="17" t="s">
         <v>195</v>
       </c>
@@ -20828,7 +21062,7 @@
       </c>
     </row>
     <row r="111" spans="1:14">
-      <c r="A111" s="217" t="s">
+      <c r="A111" s="198" t="s">
         <v>212</v>
       </c>
       <c r="B111" s="17" t="s">
@@ -20872,7 +21106,7 @@
       </c>
     </row>
     <row r="112" spans="1:14">
-      <c r="A112" s="218"/>
+      <c r="A112" s="199"/>
       <c r="B112" s="17" t="s">
         <v>214</v>
       </c>
@@ -20915,6 +21149,33 @@
     </row>
   </sheetData>
   <mergeCells count="43">
+    <mergeCell ref="A89:A91"/>
+    <mergeCell ref="A92:A94"/>
+    <mergeCell ref="A95:A97"/>
+    <mergeCell ref="A98:A100"/>
+    <mergeCell ref="A101:A103"/>
+    <mergeCell ref="A27:A30"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="A31:A34"/>
+    <mergeCell ref="A65:A67"/>
+    <mergeCell ref="A68:A70"/>
+    <mergeCell ref="B31:B34"/>
+    <mergeCell ref="A35:A38"/>
+    <mergeCell ref="B35:B38"/>
+    <mergeCell ref="A51:A54"/>
+    <mergeCell ref="B51:B54"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="A23:A26"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="B10:B13"/>
     <mergeCell ref="A111:A112"/>
     <mergeCell ref="A58:B58"/>
     <mergeCell ref="A39:A42"/>
@@ -20931,33 +21192,6 @@
     <mergeCell ref="A107:A109"/>
     <mergeCell ref="A83:A85"/>
     <mergeCell ref="A86:A88"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="A14:A17"/>
-    <mergeCell ref="B14:B17"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="A23:A26"/>
-    <mergeCell ref="B23:B26"/>
-    <mergeCell ref="A27:A30"/>
-    <mergeCell ref="B27:B30"/>
-    <mergeCell ref="A31:A34"/>
-    <mergeCell ref="A65:A67"/>
-    <mergeCell ref="A68:A70"/>
-    <mergeCell ref="B31:B34"/>
-    <mergeCell ref="A35:A38"/>
-    <mergeCell ref="B35:B38"/>
-    <mergeCell ref="A51:A54"/>
-    <mergeCell ref="B51:B54"/>
-    <mergeCell ref="A89:A91"/>
-    <mergeCell ref="A92:A94"/>
-    <mergeCell ref="A95:A97"/>
-    <mergeCell ref="A98:A100"/>
-    <mergeCell ref="A101:A103"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Updates on the models
</commit_message>
<xml_diff>
--- a/models/14sectors_cat/climate.xlsx
+++ b/models/14sectors_cat/climate.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="9945" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="9945" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Global" sheetId="1" r:id="rId1"/>
@@ -166,7 +166,6 @@
     <definedName name="initial_SF6_conc" localSheetId="1">World!$C$46</definedName>
     <definedName name="land_thickness" localSheetId="1">World!$G$23</definedName>
     <definedName name="last_historical_RF_year" localSheetId="1">World!$C$90</definedName>
-    <definedName name="last_year_process_emissions" localSheetId="1">World!$AD$202</definedName>
     <definedName name="layer_depth" localSheetId="1">World!$C$17:$C$20</definedName>
     <definedName name="mineral_aerosols_and_land_RF" localSheetId="1">World!$C$91</definedName>
     <definedName name="mixed_layer_depth" localSheetId="1">World!$C$15</definedName>
@@ -193,7 +192,6 @@
     <definedName name="preindustrial_HFC_conc" localSheetId="1">World!$C$61</definedName>
     <definedName name="preindustrial_PFC_conc" localSheetId="1">World!$C$44</definedName>
     <definedName name="preindustrial_SF6_conc" localSheetId="1">World!$C$48</definedName>
-    <definedName name="process_emissions_intensity" localSheetId="1">World!$C$203:$AD$203</definedName>
     <definedName name="ref_buffer_factor" localSheetId="1">World!$C$12</definedName>
     <definedName name="reference_CH4_time_constant" localSheetId="1">World!$C$35</definedName>
     <definedName name="reference_CO2_radiative_forcing" localSheetId="1">World!$G$18</definedName>
@@ -224,7 +222,6 @@
     <definedName name="year_emissions" localSheetId="3">Catalonia!$D$1:$P$1</definedName>
     <definedName name="year_emissions" localSheetId="2">Europe!$D$1:$P$1</definedName>
     <definedName name="year_emissions" localSheetId="1">World!$D$94:$P$94</definedName>
-    <definedName name="years_process_emissions" localSheetId="1">World!$C$202:$AD$202</definedName>
   </definedNames>
   <calcPr calcId="125725" iterateDelta="1E-4"/>
   <extLst>
@@ -1452,7 +1449,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="739" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="734" uniqueCount="215">
   <si>
     <t>Global Warming Potentials</t>
   </si>
@@ -2097,18 +2094,6 @@
   </si>
   <si>
     <t>solid sorbent</t>
-  </si>
-  <si>
-    <t>Historic carbon intensity process emissions</t>
-  </si>
-  <si>
-    <t>Time</t>
-  </si>
-  <si>
-    <t>Process emission intensity</t>
-  </si>
-  <si>
-    <t>GtCO2/T$</t>
   </si>
 </sst>
 </file>
@@ -3409,8 +3394,6 @@
     <xf numFmtId="9" fontId="9" fillId="0" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3419,33 +3402,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="16" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3456,32 +3412,14 @@
     <xf numFmtId="0" fontId="3" fillId="16" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3498,18 +3436,65 @@
     <xf numFmtId="0" fontId="2" fillId="12" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
@@ -3623,7 +3608,7 @@
         <xdr:cNvPr id="2" name="CustomShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3996,8 +3981,8 @@
   </sheetPr>
   <dimension ref="A1:FI57"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A60" sqref="A60:XFD62"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="H49" sqref="H49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -4012,11 +3997,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:165">
-      <c r="A1" s="194" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="194"/>
-      <c r="C1" s="194"/>
+      <c r="A1" s="192" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="192"/>
+      <c r="C1" s="192"/>
       <c r="E1" s="1"/>
       <c r="F1" s="2"/>
       <c r="G1" s="3"/>
@@ -4587,11 +4572,11 @@
       </c>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="195" t="s">
+      <c r="A17" s="193" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="195"/>
-      <c r="C17" s="195"/>
+      <c r="B17" s="193"/>
+      <c r="C17" s="193"/>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="17" t="s">
@@ -4965,12 +4950,12 @@
       </c>
     </row>
     <row r="48" spans="1:4">
-      <c r="A48" s="196" t="s">
+      <c r="A48" s="194" t="s">
         <v>184</v>
       </c>
-      <c r="B48" s="196"/>
-      <c r="C48" s="196"/>
-      <c r="D48" s="196"/>
+      <c r="B48" s="194"/>
+      <c r="C48" s="194"/>
+      <c r="D48" s="194"/>
     </row>
     <row r="49" spans="1:7">
       <c r="A49" s="17"/>
@@ -5016,16 +5001,16 @@
       <c r="G52" s="187"/>
     </row>
     <row r="54" spans="1:7">
-      <c r="A54" s="197" t="s">
+      <c r="A54" s="225" t="s">
         <v>208</v>
       </c>
-      <c r="B54" s="197"/>
-      <c r="C54" s="197"/>
-      <c r="D54" s="197"/>
+      <c r="B54" s="225"/>
+      <c r="C54" s="225"/>
+      <c r="D54" s="225"/>
     </row>
     <row r="55" spans="1:7">
-      <c r="A55" s="193"/>
-      <c r="B55" s="193"/>
+      <c r="A55" s="226"/>
+      <c r="B55" s="226"/>
       <c r="C55" s="19" t="s">
         <v>206</v>
       </c>
@@ -5079,10 +5064,10 @@
   <sheetPr>
     <tabColor rgb="FF9DC3E6"/>
   </sheetPr>
-  <dimension ref="A1:AJ203"/>
+  <dimension ref="A1:AJ199"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O178" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="AD202" sqref="AD202"/>
+    <sheetView topLeftCell="A154" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E175" sqref="E175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -5106,16 +5091,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="223" t="s">
+      <c r="A1" s="198" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="223"/>
-      <c r="C1" s="223"/>
-      <c r="E1" s="223" t="s">
+      <c r="B1" s="198"/>
+      <c r="C1" s="198"/>
+      <c r="E1" s="198" t="s">
         <v>49</v>
       </c>
-      <c r="F1" s="223"/>
-      <c r="G1" s="223"/>
+      <c r="F1" s="198"/>
+      <c r="G1" s="198"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="27" t="s">
@@ -5187,10 +5172,10 @@
       <c r="C5" s="35">
         <v>85.177099999999996</v>
       </c>
-      <c r="E5" s="224" t="s">
+      <c r="E5" s="199" t="s">
         <v>62</v>
       </c>
-      <c r="F5" s="224"/>
+      <c r="F5" s="199"/>
       <c r="G5" s="36"/>
     </row>
     <row r="6" spans="1:11">
@@ -5291,10 +5276,10 @@
       <c r="C10" s="42">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="E10" s="224" t="s">
+      <c r="E10" s="199" t="s">
         <v>73</v>
       </c>
-      <c r="F10" s="224"/>
+      <c r="F10" s="199"/>
       <c r="G10" s="43"/>
     </row>
     <row r="11" spans="1:11">
@@ -5389,10 +5374,10 @@
       </c>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="225" t="s">
+      <c r="A16" s="200" t="s">
         <v>82</v>
       </c>
-      <c r="B16" s="225"/>
+      <c r="B16" s="200"/>
       <c r="C16" s="50"/>
     </row>
     <row r="17" spans="1:8">
@@ -5405,11 +5390,11 @@
       <c r="C17" s="41">
         <v>300</v>
       </c>
-      <c r="E17" s="218" t="s">
+      <c r="E17" s="201" t="s">
         <v>83</v>
       </c>
-      <c r="F17" s="218"/>
-      <c r="G17" s="218"/>
+      <c r="F17" s="201"/>
+      <c r="G17" s="201"/>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="27" t="s">
@@ -5585,12 +5570,12 @@
       </c>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="219" t="s">
+      <c r="A29" s="202" t="s">
         <v>104</v>
       </c>
-      <c r="B29" s="219"/>
-      <c r="C29" s="219"/>
-      <c r="D29" s="219"/>
+      <c r="B29" s="202"/>
+      <c r="C29" s="202"/>
+      <c r="D29" s="202"/>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="67" t="s">
@@ -5602,7 +5587,7 @@
       <c r="C30" s="68">
         <v>1726</v>
       </c>
-      <c r="D30" s="220" t="s">
+      <c r="D30" s="203" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5616,7 +5601,7 @@
       <c r="C31" s="70">
         <v>2213</v>
       </c>
-      <c r="D31" s="220"/>
+      <c r="D31" s="203"/>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="69" t="s">
@@ -5628,7 +5613,7 @@
       <c r="C32" s="70">
         <v>50</v>
       </c>
-      <c r="D32" s="220"/>
+      <c r="D32" s="203"/>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="71" t="s">
@@ -5640,7 +5625,7 @@
       <c r="C33" s="72">
         <v>0</v>
       </c>
-      <c r="D33" s="220"/>
+      <c r="D33" s="203"/>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="69" t="s">
@@ -5652,7 +5637,7 @@
       <c r="C34" s="70">
         <v>1</v>
       </c>
-      <c r="D34" s="220"/>
+      <c r="D34" s="203"/>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="69" t="s">
@@ -5664,7 +5649,7 @@
       <c r="C35" s="73">
         <v>8.5</v>
       </c>
-      <c r="D35" s="220"/>
+      <c r="D35" s="203"/>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="69" t="s">
@@ -5676,7 +5661,7 @@
       <c r="C36" s="73">
         <v>0.88</v>
       </c>
-      <c r="D36" s="220"/>
+      <c r="D36" s="203"/>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="69" t="s">
@@ -5688,7 +5673,7 @@
       <c r="C37" s="73">
         <v>0.08</v>
       </c>
-      <c r="D37" s="220"/>
+      <c r="D37" s="203"/>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="74" t="s">
@@ -5700,7 +5685,7 @@
       <c r="C38" s="76">
         <v>1</v>
       </c>
-      <c r="D38" s="220"/>
+      <c r="D38" s="203"/>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="67" t="s">
@@ -5712,7 +5697,7 @@
       <c r="C39" s="77">
         <v>11</v>
       </c>
-      <c r="D39" s="221" t="s">
+      <c r="D39" s="204" t="s">
         <v>5</v>
       </c>
     </row>
@@ -5726,7 +5711,7 @@
       <c r="C40" s="78">
         <v>312.3</v>
       </c>
-      <c r="D40" s="221"/>
+      <c r="D40" s="204"/>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="74" t="s">
@@ -5738,7 +5723,7 @@
       <c r="C41" s="76">
         <v>117</v>
       </c>
-      <c r="D41" s="221"/>
+      <c r="D41" s="204"/>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="67" t="s">
@@ -5750,7 +5735,7 @@
       <c r="C42" s="77">
         <v>76</v>
       </c>
-      <c r="D42" s="222" t="s">
+      <c r="D42" s="205" t="s">
         <v>125</v>
       </c>
     </row>
@@ -5764,7 +5749,7 @@
       <c r="C43" s="70">
         <v>50000</v>
       </c>
-      <c r="D43" s="222"/>
+      <c r="D43" s="205"/>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="69" t="s">
@@ -5776,7 +5761,7 @@
       <c r="C44" s="70">
         <v>40</v>
       </c>
-      <c r="D44" s="222"/>
+      <c r="D44" s="205"/>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="74" t="s">
@@ -5788,7 +5773,7 @@
       <c r="C45" s="79">
         <v>0.09</v>
       </c>
-      <c r="D45" s="222"/>
+      <c r="D45" s="205"/>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="67" t="s">
@@ -5800,7 +5785,7 @@
       <c r="C46" s="80">
         <v>3.47</v>
       </c>
-      <c r="D46" s="214" t="s">
+      <c r="D46" s="206" t="s">
         <v>7</v>
       </c>
     </row>
@@ -5814,7 +5799,7 @@
       <c r="C47" s="70">
         <v>3200</v>
       </c>
-      <c r="D47" s="214"/>
+      <c r="D47" s="206"/>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="69" t="s">
@@ -5826,7 +5811,7 @@
       <c r="C48" s="70">
         <v>0</v>
       </c>
-      <c r="D48" s="214"/>
+      <c r="D48" s="206"/>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="81" t="s">
@@ -5838,7 +5823,7 @@
       <c r="C49" s="83">
         <v>0.56999999999999995</v>
       </c>
-      <c r="D49" s="214"/>
+      <c r="D49" s="206"/>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="84" t="s">
@@ -6006,11 +5991,11 @@
       </c>
     </row>
     <row r="64" spans="1:4">
-      <c r="A64" s="215" t="s">
+      <c r="A64" s="207" t="s">
         <v>140</v>
       </c>
-      <c r="B64" s="215"/>
-      <c r="C64" s="215"/>
+      <c r="B64" s="207"/>
+      <c r="C64" s="207"/>
     </row>
     <row r="65" spans="1:36">
       <c r="A65" s="69" t="s">
@@ -6469,7 +6454,7 @@
       <c r="A85" s="51" t="s">
         <v>158</v>
       </c>
-      <c r="B85" s="216" t="s">
+      <c r="B85" s="208" t="s">
         <v>85</v>
       </c>
       <c r="C85" s="108">
@@ -6507,7 +6492,7 @@
       <c r="A86" s="51" t="s">
         <v>159</v>
       </c>
-      <c r="B86" s="216"/>
+      <c r="B86" s="208"/>
       <c r="C86" s="108">
         <v>-0.71328999999999998</v>
       </c>
@@ -6543,7 +6528,7 @@
       <c r="A87" s="51" t="s">
         <v>160</v>
       </c>
-      <c r="B87" s="216"/>
+      <c r="B87" s="208"/>
       <c r="C87" s="108">
         <v>-0.75124999999999997</v>
       </c>
@@ -6579,7 +6564,7 @@
       <c r="A88" s="51" t="s">
         <v>161</v>
       </c>
-      <c r="B88" s="216"/>
+      <c r="B88" s="208"/>
       <c r="C88" s="108">
         <v>-0.69615000000000005</v>
       </c>
@@ -6680,7 +6665,7 @@
       </c>
     </row>
     <row r="95" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A95" s="217" t="s">
+      <c r="A95" s="209" t="s">
         <v>165</v>
       </c>
       <c r="B95" s="210" t="s">
@@ -6730,7 +6715,7 @@
       </c>
     </row>
     <row r="96" spans="1:16">
-      <c r="A96" s="217"/>
+      <c r="A96" s="209"/>
       <c r="B96" s="210"/>
       <c r="C96" s="19" t="s">
         <v>167</v>
@@ -6776,7 +6761,7 @@
       </c>
     </row>
     <row r="97" spans="1:16">
-      <c r="A97" s="217"/>
+      <c r="A97" s="209"/>
       <c r="B97" s="210"/>
       <c r="C97" s="19" t="s">
         <v>168</v>
@@ -6822,7 +6807,7 @@
       </c>
     </row>
     <row r="98" spans="1:16">
-      <c r="A98" s="217"/>
+      <c r="A98" s="209"/>
       <c r="B98" s="210"/>
       <c r="C98" s="123" t="s">
         <v>169</v>
@@ -6868,7 +6853,7 @@
       </c>
     </row>
     <row r="99" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A99" s="209" t="s">
+      <c r="A99" s="211" t="s">
         <v>170</v>
       </c>
       <c r="B99" s="210" t="s">
@@ -6921,7 +6906,7 @@
       </c>
     </row>
     <row r="100" spans="1:16">
-      <c r="A100" s="209"/>
+      <c r="A100" s="211"/>
       <c r="B100" s="210"/>
       <c r="C100" s="19" t="s">
         <v>167</v>
@@ -6970,7 +6955,7 @@
       </c>
     </row>
     <row r="101" spans="1:16">
-      <c r="A101" s="209"/>
+      <c r="A101" s="211"/>
       <c r="B101" s="210"/>
       <c r="C101" s="19" t="s">
         <v>168</v>
@@ -7019,7 +7004,7 @@
       </c>
     </row>
     <row r="102" spans="1:16">
-      <c r="A102" s="209"/>
+      <c r="A102" s="211"/>
       <c r="B102" s="210"/>
       <c r="C102" s="123" t="s">
         <v>169</v>
@@ -7068,10 +7053,10 @@
       </c>
     </row>
     <row r="103" spans="1:16">
-      <c r="A103" s="211" t="s">
+      <c r="A103" s="212" t="s">
         <v>172</v>
       </c>
-      <c r="B103" s="212" t="s">
+      <c r="B103" s="213" t="s">
         <v>173</v>
       </c>
       <c r="C103" s="115" t="s">
@@ -7118,8 +7103,8 @@
       </c>
     </row>
     <row r="104" spans="1:16">
-      <c r="A104" s="211"/>
-      <c r="B104" s="212"/>
+      <c r="A104" s="212"/>
+      <c r="B104" s="213"/>
       <c r="C104" s="19" t="s">
         <v>167</v>
       </c>
@@ -7164,8 +7149,8 @@
       </c>
     </row>
     <row r="105" spans="1:16">
-      <c r="A105" s="211"/>
-      <c r="B105" s="212"/>
+      <c r="A105" s="212"/>
+      <c r="B105" s="213"/>
       <c r="C105" s="19" t="s">
         <v>168</v>
       </c>
@@ -7210,8 +7195,8 @@
       </c>
     </row>
     <row r="106" spans="1:16">
-      <c r="A106" s="211"/>
-      <c r="B106" s="212"/>
+      <c r="A106" s="212"/>
+      <c r="B106" s="213"/>
       <c r="C106" s="144" t="s">
         <v>169</v>
       </c>
@@ -7256,10 +7241,10 @@
       </c>
     </row>
     <row r="107" spans="1:16">
-      <c r="A107" s="209" t="s">
+      <c r="A107" s="211" t="s">
         <v>174</v>
       </c>
-      <c r="B107" s="213" t="s">
+      <c r="B107" s="214" t="s">
         <v>173</v>
       </c>
       <c r="C107" s="115" t="s">
@@ -7306,8 +7291,8 @@
       </c>
     </row>
     <row r="108" spans="1:16">
-      <c r="A108" s="209"/>
-      <c r="B108" s="213"/>
+      <c r="A108" s="211"/>
+      <c r="B108" s="214"/>
       <c r="C108" s="149" t="s">
         <v>167</v>
       </c>
@@ -7352,8 +7337,8 @@
       </c>
     </row>
     <row r="109" spans="1:16">
-      <c r="A109" s="209"/>
-      <c r="B109" s="213"/>
+      <c r="A109" s="211"/>
+      <c r="B109" s="214"/>
       <c r="C109" s="149" t="s">
         <v>168</v>
       </c>
@@ -7398,8 +7383,8 @@
       </c>
     </row>
     <row r="110" spans="1:16">
-      <c r="A110" s="209"/>
-      <c r="B110" s="213"/>
+      <c r="A110" s="211"/>
+      <c r="B110" s="214"/>
       <c r="C110" s="150" t="s">
         <v>169</v>
       </c>
@@ -7464,10 +7449,10 @@
       <c r="P111" s="155"/>
     </row>
     <row r="112" spans="1:16">
-      <c r="A112" s="200" t="s">
+      <c r="A112" s="215" t="s">
         <v>8</v>
       </c>
-      <c r="B112" s="201" t="s">
+      <c r="B112" s="216" t="s">
         <v>173</v>
       </c>
       <c r="C112" s="19" t="s">
@@ -7514,8 +7499,8 @@
       </c>
     </row>
     <row r="113" spans="1:16">
-      <c r="A113" s="200"/>
-      <c r="B113" s="201"/>
+      <c r="A113" s="215"/>
+      <c r="B113" s="216"/>
       <c r="C113" s="19" t="s">
         <v>167</v>
       </c>
@@ -7560,8 +7545,8 @@
       </c>
     </row>
     <row r="114" spans="1:16">
-      <c r="A114" s="200"/>
-      <c r="B114" s="201"/>
+      <c r="A114" s="215"/>
+      <c r="B114" s="216"/>
       <c r="C114" s="19" t="s">
         <v>168</v>
       </c>
@@ -7606,8 +7591,8 @@
       </c>
     </row>
     <row r="115" spans="1:16">
-      <c r="A115" s="200"/>
-      <c r="B115" s="201"/>
+      <c r="A115" s="215"/>
+      <c r="B115" s="216"/>
       <c r="C115" s="19" t="s">
         <v>169</v>
       </c>
@@ -7652,10 +7637,10 @@
       </c>
     </row>
     <row r="116" spans="1:16">
-      <c r="A116" s="200" t="s">
+      <c r="A116" s="215" t="s">
         <v>9</v>
       </c>
-      <c r="B116" s="201" t="s">
+      <c r="B116" s="216" t="s">
         <v>173</v>
       </c>
       <c r="C116" s="157" t="s">
@@ -7702,8 +7687,8 @@
       </c>
     </row>
     <row r="117" spans="1:16">
-      <c r="A117" s="200"/>
-      <c r="B117" s="201"/>
+      <c r="A117" s="215"/>
+      <c r="B117" s="216"/>
       <c r="C117" s="19" t="s">
         <v>167</v>
       </c>
@@ -7748,8 +7733,8 @@
       </c>
     </row>
     <row r="118" spans="1:16">
-      <c r="A118" s="200"/>
-      <c r="B118" s="201"/>
+      <c r="A118" s="215"/>
+      <c r="B118" s="216"/>
       <c r="C118" s="19" t="s">
         <v>168</v>
       </c>
@@ -7794,8 +7779,8 @@
       </c>
     </row>
     <row r="119" spans="1:16">
-      <c r="A119" s="200"/>
-      <c r="B119" s="201"/>
+      <c r="A119" s="215"/>
+      <c r="B119" s="216"/>
       <c r="C119" s="19" t="s">
         <v>169</v>
       </c>
@@ -7840,10 +7825,10 @@
       </c>
     </row>
     <row r="120" spans="1:16">
-      <c r="A120" s="200" t="s">
+      <c r="A120" s="215" t="s">
         <v>10</v>
       </c>
-      <c r="B120" s="201" t="s">
+      <c r="B120" s="216" t="s">
         <v>173</v>
       </c>
       <c r="C120" s="19" t="s">
@@ -7890,8 +7875,8 @@
       </c>
     </row>
     <row r="121" spans="1:16">
-      <c r="A121" s="200"/>
-      <c r="B121" s="201"/>
+      <c r="A121" s="215"/>
+      <c r="B121" s="216"/>
       <c r="C121" s="19" t="s">
         <v>167</v>
       </c>
@@ -7936,8 +7921,8 @@
       </c>
     </row>
     <row r="122" spans="1:16">
-      <c r="A122" s="200"/>
-      <c r="B122" s="201"/>
+      <c r="A122" s="215"/>
+      <c r="B122" s="216"/>
       <c r="C122" s="19" t="s">
         <v>168</v>
       </c>
@@ -7982,8 +7967,8 @@
       </c>
     </row>
     <row r="123" spans="1:16">
-      <c r="A123" s="200"/>
-      <c r="B123" s="201"/>
+      <c r="A123" s="215"/>
+      <c r="B123" s="216"/>
       <c r="C123" s="19" t="s">
         <v>169</v>
       </c>
@@ -8028,10 +8013,10 @@
       </c>
     </row>
     <row r="124" spans="1:16">
-      <c r="A124" s="200" t="s">
+      <c r="A124" s="215" t="s">
         <v>11</v>
       </c>
-      <c r="B124" s="201" t="s">
+      <c r="B124" s="216" t="s">
         <v>173</v>
       </c>
       <c r="C124" s="19" t="s">
@@ -8078,8 +8063,8 @@
       </c>
     </row>
     <row r="125" spans="1:16">
-      <c r="A125" s="200"/>
-      <c r="B125" s="201"/>
+      <c r="A125" s="215"/>
+      <c r="B125" s="216"/>
       <c r="C125" s="19" t="s">
         <v>167</v>
       </c>
@@ -8124,8 +8109,8 @@
       </c>
     </row>
     <row r="126" spans="1:16">
-      <c r="A126" s="200"/>
-      <c r="B126" s="201"/>
+      <c r="A126" s="215"/>
+      <c r="B126" s="216"/>
       <c r="C126" s="19" t="s">
         <v>168</v>
       </c>
@@ -8170,8 +8155,8 @@
       </c>
     </row>
     <row r="127" spans="1:16">
-      <c r="A127" s="200"/>
-      <c r="B127" s="201"/>
+      <c r="A127" s="215"/>
+      <c r="B127" s="216"/>
       <c r="C127" s="19" t="s">
         <v>169</v>
       </c>
@@ -8216,10 +8201,10 @@
       </c>
     </row>
     <row r="128" spans="1:16">
-      <c r="A128" s="200" t="s">
+      <c r="A128" s="215" t="s">
         <v>12</v>
       </c>
-      <c r="B128" s="201" t="s">
+      <c r="B128" s="216" t="s">
         <v>173</v>
       </c>
       <c r="C128" s="19" t="s">
@@ -8266,8 +8251,8 @@
       </c>
     </row>
     <row r="129" spans="1:16">
-      <c r="A129" s="200"/>
-      <c r="B129" s="201"/>
+      <c r="A129" s="215"/>
+      <c r="B129" s="216"/>
       <c r="C129" s="19" t="s">
         <v>167</v>
       </c>
@@ -8312,8 +8297,8 @@
       </c>
     </row>
     <row r="130" spans="1:16">
-      <c r="A130" s="200"/>
-      <c r="B130" s="201"/>
+      <c r="A130" s="215"/>
+      <c r="B130" s="216"/>
       <c r="C130" s="19" t="s">
         <v>168</v>
       </c>
@@ -8358,8 +8343,8 @@
       </c>
     </row>
     <row r="131" spans="1:16">
-      <c r="A131" s="200"/>
-      <c r="B131" s="201"/>
+      <c r="A131" s="215"/>
+      <c r="B131" s="216"/>
       <c r="C131" s="19" t="s">
         <v>169</v>
       </c>
@@ -8404,10 +8389,10 @@
       </c>
     </row>
     <row r="132" spans="1:16">
-      <c r="A132" s="200" t="s">
+      <c r="A132" s="215" t="s">
         <v>13</v>
       </c>
-      <c r="B132" s="201" t="s">
+      <c r="B132" s="216" t="s">
         <v>173</v>
       </c>
       <c r="C132" s="19" t="s">
@@ -8454,8 +8439,8 @@
       </c>
     </row>
     <row r="133" spans="1:16">
-      <c r="A133" s="200"/>
-      <c r="B133" s="201"/>
+      <c r="A133" s="215"/>
+      <c r="B133" s="216"/>
       <c r="C133" s="19" t="s">
         <v>167</v>
       </c>
@@ -8500,8 +8485,8 @@
       </c>
     </row>
     <row r="134" spans="1:16">
-      <c r="A134" s="200"/>
-      <c r="B134" s="201"/>
+      <c r="A134" s="215"/>
+      <c r="B134" s="216"/>
       <c r="C134" s="19" t="s">
         <v>168</v>
       </c>
@@ -8546,8 +8531,8 @@
       </c>
     </row>
     <row r="135" spans="1:16">
-      <c r="A135" s="200"/>
-      <c r="B135" s="201"/>
+      <c r="A135" s="215"/>
+      <c r="B135" s="216"/>
       <c r="C135" s="19" t="s">
         <v>169</v>
       </c>
@@ -8592,10 +8577,10 @@
       </c>
     </row>
     <row r="136" spans="1:16">
-      <c r="A136" s="200" t="s">
+      <c r="A136" s="215" t="s">
         <v>14</v>
       </c>
-      <c r="B136" s="201" t="s">
+      <c r="B136" s="216" t="s">
         <v>173</v>
       </c>
       <c r="C136" s="19" t="s">
@@ -8642,8 +8627,8 @@
       </c>
     </row>
     <row r="137" spans="1:16">
-      <c r="A137" s="200"/>
-      <c r="B137" s="201"/>
+      <c r="A137" s="215"/>
+      <c r="B137" s="216"/>
       <c r="C137" s="19" t="s">
         <v>167</v>
       </c>
@@ -8688,8 +8673,8 @@
       </c>
     </row>
     <row r="138" spans="1:16">
-      <c r="A138" s="200"/>
-      <c r="B138" s="201"/>
+      <c r="A138" s="215"/>
+      <c r="B138" s="216"/>
       <c r="C138" s="19" t="s">
         <v>168</v>
       </c>
@@ -8734,8 +8719,8 @@
       </c>
     </row>
     <row r="139" spans="1:16">
-      <c r="A139" s="200"/>
-      <c r="B139" s="201"/>
+      <c r="A139" s="215"/>
+      <c r="B139" s="216"/>
       <c r="C139" s="19" t="s">
         <v>169</v>
       </c>
@@ -8780,10 +8765,10 @@
       </c>
     </row>
     <row r="140" spans="1:16">
-      <c r="A140" s="202" t="s">
+      <c r="A140" s="219" t="s">
         <v>15</v>
       </c>
-      <c r="B140" s="201" t="s">
+      <c r="B140" s="216" t="s">
         <v>173</v>
       </c>
       <c r="C140" s="19" t="s">
@@ -8830,8 +8815,8 @@
       </c>
     </row>
     <row r="141" spans="1:16">
-      <c r="A141" s="202"/>
-      <c r="B141" s="201"/>
+      <c r="A141" s="219"/>
+      <c r="B141" s="216"/>
       <c r="C141" s="19" t="s">
         <v>167</v>
       </c>
@@ -8876,8 +8861,8 @@
       </c>
     </row>
     <row r="142" spans="1:16">
-      <c r="A142" s="202"/>
-      <c r="B142" s="201"/>
+      <c r="A142" s="219"/>
+      <c r="B142" s="216"/>
       <c r="C142" s="19" t="s">
         <v>168</v>
       </c>
@@ -8922,8 +8907,8 @@
       </c>
     </row>
     <row r="143" spans="1:16">
-      <c r="A143" s="202"/>
-      <c r="B143" s="201"/>
+      <c r="A143" s="219"/>
+      <c r="B143" s="216"/>
       <c r="C143" s="19" t="s">
         <v>169</v>
       </c>
@@ -8968,10 +8953,10 @@
       </c>
     </row>
     <row r="144" spans="1:16">
-      <c r="A144" s="203" t="s">
+      <c r="A144" s="220" t="s">
         <v>16</v>
       </c>
-      <c r="B144" s="204" t="s">
+      <c r="B144" s="221" t="s">
         <v>173</v>
       </c>
       <c r="C144" s="19" t="s">
@@ -9018,8 +9003,8 @@
       </c>
     </row>
     <row r="145" spans="1:16">
-      <c r="A145" s="203"/>
-      <c r="B145" s="204"/>
+      <c r="A145" s="220"/>
+      <c r="B145" s="221"/>
       <c r="C145" s="19" t="s">
         <v>167</v>
       </c>
@@ -9064,8 +9049,8 @@
       </c>
     </row>
     <row r="146" spans="1:16">
-      <c r="A146" s="203"/>
-      <c r="B146" s="204"/>
+      <c r="A146" s="220"/>
+      <c r="B146" s="221"/>
       <c r="C146" s="19" t="s">
         <v>168</v>
       </c>
@@ -9110,8 +9095,8 @@
       </c>
     </row>
     <row r="147" spans="1:16">
-      <c r="A147" s="203"/>
-      <c r="B147" s="204"/>
+      <c r="A147" s="220"/>
+      <c r="B147" s="221"/>
       <c r="C147" s="123" t="s">
         <v>169</v>
       </c>
@@ -9156,7 +9141,7 @@
       </c>
     </row>
     <row r="149" spans="1:16">
-      <c r="C149" s="192"/>
+      <c r="C149" s="224"/>
     </row>
     <row r="151" spans="1:16">
       <c r="A151" s="188" t="s">
@@ -9203,7 +9188,7 @@
       </c>
     </row>
     <row r="152" spans="1:16">
-      <c r="A152" s="198" t="s">
+      <c r="A152" s="217" t="s">
         <v>196</v>
       </c>
       <c r="B152" s="17" t="s">
@@ -9247,7 +9232,7 @@
       </c>
     </row>
     <row r="153" spans="1:16">
-      <c r="A153" s="199"/>
+      <c r="A153" s="218"/>
       <c r="B153" s="17" t="s">
         <v>194</v>
       </c>
@@ -9289,7 +9274,7 @@
       </c>
     </row>
     <row r="154" spans="1:16">
-      <c r="A154" s="205"/>
+      <c r="A154" s="222"/>
       <c r="B154" s="17" t="s">
         <v>195</v>
       </c>
@@ -9331,7 +9316,7 @@
       </c>
     </row>
     <row r="155" spans="1:16">
-      <c r="A155" s="206" t="s">
+      <c r="A155" s="195" t="s">
         <v>197</v>
       </c>
       <c r="B155" s="17" t="s">
@@ -9375,7 +9360,7 @@
       </c>
     </row>
     <row r="156" spans="1:16">
-      <c r="A156" s="207"/>
+      <c r="A156" s="196"/>
       <c r="B156" s="17" t="s">
         <v>194</v>
       </c>
@@ -9417,7 +9402,7 @@
       </c>
     </row>
     <row r="157" spans="1:16">
-      <c r="A157" s="208"/>
+      <c r="A157" s="197"/>
       <c r="B157" s="17" t="s">
         <v>195</v>
       </c>
@@ -9459,7 +9444,7 @@
       </c>
     </row>
     <row r="158" spans="1:16">
-      <c r="A158" s="206" t="s">
+      <c r="A158" s="195" t="s">
         <v>186</v>
       </c>
       <c r="B158" s="17" t="s">
@@ -9515,7 +9500,7 @@
       </c>
     </row>
     <row r="159" spans="1:16">
-      <c r="A159" s="207"/>
+      <c r="A159" s="196"/>
       <c r="B159" s="17" t="s">
         <v>194</v>
       </c>
@@ -9557,7 +9542,7 @@
       </c>
     </row>
     <row r="160" spans="1:16">
-      <c r="A160" s="208"/>
+      <c r="A160" s="197"/>
       <c r="B160" s="17" t="s">
         <v>195</v>
       </c>
@@ -9599,7 +9584,7 @@
       </c>
     </row>
     <row r="161" spans="1:14">
-      <c r="A161" s="206" t="s">
+      <c r="A161" s="195" t="s">
         <v>187</v>
       </c>
       <c r="B161" s="17" t="s">
@@ -9643,7 +9628,7 @@
       </c>
     </row>
     <row r="162" spans="1:14">
-      <c r="A162" s="207"/>
+      <c r="A162" s="196"/>
       <c r="B162" s="17" t="s">
         <v>194</v>
       </c>
@@ -9685,7 +9670,7 @@
       </c>
     </row>
     <row r="163" spans="1:14">
-      <c r="A163" s="208"/>
+      <c r="A163" s="197"/>
       <c r="B163" s="17" t="s">
         <v>195</v>
       </c>
@@ -9727,7 +9712,7 @@
       </c>
     </row>
     <row r="164" spans="1:14">
-      <c r="A164" s="206" t="s">
+      <c r="A164" s="195" t="s">
         <v>188</v>
       </c>
       <c r="B164" s="17" t="s">
@@ -9771,7 +9756,7 @@
       </c>
     </row>
     <row r="165" spans="1:14">
-      <c r="A165" s="207"/>
+      <c r="A165" s="196"/>
       <c r="B165" s="17" t="s">
         <v>194</v>
       </c>
@@ -9813,7 +9798,7 @@
       </c>
     </row>
     <row r="166" spans="1:14">
-      <c r="A166" s="208"/>
+      <c r="A166" s="197"/>
       <c r="B166" s="17" t="s">
         <v>195</v>
       </c>
@@ -9855,7 +9840,7 @@
       </c>
     </row>
     <row r="167" spans="1:14">
-      <c r="A167" s="206" t="s">
+      <c r="A167" s="195" t="s">
         <v>189</v>
       </c>
       <c r="B167" s="17" t="s">
@@ -9899,7 +9884,7 @@
       </c>
     </row>
     <row r="168" spans="1:14">
-      <c r="A168" s="207"/>
+      <c r="A168" s="196"/>
       <c r="B168" s="17" t="s">
         <v>194</v>
       </c>
@@ -9941,7 +9926,7 @@
       </c>
     </row>
     <row r="169" spans="1:14">
-      <c r="A169" s="208"/>
+      <c r="A169" s="197"/>
       <c r="B169" s="17" t="s">
         <v>195</v>
       </c>
@@ -9983,7 +9968,7 @@
       </c>
     </row>
     <row r="170" spans="1:14">
-      <c r="A170" s="206" t="s">
+      <c r="A170" s="195" t="s">
         <v>190</v>
       </c>
       <c r="B170" s="17" t="s">
@@ -10027,7 +10012,7 @@
       </c>
     </row>
     <row r="171" spans="1:14">
-      <c r="A171" s="207"/>
+      <c r="A171" s="196"/>
       <c r="B171" s="17" t="s">
         <v>194</v>
       </c>
@@ -10069,7 +10054,7 @@
       </c>
     </row>
     <row r="172" spans="1:14">
-      <c r="A172" s="208"/>
+      <c r="A172" s="197"/>
       <c r="B172" s="17" t="s">
         <v>195</v>
       </c>
@@ -10111,7 +10096,7 @@
       </c>
     </row>
     <row r="173" spans="1:14">
-      <c r="A173" s="206" t="s">
+      <c r="A173" s="195" t="s">
         <v>191</v>
       </c>
       <c r="B173" s="17" t="s">
@@ -10155,7 +10140,7 @@
       </c>
     </row>
     <row r="174" spans="1:14">
-      <c r="A174" s="207"/>
+      <c r="A174" s="196"/>
       <c r="B174" s="17" t="s">
         <v>194</v>
       </c>
@@ -10197,7 +10182,7 @@
       </c>
     </row>
     <row r="175" spans="1:14">
-      <c r="A175" s="208"/>
+      <c r="A175" s="197"/>
       <c r="B175" s="17" t="s">
         <v>195</v>
       </c>
@@ -10239,7 +10224,7 @@
       </c>
     </row>
     <row r="176" spans="1:14">
-      <c r="A176" s="206" t="s">
+      <c r="A176" s="195" t="s">
         <v>198</v>
       </c>
       <c r="B176" s="17" t="s">
@@ -10283,7 +10268,7 @@
       </c>
     </row>
     <row r="177" spans="1:14">
-      <c r="A177" s="207"/>
+      <c r="A177" s="196"/>
       <c r="B177" s="17" t="s">
         <v>194</v>
       </c>
@@ -10325,7 +10310,7 @@
       </c>
     </row>
     <row r="178" spans="1:14">
-      <c r="A178" s="208"/>
+      <c r="A178" s="197"/>
       <c r="B178" s="17" t="s">
         <v>195</v>
       </c>
@@ -10367,7 +10352,7 @@
       </c>
     </row>
     <row r="179" spans="1:14">
-      <c r="A179" s="206" t="s">
+      <c r="A179" s="195" t="s">
         <v>199</v>
       </c>
       <c r="B179" s="17" t="s">
@@ -10411,7 +10396,7 @@
       </c>
     </row>
     <row r="180" spans="1:14">
-      <c r="A180" s="207"/>
+      <c r="A180" s="196"/>
       <c r="B180" s="17" t="s">
         <v>194</v>
       </c>
@@ -10453,7 +10438,7 @@
       </c>
     </row>
     <row r="181" spans="1:14">
-      <c r="A181" s="208"/>
+      <c r="A181" s="197"/>
       <c r="B181" s="17" t="s">
         <v>195</v>
       </c>
@@ -10495,7 +10480,7 @@
       </c>
     </row>
     <row r="182" spans="1:14">
-      <c r="A182" s="206" t="s">
+      <c r="A182" s="195" t="s">
         <v>200</v>
       </c>
       <c r="B182" s="17" t="s">
@@ -10539,7 +10524,7 @@
       </c>
     </row>
     <row r="183" spans="1:14">
-      <c r="A183" s="207"/>
+      <c r="A183" s="196"/>
       <c r="B183" s="17" t="s">
         <v>194</v>
       </c>
@@ -10581,7 +10566,7 @@
       </c>
     </row>
     <row r="184" spans="1:14">
-      <c r="A184" s="208"/>
+      <c r="A184" s="197"/>
       <c r="B184" s="17" t="s">
         <v>195</v>
       </c>
@@ -10623,7 +10608,7 @@
       </c>
     </row>
     <row r="185" spans="1:14">
-      <c r="A185" s="206" t="s">
+      <c r="A185" s="195" t="s">
         <v>201</v>
       </c>
       <c r="B185" s="17" t="s">
@@ -10667,7 +10652,7 @@
       </c>
     </row>
     <row r="186" spans="1:14">
-      <c r="A186" s="207"/>
+      <c r="A186" s="196"/>
       <c r="B186" s="17" t="s">
         <v>194</v>
       </c>
@@ -10709,7 +10694,7 @@
       </c>
     </row>
     <row r="187" spans="1:14">
-      <c r="A187" s="208"/>
+      <c r="A187" s="197"/>
       <c r="B187" s="17" t="s">
         <v>195</v>
       </c>
@@ -10751,7 +10736,7 @@
       </c>
     </row>
     <row r="188" spans="1:14">
-      <c r="A188" s="206" t="s">
+      <c r="A188" s="195" t="s">
         <v>202</v>
       </c>
       <c r="B188" s="17" t="s">
@@ -10795,7 +10780,7 @@
       </c>
     </row>
     <row r="189" spans="1:14">
-      <c r="A189" s="207"/>
+      <c r="A189" s="196"/>
       <c r="B189" s="17" t="s">
         <v>194</v>
       </c>
@@ -10837,7 +10822,7 @@
       </c>
     </row>
     <row r="190" spans="1:14">
-      <c r="A190" s="208"/>
+      <c r="A190" s="197"/>
       <c r="B190" s="17" t="s">
         <v>195</v>
       </c>
@@ -10879,7 +10864,7 @@
       </c>
     </row>
     <row r="191" spans="1:14">
-      <c r="A191" s="206" t="s">
+      <c r="A191" s="195" t="s">
         <v>203</v>
       </c>
       <c r="B191" s="17" t="s">
@@ -10923,7 +10908,7 @@
       </c>
     </row>
     <row r="192" spans="1:14">
-      <c r="A192" s="207"/>
+      <c r="A192" s="196"/>
       <c r="B192" s="17" t="s">
         <v>194</v>
       </c>
@@ -10964,8 +10949,8 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="193" spans="1:30">
-      <c r="A193" s="208"/>
+    <row r="193" spans="1:14">
+      <c r="A193" s="197"/>
       <c r="B193" s="17" t="s">
         <v>195</v>
       </c>
@@ -11006,8 +10991,8 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="194" spans="1:30">
-      <c r="A194" s="206" t="s">
+    <row r="194" spans="1:14">
+      <c r="A194" s="195" t="s">
         <v>204</v>
       </c>
       <c r="B194" s="17" t="s">
@@ -11050,8 +11035,8 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="195" spans="1:30">
-      <c r="A195" s="207"/>
+    <row r="195" spans="1:14">
+      <c r="A195" s="196"/>
       <c r="B195" s="17" t="s">
         <v>194</v>
       </c>
@@ -11092,8 +11077,8 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="196" spans="1:30">
-      <c r="A196" s="208"/>
+    <row r="196" spans="1:14">
+      <c r="A196" s="197"/>
       <c r="B196" s="17" t="s">
         <v>195</v>
       </c>
@@ -11134,7 +11119,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="197" spans="1:30">
+    <row r="197" spans="1:14">
       <c r="A197" s="188" t="s">
         <v>211</v>
       </c>
@@ -11178,8 +11163,8 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="198" spans="1:30">
-      <c r="A198" s="198" t="s">
+    <row r="198" spans="1:14">
+      <c r="A198" s="217" t="s">
         <v>212</v>
       </c>
       <c r="B198" s="17" t="s">
@@ -11222,8 +11207,8 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="199" spans="1:30">
-      <c r="A199" s="199"/>
+    <row r="199" spans="1:14">
+      <c r="A199" s="218"/>
       <c r="B199" s="17" t="s">
         <v>214</v>
       </c>
@@ -11264,266 +11249,8 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="201" spans="1:30">
-      <c r="A201" s="197" t="s">
-        <v>215</v>
-      </c>
-      <c r="B201" s="197"/>
-      <c r="C201" s="197"/>
-      <c r="D201" s="197"/>
-      <c r="E201" s="197"/>
-      <c r="F201" s="197"/>
-      <c r="G201" s="197"/>
-      <c r="H201" s="197"/>
-      <c r="I201" s="197"/>
-      <c r="J201" s="197"/>
-      <c r="K201" s="197"/>
-      <c r="L201" s="197"/>
-      <c r="M201" s="197"/>
-      <c r="N201" s="197"/>
-      <c r="O201" s="197"/>
-      <c r="P201" s="197"/>
-      <c r="Q201" s="197"/>
-      <c r="R201" s="197"/>
-      <c r="S201" s="197"/>
-      <c r="T201" s="197"/>
-      <c r="U201" s="197"/>
-      <c r="V201" s="197"/>
-      <c r="W201" s="197"/>
-      <c r="X201" s="197"/>
-      <c r="Y201" s="197"/>
-      <c r="Z201" s="197"/>
-      <c r="AA201" s="197"/>
-      <c r="AB201" s="197"/>
-      <c r="AC201" s="197"/>
-      <c r="AD201" s="197"/>
-    </row>
-    <row r="202" spans="1:30">
-      <c r="A202" s="17" t="s">
-        <v>216</v>
-      </c>
-      <c r="B202" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="C202" s="19">
-        <v>1995</v>
-      </c>
-      <c r="D202" s="19">
-        <v>1996</v>
-      </c>
-      <c r="E202" s="19">
-        <v>1997</v>
-      </c>
-      <c r="F202" s="19">
-        <v>1998</v>
-      </c>
-      <c r="G202" s="19">
-        <v>1999</v>
-      </c>
-      <c r="H202" s="19">
-        <v>2000</v>
-      </c>
-      <c r="I202" s="19">
-        <v>2001</v>
-      </c>
-      <c r="J202" s="19">
-        <v>2002</v>
-      </c>
-      <c r="K202" s="19">
-        <v>2003</v>
-      </c>
-      <c r="L202" s="19">
-        <v>2004</v>
-      </c>
-      <c r="M202" s="19">
-        <v>2005</v>
-      </c>
-      <c r="N202" s="19">
-        <v>2006</v>
-      </c>
-      <c r="O202" s="19">
-        <v>2007</v>
-      </c>
-      <c r="P202" s="19">
-        <v>2008</v>
-      </c>
-      <c r="Q202" s="19">
-        <v>2009</v>
-      </c>
-      <c r="R202" s="19">
-        <v>2010</v>
-      </c>
-      <c r="S202" s="19">
-        <v>2011</v>
-      </c>
-      <c r="T202" s="19">
-        <v>2012</v>
-      </c>
-      <c r="U202" s="19">
-        <v>2013</v>
-      </c>
-      <c r="V202" s="19">
-        <v>2014</v>
-      </c>
-      <c r="W202" s="19">
-        <v>2015</v>
-      </c>
-      <c r="X202" s="19">
-        <v>2016</v>
-      </c>
-      <c r="Y202" s="19">
-        <v>2017</v>
-      </c>
-      <c r="Z202" s="19">
-        <v>2018</v>
-      </c>
-      <c r="AA202" s="19">
-        <v>2019</v>
-      </c>
-      <c r="AB202" s="19">
-        <v>2020</v>
-      </c>
-      <c r="AC202" s="19">
-        <v>2021</v>
-      </c>
-      <c r="AD202" s="19">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="203" spans="1:30">
-      <c r="A203" s="17" t="s">
-        <v>217</v>
-      </c>
-      <c r="B203" s="19" t="s">
-        <v>218</v>
-      </c>
-      <c r="C203" s="19">
-        <v>0.197862902023071</v>
-      </c>
-      <c r="D203" s="19">
-        <v>0.19705245774944699</v>
-      </c>
-      <c r="E203" s="19">
-        <v>0.195862164585204</v>
-      </c>
-      <c r="F203" s="19">
-        <v>0.201506494990219</v>
-      </c>
-      <c r="G203" s="19">
-        <v>0.20239331346144401</v>
-      </c>
-      <c r="H203" s="19">
-        <v>0.19184050965229399</v>
-      </c>
-      <c r="I203" s="19">
-        <v>0.19816391062786801</v>
-      </c>
-      <c r="J203" s="19">
-        <v>0.20784587230133</v>
-      </c>
-      <c r="K203" s="19">
-        <v>0.20742275052980599</v>
-      </c>
-      <c r="L203" s="19">
-        <v>0.199178611956073</v>
-      </c>
-      <c r="M203" s="19">
-        <v>0.191773175691209</v>
-      </c>
-      <c r="N203" s="19">
-        <v>0.18843581838972301</v>
-      </c>
-      <c r="O203" s="19">
-        <v>0.18492183987135299</v>
-      </c>
-      <c r="P203" s="19">
-        <v>0.17476484558917099</v>
-      </c>
-      <c r="Q203" s="19">
-        <v>0.18473705831690901</v>
-      </c>
-      <c r="R203" s="19">
-        <v>0.18654754004049501</v>
-      </c>
-      <c r="S203" s="19">
-        <v>0.189454834248799</v>
-      </c>
-      <c r="T203" s="19">
-        <v>0.18970988362343699</v>
-      </c>
-      <c r="U203" s="19">
-        <v>0.191084988644315</v>
-      </c>
-      <c r="V203" s="19">
-        <v>0.195502781940076</v>
-      </c>
-      <c r="W203" s="19">
-        <v>0.18767352366145501</v>
-      </c>
-      <c r="X203" s="19">
-        <v>0.18955666805548799</v>
-      </c>
-      <c r="Y203" s="19">
-        <v>0.18919126608338799</v>
-      </c>
-      <c r="Z203" s="19">
-        <v>0.19123080280548899</v>
-      </c>
-      <c r="AA203" s="19">
-        <v>0.20390796789551899</v>
-      </c>
-      <c r="AB203" s="19">
-        <v>0.192958485556329</v>
-      </c>
-      <c r="AC203" s="19">
-        <v>0.195589643486903</v>
-      </c>
-      <c r="AD203" s="19">
-        <v>0.185678435467685</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="56">
-    <mergeCell ref="A201:AD201"/>
-    <mergeCell ref="A194:A196"/>
-    <mergeCell ref="A179:A181"/>
-    <mergeCell ref="A182:A184"/>
-    <mergeCell ref="A185:A187"/>
-    <mergeCell ref="A188:A190"/>
-    <mergeCell ref="A191:A193"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="A29:D29"/>
-    <mergeCell ref="D30:D38"/>
-    <mergeCell ref="D39:D41"/>
-    <mergeCell ref="D42:D45"/>
-    <mergeCell ref="D46:D49"/>
-    <mergeCell ref="A64:C64"/>
-    <mergeCell ref="B85:B88"/>
-    <mergeCell ref="A95:A98"/>
-    <mergeCell ref="B95:B98"/>
-    <mergeCell ref="A99:A102"/>
-    <mergeCell ref="B99:B102"/>
-    <mergeCell ref="A103:A106"/>
-    <mergeCell ref="B103:B106"/>
-    <mergeCell ref="A107:A110"/>
-    <mergeCell ref="B107:B110"/>
-    <mergeCell ref="A112:A115"/>
-    <mergeCell ref="B112:B115"/>
-    <mergeCell ref="A116:A119"/>
-    <mergeCell ref="B116:B119"/>
-    <mergeCell ref="A120:A123"/>
-    <mergeCell ref="B120:B123"/>
-    <mergeCell ref="A124:A127"/>
-    <mergeCell ref="B124:B127"/>
-    <mergeCell ref="A128:A131"/>
-    <mergeCell ref="B128:B131"/>
-    <mergeCell ref="A132:A135"/>
-    <mergeCell ref="B132:B135"/>
+  <mergeCells count="55">
     <mergeCell ref="A198:A199"/>
     <mergeCell ref="A136:A139"/>
     <mergeCell ref="B136:B139"/>
@@ -11540,6 +11267,45 @@
     <mergeCell ref="A170:A172"/>
     <mergeCell ref="A173:A175"/>
     <mergeCell ref="A176:A178"/>
+    <mergeCell ref="A124:A127"/>
+    <mergeCell ref="B124:B127"/>
+    <mergeCell ref="A128:A131"/>
+    <mergeCell ref="B128:B131"/>
+    <mergeCell ref="A132:A135"/>
+    <mergeCell ref="B132:B135"/>
+    <mergeCell ref="A112:A115"/>
+    <mergeCell ref="B112:B115"/>
+    <mergeCell ref="A116:A119"/>
+    <mergeCell ref="B116:B119"/>
+    <mergeCell ref="A120:A123"/>
+    <mergeCell ref="B120:B123"/>
+    <mergeCell ref="A99:A102"/>
+    <mergeCell ref="B99:B102"/>
+    <mergeCell ref="A103:A106"/>
+    <mergeCell ref="B103:B106"/>
+    <mergeCell ref="A107:A110"/>
+    <mergeCell ref="B107:B110"/>
+    <mergeCell ref="D46:D49"/>
+    <mergeCell ref="A64:C64"/>
+    <mergeCell ref="B85:B88"/>
+    <mergeCell ref="A95:A98"/>
+    <mergeCell ref="B95:B98"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="A29:D29"/>
+    <mergeCell ref="D30:D38"/>
+    <mergeCell ref="D39:D41"/>
+    <mergeCell ref="D42:D45"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A194:A196"/>
+    <mergeCell ref="A179:A181"/>
+    <mergeCell ref="A182:A184"/>
+    <mergeCell ref="A185:A187"/>
+    <mergeCell ref="A188:A190"/>
+    <mergeCell ref="A191:A193"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -11616,7 +11382,7 @@
       </c>
     </row>
     <row r="2" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A2" s="217" t="s">
+      <c r="A2" s="209" t="s">
         <v>165</v>
       </c>
       <c r="B2" s="210" t="s">
@@ -11666,7 +11432,7 @@
       </c>
     </row>
     <row r="3" spans="1:16">
-      <c r="A3" s="217"/>
+      <c r="A3" s="209"/>
       <c r="B3" s="210"/>
       <c r="C3" s="19" t="s">
         <v>167</v>
@@ -11712,7 +11478,7 @@
       </c>
     </row>
     <row r="4" spans="1:16">
-      <c r="A4" s="217"/>
+      <c r="A4" s="209"/>
       <c r="B4" s="210"/>
       <c r="C4" s="19" t="s">
         <v>168</v>
@@ -11758,7 +11524,7 @@
       </c>
     </row>
     <row r="5" spans="1:16">
-      <c r="A5" s="217"/>
+      <c r="A5" s="209"/>
       <c r="B5" s="210"/>
       <c r="C5" s="123" t="s">
         <v>169</v>
@@ -11804,7 +11570,7 @@
       </c>
     </row>
     <row r="6" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A6" s="209" t="s">
+      <c r="A6" s="211" t="s">
         <v>170</v>
       </c>
       <c r="B6" s="210" t="s">
@@ -11854,7 +11620,7 @@
       </c>
     </row>
     <row r="7" spans="1:16">
-      <c r="A7" s="209"/>
+      <c r="A7" s="211"/>
       <c r="B7" s="210"/>
       <c r="C7" s="19" t="s">
         <v>167</v>
@@ -11900,7 +11666,7 @@
       </c>
     </row>
     <row r="8" spans="1:16">
-      <c r="A8" s="209"/>
+      <c r="A8" s="211"/>
       <c r="B8" s="210"/>
       <c r="C8" s="19" t="s">
         <v>168</v>
@@ -11946,7 +11712,7 @@
       </c>
     </row>
     <row r="9" spans="1:16">
-      <c r="A9" s="209"/>
+      <c r="A9" s="211"/>
       <c r="B9" s="210"/>
       <c r="C9" s="123" t="s">
         <v>169</v>
@@ -11992,10 +11758,10 @@
       </c>
     </row>
     <row r="10" spans="1:16">
-      <c r="A10" s="211" t="s">
+      <c r="A10" s="212" t="s">
         <v>172</v>
       </c>
-      <c r="B10" s="212" t="s">
+      <c r="B10" s="213" t="s">
         <v>173</v>
       </c>
       <c r="C10" s="115" t="s">
@@ -12042,8 +11808,8 @@
       </c>
     </row>
     <row r="11" spans="1:16">
-      <c r="A11" s="211"/>
-      <c r="B11" s="212"/>
+      <c r="A11" s="212"/>
+      <c r="B11" s="213"/>
       <c r="C11" s="19" t="s">
         <v>167</v>
       </c>
@@ -12088,8 +11854,8 @@
       </c>
     </row>
     <row r="12" spans="1:16">
-      <c r="A12" s="211"/>
-      <c r="B12" s="212"/>
+      <c r="A12" s="212"/>
+      <c r="B12" s="213"/>
       <c r="C12" s="19" t="s">
         <v>168</v>
       </c>
@@ -12134,8 +11900,8 @@
       </c>
     </row>
     <row r="13" spans="1:16">
-      <c r="A13" s="211"/>
-      <c r="B13" s="212"/>
+      <c r="A13" s="212"/>
+      <c r="B13" s="213"/>
       <c r="C13" s="144" t="s">
         <v>169</v>
       </c>
@@ -12180,10 +11946,10 @@
       </c>
     </row>
     <row r="14" spans="1:16">
-      <c r="A14" s="209" t="s">
+      <c r="A14" s="211" t="s">
         <v>174</v>
       </c>
-      <c r="B14" s="213" t="s">
+      <c r="B14" s="214" t="s">
         <v>173</v>
       </c>
       <c r="C14" s="115" t="s">
@@ -12230,8 +11996,8 @@
       </c>
     </row>
     <row r="15" spans="1:16">
-      <c r="A15" s="209"/>
-      <c r="B15" s="213"/>
+      <c r="A15" s="211"/>
+      <c r="B15" s="214"/>
       <c r="C15" s="149" t="s">
         <v>167</v>
       </c>
@@ -12276,8 +12042,8 @@
       </c>
     </row>
     <row r="16" spans="1:16">
-      <c r="A16" s="209"/>
-      <c r="B16" s="213"/>
+      <c r="A16" s="211"/>
+      <c r="B16" s="214"/>
       <c r="C16" s="149" t="s">
         <v>168</v>
       </c>
@@ -12322,8 +12088,8 @@
       </c>
     </row>
     <row r="17" spans="1:16">
-      <c r="A17" s="209"/>
-      <c r="B17" s="213"/>
+      <c r="A17" s="211"/>
+      <c r="B17" s="214"/>
       <c r="C17" s="150" t="s">
         <v>169</v>
       </c>
@@ -12388,10 +12154,10 @@
       <c r="P18" s="155"/>
     </row>
     <row r="19" spans="1:16">
-      <c r="A19" s="200" t="s">
+      <c r="A19" s="215" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="201" t="s">
+      <c r="B19" s="216" t="s">
         <v>173</v>
       </c>
       <c r="C19" s="19" t="s">
@@ -12438,8 +12204,8 @@
       </c>
     </row>
     <row r="20" spans="1:16">
-      <c r="A20" s="200"/>
-      <c r="B20" s="201"/>
+      <c r="A20" s="215"/>
+      <c r="B20" s="216"/>
       <c r="C20" s="19" t="s">
         <v>167</v>
       </c>
@@ -12484,8 +12250,8 @@
       </c>
     </row>
     <row r="21" spans="1:16">
-      <c r="A21" s="200"/>
-      <c r="B21" s="201"/>
+      <c r="A21" s="215"/>
+      <c r="B21" s="216"/>
       <c r="C21" s="19" t="s">
         <v>168</v>
       </c>
@@ -12530,8 +12296,8 @@
       </c>
     </row>
     <row r="22" spans="1:16">
-      <c r="A22" s="200"/>
-      <c r="B22" s="201"/>
+      <c r="A22" s="215"/>
+      <c r="B22" s="216"/>
       <c r="C22" s="19" t="s">
         <v>169</v>
       </c>
@@ -12576,10 +12342,10 @@
       </c>
     </row>
     <row r="23" spans="1:16">
-      <c r="A23" s="200" t="s">
+      <c r="A23" s="215" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="201" t="s">
+      <c r="B23" s="216" t="s">
         <v>173</v>
       </c>
       <c r="C23" s="157" t="s">
@@ -12626,8 +12392,8 @@
       </c>
     </row>
     <row r="24" spans="1:16">
-      <c r="A24" s="200"/>
-      <c r="B24" s="201"/>
+      <c r="A24" s="215"/>
+      <c r="B24" s="216"/>
       <c r="C24" s="19" t="s">
         <v>167</v>
       </c>
@@ -12672,8 +12438,8 @@
       </c>
     </row>
     <row r="25" spans="1:16">
-      <c r="A25" s="200"/>
-      <c r="B25" s="201"/>
+      <c r="A25" s="215"/>
+      <c r="B25" s="216"/>
       <c r="C25" s="19" t="s">
         <v>168</v>
       </c>
@@ -12718,8 +12484,8 @@
       </c>
     </row>
     <row r="26" spans="1:16">
-      <c r="A26" s="200"/>
-      <c r="B26" s="201"/>
+      <c r="A26" s="215"/>
+      <c r="B26" s="216"/>
       <c r="C26" s="19" t="s">
         <v>169</v>
       </c>
@@ -12764,10 +12530,10 @@
       </c>
     </row>
     <row r="27" spans="1:16">
-      <c r="A27" s="200" t="s">
+      <c r="A27" s="215" t="s">
         <v>10</v>
       </c>
-      <c r="B27" s="201" t="s">
+      <c r="B27" s="216" t="s">
         <v>173</v>
       </c>
       <c r="C27" s="19" t="s">
@@ -12814,8 +12580,8 @@
       </c>
     </row>
     <row r="28" spans="1:16">
-      <c r="A28" s="200"/>
-      <c r="B28" s="201"/>
+      <c r="A28" s="215"/>
+      <c r="B28" s="216"/>
       <c r="C28" s="19" t="s">
         <v>167</v>
       </c>
@@ -12860,8 +12626,8 @@
       </c>
     </row>
     <row r="29" spans="1:16">
-      <c r="A29" s="200"/>
-      <c r="B29" s="201"/>
+      <c r="A29" s="215"/>
+      <c r="B29" s="216"/>
       <c r="C29" s="19" t="s">
         <v>168</v>
       </c>
@@ -12906,8 +12672,8 @@
       </c>
     </row>
     <row r="30" spans="1:16">
-      <c r="A30" s="200"/>
-      <c r="B30" s="201"/>
+      <c r="A30" s="215"/>
+      <c r="B30" s="216"/>
       <c r="C30" s="19" t="s">
         <v>169</v>
       </c>
@@ -12952,10 +12718,10 @@
       </c>
     </row>
     <row r="31" spans="1:16">
-      <c r="A31" s="200" t="s">
+      <c r="A31" s="215" t="s">
         <v>11</v>
       </c>
-      <c r="B31" s="201" t="s">
+      <c r="B31" s="216" t="s">
         <v>173</v>
       </c>
       <c r="C31" s="19" t="s">
@@ -13002,8 +12768,8 @@
       </c>
     </row>
     <row r="32" spans="1:16">
-      <c r="A32" s="200"/>
-      <c r="B32" s="201"/>
+      <c r="A32" s="215"/>
+      <c r="B32" s="216"/>
       <c r="C32" s="19" t="s">
         <v>167</v>
       </c>
@@ -13048,8 +12814,8 @@
       </c>
     </row>
     <row r="33" spans="1:16">
-      <c r="A33" s="200"/>
-      <c r="B33" s="201"/>
+      <c r="A33" s="215"/>
+      <c r="B33" s="216"/>
       <c r="C33" s="19" t="s">
         <v>168</v>
       </c>
@@ -13094,8 +12860,8 @@
       </c>
     </row>
     <row r="34" spans="1:16">
-      <c r="A34" s="200"/>
-      <c r="B34" s="201"/>
+      <c r="A34" s="215"/>
+      <c r="B34" s="216"/>
       <c r="C34" s="19" t="s">
         <v>169</v>
       </c>
@@ -13140,10 +12906,10 @@
       </c>
     </row>
     <row r="35" spans="1:16">
-      <c r="A35" s="200" t="s">
+      <c r="A35" s="215" t="s">
         <v>12</v>
       </c>
-      <c r="B35" s="201" t="s">
+      <c r="B35" s="216" t="s">
         <v>173</v>
       </c>
       <c r="C35" s="19" t="s">
@@ -13190,8 +12956,8 @@
       </c>
     </row>
     <row r="36" spans="1:16">
-      <c r="A36" s="200"/>
-      <c r="B36" s="201"/>
+      <c r="A36" s="215"/>
+      <c r="B36" s="216"/>
       <c r="C36" s="19" t="s">
         <v>167</v>
       </c>
@@ -13236,8 +13002,8 @@
       </c>
     </row>
     <row r="37" spans="1:16">
-      <c r="A37" s="200"/>
-      <c r="B37" s="201"/>
+      <c r="A37" s="215"/>
+      <c r="B37" s="216"/>
       <c r="C37" s="19" t="s">
         <v>168</v>
       </c>
@@ -13282,8 +13048,8 @@
       </c>
     </row>
     <row r="38" spans="1:16">
-      <c r="A38" s="200"/>
-      <c r="B38" s="201"/>
+      <c r="A38" s="215"/>
+      <c r="B38" s="216"/>
       <c r="C38" s="19" t="s">
         <v>169</v>
       </c>
@@ -13328,10 +13094,10 @@
       </c>
     </row>
     <row r="39" spans="1:16">
-      <c r="A39" s="200" t="s">
+      <c r="A39" s="215" t="s">
         <v>13</v>
       </c>
-      <c r="B39" s="201" t="s">
+      <c r="B39" s="216" t="s">
         <v>173</v>
       </c>
       <c r="C39" s="19" t="s">
@@ -13378,8 +13144,8 @@
       </c>
     </row>
     <row r="40" spans="1:16">
-      <c r="A40" s="200"/>
-      <c r="B40" s="201"/>
+      <c r="A40" s="215"/>
+      <c r="B40" s="216"/>
       <c r="C40" s="19" t="s">
         <v>167</v>
       </c>
@@ -13424,8 +13190,8 @@
       </c>
     </row>
     <row r="41" spans="1:16">
-      <c r="A41" s="200"/>
-      <c r="B41" s="201"/>
+      <c r="A41" s="215"/>
+      <c r="B41" s="216"/>
       <c r="C41" s="19" t="s">
         <v>168</v>
       </c>
@@ -13470,8 +13236,8 @@
       </c>
     </row>
     <row r="42" spans="1:16">
-      <c r="A42" s="200"/>
-      <c r="B42" s="201"/>
+      <c r="A42" s="215"/>
+      <c r="B42" s="216"/>
       <c r="C42" s="19" t="s">
         <v>169</v>
       </c>
@@ -13516,10 +13282,10 @@
       </c>
     </row>
     <row r="43" spans="1:16">
-      <c r="A43" s="200" t="s">
+      <c r="A43" s="215" t="s">
         <v>14</v>
       </c>
-      <c r="B43" s="201" t="s">
+      <c r="B43" s="216" t="s">
         <v>173</v>
       </c>
       <c r="C43" s="19" t="s">
@@ -13566,8 +13332,8 @@
       </c>
     </row>
     <row r="44" spans="1:16">
-      <c r="A44" s="200"/>
-      <c r="B44" s="201"/>
+      <c r="A44" s="215"/>
+      <c r="B44" s="216"/>
       <c r="C44" s="19" t="s">
         <v>167</v>
       </c>
@@ -13612,8 +13378,8 @@
       </c>
     </row>
     <row r="45" spans="1:16">
-      <c r="A45" s="200"/>
-      <c r="B45" s="201"/>
+      <c r="A45" s="215"/>
+      <c r="B45" s="216"/>
       <c r="C45" s="19" t="s">
         <v>168</v>
       </c>
@@ -13658,8 +13424,8 @@
       </c>
     </row>
     <row r="46" spans="1:16">
-      <c r="A46" s="200"/>
-      <c r="B46" s="201"/>
+      <c r="A46" s="215"/>
+      <c r="B46" s="216"/>
       <c r="C46" s="19" t="s">
         <v>169</v>
       </c>
@@ -13704,10 +13470,10 @@
       </c>
     </row>
     <row r="47" spans="1:16">
-      <c r="A47" s="202" t="s">
+      <c r="A47" s="219" t="s">
         <v>15</v>
       </c>
-      <c r="B47" s="201" t="s">
+      <c r="B47" s="216" t="s">
         <v>173</v>
       </c>
       <c r="C47" s="19" t="s">
@@ -13754,8 +13520,8 @@
       </c>
     </row>
     <row r="48" spans="1:16">
-      <c r="A48" s="202"/>
-      <c r="B48" s="201"/>
+      <c r="A48" s="219"/>
+      <c r="B48" s="216"/>
       <c r="C48" s="19" t="s">
         <v>167</v>
       </c>
@@ -13800,8 +13566,8 @@
       </c>
     </row>
     <row r="49" spans="1:16">
-      <c r="A49" s="202"/>
-      <c r="B49" s="201"/>
+      <c r="A49" s="219"/>
+      <c r="B49" s="216"/>
       <c r="C49" s="19" t="s">
         <v>168</v>
       </c>
@@ -13846,8 +13612,8 @@
       </c>
     </row>
     <row r="50" spans="1:16">
-      <c r="A50" s="202"/>
-      <c r="B50" s="201"/>
+      <c r="A50" s="219"/>
+      <c r="B50" s="216"/>
       <c r="C50" s="19" t="s">
         <v>169</v>
       </c>
@@ -13892,10 +13658,10 @@
       </c>
     </row>
     <row r="51" spans="1:16">
-      <c r="A51" s="203" t="s">
+      <c r="A51" s="220" t="s">
         <v>16</v>
       </c>
-      <c r="B51" s="204" t="s">
+      <c r="B51" s="221" t="s">
         <v>173</v>
       </c>
       <c r="C51" s="19" t="s">
@@ -13942,8 +13708,8 @@
       </c>
     </row>
     <row r="52" spans="1:16">
-      <c r="A52" s="203"/>
-      <c r="B52" s="204"/>
+      <c r="A52" s="220"/>
+      <c r="B52" s="221"/>
       <c r="C52" s="19" t="s">
         <v>167</v>
       </c>
@@ -13988,8 +13754,8 @@
       </c>
     </row>
     <row r="53" spans="1:16">
-      <c r="A53" s="203"/>
-      <c r="B53" s="204"/>
+      <c r="A53" s="220"/>
+      <c r="B53" s="221"/>
       <c r="C53" s="19" t="s">
         <v>168</v>
       </c>
@@ -14034,8 +13800,8 @@
       </c>
     </row>
     <row r="54" spans="1:16">
-      <c r="A54" s="203"/>
-      <c r="B54" s="204"/>
+      <c r="A54" s="220"/>
+      <c r="B54" s="221"/>
       <c r="C54" s="123" t="s">
         <v>169</v>
       </c>
@@ -14124,7 +13890,7 @@
       </c>
     </row>
     <row r="59" spans="1:16">
-      <c r="A59" s="198" t="s">
+      <c r="A59" s="217" t="s">
         <v>196</v>
       </c>
       <c r="B59" s="17" t="s">
@@ -14168,7 +13934,7 @@
       </c>
     </row>
     <row r="60" spans="1:16">
-      <c r="A60" s="199"/>
+      <c r="A60" s="218"/>
       <c r="B60" s="17" t="s">
         <v>194</v>
       </c>
@@ -14210,7 +13976,7 @@
       </c>
     </row>
     <row r="61" spans="1:16">
-      <c r="A61" s="205"/>
+      <c r="A61" s="222"/>
       <c r="B61" s="17" t="s">
         <v>195</v>
       </c>
@@ -14252,7 +14018,7 @@
       </c>
     </row>
     <row r="62" spans="1:16">
-      <c r="A62" s="198" t="s">
+      <c r="A62" s="217" t="s">
         <v>197</v>
       </c>
       <c r="B62" s="17" t="s">
@@ -14296,7 +14062,7 @@
       </c>
     </row>
     <row r="63" spans="1:16">
-      <c r="A63" s="199"/>
+      <c r="A63" s="218"/>
       <c r="B63" s="17" t="s">
         <v>194</v>
       </c>
@@ -14338,7 +14104,7 @@
       </c>
     </row>
     <row r="64" spans="1:16">
-      <c r="A64" s="205"/>
+      <c r="A64" s="222"/>
       <c r="B64" s="17" t="s">
         <v>195</v>
       </c>
@@ -14380,7 +14146,7 @@
       </c>
     </row>
     <row r="65" spans="1:14">
-      <c r="A65" s="198" t="s">
+      <c r="A65" s="217" t="s">
         <v>186</v>
       </c>
       <c r="B65" s="17" t="s">
@@ -14436,7 +14202,7 @@
       </c>
     </row>
     <row r="66" spans="1:14">
-      <c r="A66" s="199"/>
+      <c r="A66" s="218"/>
       <c r="B66" s="17" t="s">
         <v>194</v>
       </c>
@@ -14478,7 +14244,7 @@
       </c>
     </row>
     <row r="67" spans="1:14">
-      <c r="A67" s="205"/>
+      <c r="A67" s="222"/>
       <c r="B67" s="17" t="s">
         <v>195</v>
       </c>
@@ -14520,7 +14286,7 @@
       </c>
     </row>
     <row r="68" spans="1:14">
-      <c r="A68" s="198" t="s">
+      <c r="A68" s="217" t="s">
         <v>187</v>
       </c>
       <c r="B68" s="17" t="s">
@@ -14564,7 +14330,7 @@
       </c>
     </row>
     <row r="69" spans="1:14">
-      <c r="A69" s="199"/>
+      <c r="A69" s="218"/>
       <c r="B69" s="17" t="s">
         <v>194</v>
       </c>
@@ -14606,7 +14372,7 @@
       </c>
     </row>
     <row r="70" spans="1:14">
-      <c r="A70" s="205"/>
+      <c r="A70" s="222"/>
       <c r="B70" s="17" t="s">
         <v>195</v>
       </c>
@@ -14648,7 +14414,7 @@
       </c>
     </row>
     <row r="71" spans="1:14">
-      <c r="A71" s="198" t="s">
+      <c r="A71" s="217" t="s">
         <v>188</v>
       </c>
       <c r="B71" s="17" t="s">
@@ -14692,7 +14458,7 @@
       </c>
     </row>
     <row r="72" spans="1:14">
-      <c r="A72" s="199"/>
+      <c r="A72" s="218"/>
       <c r="B72" s="17" t="s">
         <v>194</v>
       </c>
@@ -14734,7 +14500,7 @@
       </c>
     </row>
     <row r="73" spans="1:14">
-      <c r="A73" s="205"/>
+      <c r="A73" s="222"/>
       <c r="B73" s="17" t="s">
         <v>195</v>
       </c>
@@ -14776,7 +14542,7 @@
       </c>
     </row>
     <row r="74" spans="1:14">
-      <c r="A74" s="198" t="s">
+      <c r="A74" s="217" t="s">
         <v>189</v>
       </c>
       <c r="B74" s="17" t="s">
@@ -14820,7 +14586,7 @@
       </c>
     </row>
     <row r="75" spans="1:14">
-      <c r="A75" s="199"/>
+      <c r="A75" s="218"/>
       <c r="B75" s="17" t="s">
         <v>194</v>
       </c>
@@ -14862,7 +14628,7 @@
       </c>
     </row>
     <row r="76" spans="1:14">
-      <c r="A76" s="205"/>
+      <c r="A76" s="222"/>
       <c r="B76" s="17" t="s">
         <v>195</v>
       </c>
@@ -14904,7 +14670,7 @@
       </c>
     </row>
     <row r="77" spans="1:14">
-      <c r="A77" s="198" t="s">
+      <c r="A77" s="217" t="s">
         <v>190</v>
       </c>
       <c r="B77" s="17" t="s">
@@ -14948,7 +14714,7 @@
       </c>
     </row>
     <row r="78" spans="1:14">
-      <c r="A78" s="199"/>
+      <c r="A78" s="218"/>
       <c r="B78" s="17" t="s">
         <v>194</v>
       </c>
@@ -14990,7 +14756,7 @@
       </c>
     </row>
     <row r="79" spans="1:14">
-      <c r="A79" s="205"/>
+      <c r="A79" s="222"/>
       <c r="B79" s="17" t="s">
         <v>195</v>
       </c>
@@ -15032,7 +14798,7 @@
       </c>
     </row>
     <row r="80" spans="1:14">
-      <c r="A80" s="198" t="s">
+      <c r="A80" s="217" t="s">
         <v>191</v>
       </c>
       <c r="B80" s="17" t="s">
@@ -15076,7 +14842,7 @@
       </c>
     </row>
     <row r="81" spans="1:14">
-      <c r="A81" s="199"/>
+      <c r="A81" s="218"/>
       <c r="B81" s="17" t="s">
         <v>194</v>
       </c>
@@ -15118,7 +14884,7 @@
       </c>
     </row>
     <row r="82" spans="1:14">
-      <c r="A82" s="205"/>
+      <c r="A82" s="222"/>
       <c r="B82" s="17" t="s">
         <v>195</v>
       </c>
@@ -15160,7 +14926,7 @@
       </c>
     </row>
     <row r="83" spans="1:14">
-      <c r="A83" s="198" t="s">
+      <c r="A83" s="217" t="s">
         <v>198</v>
       </c>
       <c r="B83" s="17" t="s">
@@ -15204,7 +14970,7 @@
       </c>
     </row>
     <row r="84" spans="1:14">
-      <c r="A84" s="199"/>
+      <c r="A84" s="218"/>
       <c r="B84" s="17" t="s">
         <v>194</v>
       </c>
@@ -15246,7 +15012,7 @@
       </c>
     </row>
     <row r="85" spans="1:14">
-      <c r="A85" s="205"/>
+      <c r="A85" s="222"/>
       <c r="B85" s="17" t="s">
         <v>195</v>
       </c>
@@ -15288,7 +15054,7 @@
       </c>
     </row>
     <row r="86" spans="1:14">
-      <c r="A86" s="198" t="s">
+      <c r="A86" s="217" t="s">
         <v>199</v>
       </c>
       <c r="B86" s="17" t="s">
@@ -15332,7 +15098,7 @@
       </c>
     </row>
     <row r="87" spans="1:14">
-      <c r="A87" s="199"/>
+      <c r="A87" s="218"/>
       <c r="B87" s="17" t="s">
         <v>194</v>
       </c>
@@ -15374,7 +15140,7 @@
       </c>
     </row>
     <row r="88" spans="1:14">
-      <c r="A88" s="205"/>
+      <c r="A88" s="222"/>
       <c r="B88" s="17" t="s">
         <v>195</v>
       </c>
@@ -15416,7 +15182,7 @@
       </c>
     </row>
     <row r="89" spans="1:14">
-      <c r="A89" s="198" t="s">
+      <c r="A89" s="217" t="s">
         <v>200</v>
       </c>
       <c r="B89" s="17" t="s">
@@ -15460,7 +15226,7 @@
       </c>
     </row>
     <row r="90" spans="1:14">
-      <c r="A90" s="199"/>
+      <c r="A90" s="218"/>
       <c r="B90" s="17" t="s">
         <v>194</v>
       </c>
@@ -15502,7 +15268,7 @@
       </c>
     </row>
     <row r="91" spans="1:14">
-      <c r="A91" s="205"/>
+      <c r="A91" s="222"/>
       <c r="B91" s="17" t="s">
         <v>195</v>
       </c>
@@ -15544,7 +15310,7 @@
       </c>
     </row>
     <row r="92" spans="1:14">
-      <c r="A92" s="198" t="s">
+      <c r="A92" s="217" t="s">
         <v>201</v>
       </c>
       <c r="B92" s="17" t="s">
@@ -15588,7 +15354,7 @@
       </c>
     </row>
     <row r="93" spans="1:14">
-      <c r="A93" s="199"/>
+      <c r="A93" s="218"/>
       <c r="B93" s="17" t="s">
         <v>194</v>
       </c>
@@ -15630,7 +15396,7 @@
       </c>
     </row>
     <row r="94" spans="1:14">
-      <c r="A94" s="205"/>
+      <c r="A94" s="222"/>
       <c r="B94" s="17" t="s">
         <v>195</v>
       </c>
@@ -15672,7 +15438,7 @@
       </c>
     </row>
     <row r="95" spans="1:14">
-      <c r="A95" s="198" t="s">
+      <c r="A95" s="217" t="s">
         <v>202</v>
       </c>
       <c r="B95" s="17" t="s">
@@ -15716,7 +15482,7 @@
       </c>
     </row>
     <row r="96" spans="1:14">
-      <c r="A96" s="199"/>
+      <c r="A96" s="218"/>
       <c r="B96" s="17" t="s">
         <v>194</v>
       </c>
@@ -15758,7 +15524,7 @@
       </c>
     </row>
     <row r="97" spans="1:14">
-      <c r="A97" s="205"/>
+      <c r="A97" s="222"/>
       <c r="B97" s="17" t="s">
         <v>195</v>
       </c>
@@ -15800,7 +15566,7 @@
       </c>
     </row>
     <row r="98" spans="1:14">
-      <c r="A98" s="198" t="s">
+      <c r="A98" s="217" t="s">
         <v>203</v>
       </c>
       <c r="B98" s="17" t="s">
@@ -15844,7 +15610,7 @@
       </c>
     </row>
     <row r="99" spans="1:14">
-      <c r="A99" s="199"/>
+      <c r="A99" s="218"/>
       <c r="B99" s="17" t="s">
         <v>194</v>
       </c>
@@ -15886,7 +15652,7 @@
       </c>
     </row>
     <row r="100" spans="1:14">
-      <c r="A100" s="205"/>
+      <c r="A100" s="222"/>
       <c r="B100" s="17" t="s">
         <v>195</v>
       </c>
@@ -15928,7 +15694,7 @@
       </c>
     </row>
     <row r="101" spans="1:14">
-      <c r="A101" s="198" t="s">
+      <c r="A101" s="217" t="s">
         <v>204</v>
       </c>
       <c r="B101" s="17" t="s">
@@ -15972,7 +15738,7 @@
       </c>
     </row>
     <row r="102" spans="1:14">
-      <c r="A102" s="199"/>
+      <c r="A102" s="218"/>
       <c r="B102" s="17" t="s">
         <v>194</v>
       </c>
@@ -16014,7 +15780,7 @@
       </c>
     </row>
     <row r="103" spans="1:14">
-      <c r="A103" s="205"/>
+      <c r="A103" s="222"/>
       <c r="B103" s="17" t="s">
         <v>195</v>
       </c>
@@ -16100,7 +15866,7 @@
       </c>
     </row>
     <row r="105" spans="1:14">
-      <c r="A105" s="198" t="s">
+      <c r="A105" s="217" t="s">
         <v>212</v>
       </c>
       <c r="B105" s="17" t="s">
@@ -16144,7 +15910,7 @@
       </c>
     </row>
     <row r="106" spans="1:14">
-      <c r="A106" s="199"/>
+      <c r="A106" s="218"/>
       <c r="B106" s="17" t="s">
         <v>214</v>
       </c>
@@ -16187,32 +15953,6 @@
     </row>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="A98:A100"/>
-    <mergeCell ref="A101:A103"/>
-    <mergeCell ref="A77:A79"/>
-    <mergeCell ref="A80:A82"/>
-    <mergeCell ref="A83:A85"/>
-    <mergeCell ref="A86:A88"/>
-    <mergeCell ref="A89:A91"/>
-    <mergeCell ref="A92:A94"/>
-    <mergeCell ref="A95:A97"/>
-    <mergeCell ref="A27:A30"/>
-    <mergeCell ref="B27:B30"/>
-    <mergeCell ref="A31:A34"/>
-    <mergeCell ref="A59:A61"/>
-    <mergeCell ref="A62:A64"/>
-    <mergeCell ref="A14:A17"/>
-    <mergeCell ref="B14:B17"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="A23:A26"/>
-    <mergeCell ref="B23:B26"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="B10:B13"/>
     <mergeCell ref="A105:A106"/>
     <mergeCell ref="B31:B34"/>
     <mergeCell ref="A35:A38"/>
@@ -16229,6 +15969,32 @@
     <mergeCell ref="A65:A67"/>
     <mergeCell ref="A68:A70"/>
     <mergeCell ref="A71:A73"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="A23:A26"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="A27:A30"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="A31:A34"/>
+    <mergeCell ref="A59:A61"/>
+    <mergeCell ref="A62:A64"/>
+    <mergeCell ref="A98:A100"/>
+    <mergeCell ref="A101:A103"/>
+    <mergeCell ref="A77:A79"/>
+    <mergeCell ref="A80:A82"/>
+    <mergeCell ref="A83:A85"/>
+    <mergeCell ref="A86:A88"/>
+    <mergeCell ref="A89:A91"/>
+    <mergeCell ref="A92:A94"/>
+    <mergeCell ref="A95:A97"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -16304,7 +16070,7 @@
       </c>
     </row>
     <row r="2" spans="1:16" ht="13.5" customHeight="1">
-      <c r="A2" s="217" t="s">
+      <c r="A2" s="209" t="s">
         <v>165</v>
       </c>
       <c r="B2" s="210" t="s">
@@ -16354,7 +16120,7 @@
       </c>
     </row>
     <row r="3" spans="1:16">
-      <c r="A3" s="217"/>
+      <c r="A3" s="209"/>
       <c r="B3" s="210"/>
       <c r="C3" s="19" t="s">
         <v>167</v>
@@ -16400,7 +16166,7 @@
       </c>
     </row>
     <row r="4" spans="1:16">
-      <c r="A4" s="217"/>
+      <c r="A4" s="209"/>
       <c r="B4" s="210"/>
       <c r="C4" s="19" t="s">
         <v>168</v>
@@ -16446,7 +16212,7 @@
       </c>
     </row>
     <row r="5" spans="1:16">
-      <c r="A5" s="217"/>
+      <c r="A5" s="209"/>
       <c r="B5" s="210"/>
       <c r="C5" s="123" t="s">
         <v>169</v>
@@ -16492,7 +16258,7 @@
       </c>
     </row>
     <row r="6" spans="1:16" ht="13.5" customHeight="1">
-      <c r="A6" s="209" t="s">
+      <c r="A6" s="211" t="s">
         <v>170</v>
       </c>
       <c r="B6" s="210" t="s">
@@ -16542,7 +16308,7 @@
       </c>
     </row>
     <row r="7" spans="1:16">
-      <c r="A7" s="209"/>
+      <c r="A7" s="211"/>
       <c r="B7" s="210"/>
       <c r="C7" s="19" t="s">
         <v>167</v>
@@ -16588,7 +16354,7 @@
       </c>
     </row>
     <row r="8" spans="1:16">
-      <c r="A8" s="209"/>
+      <c r="A8" s="211"/>
       <c r="B8" s="210"/>
       <c r="C8" s="19" t="s">
         <v>168</v>
@@ -16634,7 +16400,7 @@
       </c>
     </row>
     <row r="9" spans="1:16">
-      <c r="A9" s="209"/>
+      <c r="A9" s="211"/>
       <c r="B9" s="210"/>
       <c r="C9" s="123" t="s">
         <v>169</v>
@@ -16680,10 +16446,10 @@
       </c>
     </row>
     <row r="10" spans="1:16">
-      <c r="A10" s="211" t="s">
+      <c r="A10" s="212" t="s">
         <v>172</v>
       </c>
-      <c r="B10" s="212" t="s">
+      <c r="B10" s="213" t="s">
         <v>173</v>
       </c>
       <c r="C10" s="115" t="s">
@@ -16730,8 +16496,8 @@
       </c>
     </row>
     <row r="11" spans="1:16">
-      <c r="A11" s="211"/>
-      <c r="B11" s="212"/>
+      <c r="A11" s="212"/>
+      <c r="B11" s="213"/>
       <c r="C11" s="19" t="s">
         <v>167</v>
       </c>
@@ -16776,8 +16542,8 @@
       </c>
     </row>
     <row r="12" spans="1:16">
-      <c r="A12" s="211"/>
-      <c r="B12" s="212"/>
+      <c r="A12" s="212"/>
+      <c r="B12" s="213"/>
       <c r="C12" s="19" t="s">
         <v>168</v>
       </c>
@@ -16822,8 +16588,8 @@
       </c>
     </row>
     <row r="13" spans="1:16">
-      <c r="A13" s="211"/>
-      <c r="B13" s="212"/>
+      <c r="A13" s="212"/>
+      <c r="B13" s="213"/>
       <c r="C13" s="144" t="s">
         <v>169</v>
       </c>
@@ -16868,10 +16634,10 @@
       </c>
     </row>
     <row r="14" spans="1:16">
-      <c r="A14" s="209" t="s">
+      <c r="A14" s="211" t="s">
         <v>174</v>
       </c>
-      <c r="B14" s="213" t="s">
+      <c r="B14" s="214" t="s">
         <v>173</v>
       </c>
       <c r="C14" s="115" t="s">
@@ -16919,8 +16685,8 @@
       </c>
     </row>
     <row r="15" spans="1:16">
-      <c r="A15" s="209"/>
-      <c r="B15" s="213"/>
+      <c r="A15" s="211"/>
+      <c r="B15" s="214"/>
       <c r="C15" s="149" t="s">
         <v>167</v>
       </c>
@@ -16966,8 +16732,8 @@
       </c>
     </row>
     <row r="16" spans="1:16">
-      <c r="A16" s="209"/>
-      <c r="B16" s="213"/>
+      <c r="A16" s="211"/>
+      <c r="B16" s="214"/>
       <c r="C16" s="149" t="s">
         <v>168</v>
       </c>
@@ -17013,8 +16779,8 @@
       </c>
     </row>
     <row r="17" spans="1:16">
-      <c r="A17" s="209"/>
-      <c r="B17" s="213"/>
+      <c r="A17" s="211"/>
+      <c r="B17" s="214"/>
       <c r="C17" s="150" t="s">
         <v>169</v>
       </c>
@@ -17080,10 +16846,10 @@
       <c r="P18" s="155"/>
     </row>
     <row r="19" spans="1:16">
-      <c r="A19" s="200" t="s">
+      <c r="A19" s="215" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="201" t="s">
+      <c r="B19" s="216" t="s">
         <v>173</v>
       </c>
       <c r="C19" s="19" t="s">
@@ -17130,8 +16896,8 @@
       </c>
     </row>
     <row r="20" spans="1:16">
-      <c r="A20" s="200"/>
-      <c r="B20" s="201"/>
+      <c r="A20" s="215"/>
+      <c r="B20" s="216"/>
       <c r="C20" s="19" t="s">
         <v>167</v>
       </c>
@@ -17176,8 +16942,8 @@
       </c>
     </row>
     <row r="21" spans="1:16">
-      <c r="A21" s="200"/>
-      <c r="B21" s="201"/>
+      <c r="A21" s="215"/>
+      <c r="B21" s="216"/>
       <c r="C21" s="19" t="s">
         <v>168</v>
       </c>
@@ -17222,8 +16988,8 @@
       </c>
     </row>
     <row r="22" spans="1:16">
-      <c r="A22" s="200"/>
-      <c r="B22" s="201"/>
+      <c r="A22" s="215"/>
+      <c r="B22" s="216"/>
       <c r="C22" s="19" t="s">
         <v>169</v>
       </c>
@@ -17268,10 +17034,10 @@
       </c>
     </row>
     <row r="23" spans="1:16">
-      <c r="A23" s="200" t="s">
+      <c r="A23" s="215" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="201" t="s">
+      <c r="B23" s="216" t="s">
         <v>173</v>
       </c>
       <c r="C23" s="157" t="s">
@@ -17318,8 +17084,8 @@
       </c>
     </row>
     <row r="24" spans="1:16">
-      <c r="A24" s="200"/>
-      <c r="B24" s="201"/>
+      <c r="A24" s="215"/>
+      <c r="B24" s="216"/>
       <c r="C24" s="19" t="s">
         <v>167</v>
       </c>
@@ -17364,8 +17130,8 @@
       </c>
     </row>
     <row r="25" spans="1:16">
-      <c r="A25" s="200"/>
-      <c r="B25" s="201"/>
+      <c r="A25" s="215"/>
+      <c r="B25" s="216"/>
       <c r="C25" s="19" t="s">
         <v>168</v>
       </c>
@@ -17410,8 +17176,8 @@
       </c>
     </row>
     <row r="26" spans="1:16">
-      <c r="A26" s="200"/>
-      <c r="B26" s="201"/>
+      <c r="A26" s="215"/>
+      <c r="B26" s="216"/>
       <c r="C26" s="19" t="s">
         <v>169</v>
       </c>
@@ -17456,10 +17222,10 @@
       </c>
     </row>
     <row r="27" spans="1:16">
-      <c r="A27" s="200" t="s">
+      <c r="A27" s="215" t="s">
         <v>10</v>
       </c>
-      <c r="B27" s="201" t="s">
+      <c r="B27" s="216" t="s">
         <v>173</v>
       </c>
       <c r="C27" s="19" t="s">
@@ -17506,8 +17272,8 @@
       </c>
     </row>
     <row r="28" spans="1:16">
-      <c r="A28" s="200"/>
-      <c r="B28" s="201"/>
+      <c r="A28" s="215"/>
+      <c r="B28" s="216"/>
       <c r="C28" s="19" t="s">
         <v>167</v>
       </c>
@@ -17552,8 +17318,8 @@
       </c>
     </row>
     <row r="29" spans="1:16">
-      <c r="A29" s="200"/>
-      <c r="B29" s="201"/>
+      <c r="A29" s="215"/>
+      <c r="B29" s="216"/>
       <c r="C29" s="19" t="s">
         <v>168</v>
       </c>
@@ -17598,8 +17364,8 @@
       </c>
     </row>
     <row r="30" spans="1:16">
-      <c r="A30" s="200"/>
-      <c r="B30" s="201"/>
+      <c r="A30" s="215"/>
+      <c r="B30" s="216"/>
       <c r="C30" s="19" t="s">
         <v>169</v>
       </c>
@@ -17644,10 +17410,10 @@
       </c>
     </row>
     <row r="31" spans="1:16">
-      <c r="A31" s="200" t="s">
+      <c r="A31" s="215" t="s">
         <v>11</v>
       </c>
-      <c r="B31" s="201" t="s">
+      <c r="B31" s="216" t="s">
         <v>173</v>
       </c>
       <c r="C31" s="19" t="s">
@@ -17694,8 +17460,8 @@
       </c>
     </row>
     <row r="32" spans="1:16">
-      <c r="A32" s="200"/>
-      <c r="B32" s="201"/>
+      <c r="A32" s="215"/>
+      <c r="B32" s="216"/>
       <c r="C32" s="19" t="s">
         <v>167</v>
       </c>
@@ -17740,8 +17506,8 @@
       </c>
     </row>
     <row r="33" spans="1:16">
-      <c r="A33" s="200"/>
-      <c r="B33" s="201"/>
+      <c r="A33" s="215"/>
+      <c r="B33" s="216"/>
       <c r="C33" s="19" t="s">
         <v>168</v>
       </c>
@@ -17786,8 +17552,8 @@
       </c>
     </row>
     <row r="34" spans="1:16">
-      <c r="A34" s="200"/>
-      <c r="B34" s="201"/>
+      <c r="A34" s="215"/>
+      <c r="B34" s="216"/>
       <c r="C34" s="19" t="s">
         <v>169</v>
       </c>
@@ -17832,10 +17598,10 @@
       </c>
     </row>
     <row r="35" spans="1:16">
-      <c r="A35" s="200" t="s">
+      <c r="A35" s="215" t="s">
         <v>12</v>
       </c>
-      <c r="B35" s="201" t="s">
+      <c r="B35" s="216" t="s">
         <v>173</v>
       </c>
       <c r="C35" s="19" t="s">
@@ -17882,8 +17648,8 @@
       </c>
     </row>
     <row r="36" spans="1:16">
-      <c r="A36" s="200"/>
-      <c r="B36" s="201"/>
+      <c r="A36" s="215"/>
+      <c r="B36" s="216"/>
       <c r="C36" s="19" t="s">
         <v>167</v>
       </c>
@@ -17928,8 +17694,8 @@
       </c>
     </row>
     <row r="37" spans="1:16">
-      <c r="A37" s="200"/>
-      <c r="B37" s="201"/>
+      <c r="A37" s="215"/>
+      <c r="B37" s="216"/>
       <c r="C37" s="19" t="s">
         <v>168</v>
       </c>
@@ -17974,8 +17740,8 @@
       </c>
     </row>
     <row r="38" spans="1:16">
-      <c r="A38" s="200"/>
-      <c r="B38" s="201"/>
+      <c r="A38" s="215"/>
+      <c r="B38" s="216"/>
       <c r="C38" s="19" t="s">
         <v>169</v>
       </c>
@@ -18020,10 +17786,10 @@
       </c>
     </row>
     <row r="39" spans="1:16">
-      <c r="A39" s="200" t="s">
+      <c r="A39" s="215" t="s">
         <v>13</v>
       </c>
-      <c r="B39" s="201" t="s">
+      <c r="B39" s="216" t="s">
         <v>173</v>
       </c>
       <c r="C39" s="19" t="s">
@@ -18070,8 +17836,8 @@
       </c>
     </row>
     <row r="40" spans="1:16">
-      <c r="A40" s="200"/>
-      <c r="B40" s="201"/>
+      <c r="A40" s="215"/>
+      <c r="B40" s="216"/>
       <c r="C40" s="19" t="s">
         <v>167</v>
       </c>
@@ -18116,8 +17882,8 @@
       </c>
     </row>
     <row r="41" spans="1:16">
-      <c r="A41" s="200"/>
-      <c r="B41" s="201"/>
+      <c r="A41" s="215"/>
+      <c r="B41" s="216"/>
       <c r="C41" s="19" t="s">
         <v>168</v>
       </c>
@@ -18162,8 +17928,8 @@
       </c>
     </row>
     <row r="42" spans="1:16">
-      <c r="A42" s="200"/>
-      <c r="B42" s="201"/>
+      <c r="A42" s="215"/>
+      <c r="B42" s="216"/>
       <c r="C42" s="19" t="s">
         <v>169</v>
       </c>
@@ -18208,10 +17974,10 @@
       </c>
     </row>
     <row r="43" spans="1:16">
-      <c r="A43" s="200" t="s">
+      <c r="A43" s="215" t="s">
         <v>14</v>
       </c>
-      <c r="B43" s="201" t="s">
+      <c r="B43" s="216" t="s">
         <v>173</v>
       </c>
       <c r="C43" s="19" t="s">
@@ -18258,8 +18024,8 @@
       </c>
     </row>
     <row r="44" spans="1:16">
-      <c r="A44" s="200"/>
-      <c r="B44" s="201"/>
+      <c r="A44" s="215"/>
+      <c r="B44" s="216"/>
       <c r="C44" s="19" t="s">
         <v>167</v>
       </c>
@@ -18304,8 +18070,8 @@
       </c>
     </row>
     <row r="45" spans="1:16">
-      <c r="A45" s="200"/>
-      <c r="B45" s="201"/>
+      <c r="A45" s="215"/>
+      <c r="B45" s="216"/>
       <c r="C45" s="19" t="s">
         <v>168</v>
       </c>
@@ -18350,8 +18116,8 @@
       </c>
     </row>
     <row r="46" spans="1:16">
-      <c r="A46" s="200"/>
-      <c r="B46" s="201"/>
+      <c r="A46" s="215"/>
+      <c r="B46" s="216"/>
       <c r="C46" s="19" t="s">
         <v>169</v>
       </c>
@@ -18396,10 +18162,10 @@
       </c>
     </row>
     <row r="47" spans="1:16">
-      <c r="A47" s="202" t="s">
+      <c r="A47" s="219" t="s">
         <v>15</v>
       </c>
-      <c r="B47" s="201" t="s">
+      <c r="B47" s="216" t="s">
         <v>173</v>
       </c>
       <c r="C47" s="19" t="s">
@@ -18446,8 +18212,8 @@
       </c>
     </row>
     <row r="48" spans="1:16">
-      <c r="A48" s="202"/>
-      <c r="B48" s="201"/>
+      <c r="A48" s="219"/>
+      <c r="B48" s="216"/>
       <c r="C48" s="19" t="s">
         <v>167</v>
       </c>
@@ -18492,8 +18258,8 @@
       </c>
     </row>
     <row r="49" spans="1:23">
-      <c r="A49" s="202"/>
-      <c r="B49" s="201"/>
+      <c r="A49" s="219"/>
+      <c r="B49" s="216"/>
       <c r="C49" s="19" t="s">
         <v>168</v>
       </c>
@@ -18538,8 +18304,8 @@
       </c>
     </row>
     <row r="50" spans="1:23">
-      <c r="A50" s="202"/>
-      <c r="B50" s="201"/>
+      <c r="A50" s="219"/>
+      <c r="B50" s="216"/>
       <c r="C50" s="19" t="s">
         <v>169</v>
       </c>
@@ -18584,10 +18350,10 @@
       </c>
     </row>
     <row r="51" spans="1:23">
-      <c r="A51" s="203" t="s">
+      <c r="A51" s="220" t="s">
         <v>16</v>
       </c>
-      <c r="B51" s="204" t="s">
+      <c r="B51" s="221" t="s">
         <v>173</v>
       </c>
       <c r="C51" s="19" t="s">
@@ -18634,8 +18400,8 @@
       </c>
     </row>
     <row r="52" spans="1:23">
-      <c r="A52" s="203"/>
-      <c r="B52" s="204"/>
+      <c r="A52" s="220"/>
+      <c r="B52" s="221"/>
       <c r="C52" s="19" t="s">
         <v>167</v>
       </c>
@@ -18680,8 +18446,8 @@
       </c>
     </row>
     <row r="53" spans="1:23">
-      <c r="A53" s="203"/>
-      <c r="B53" s="204"/>
+      <c r="A53" s="220"/>
+      <c r="B53" s="221"/>
       <c r="C53" s="19" t="s">
         <v>168</v>
       </c>
@@ -18726,8 +18492,8 @@
       </c>
     </row>
     <row r="54" spans="1:23">
-      <c r="A54" s="203"/>
-      <c r="B54" s="204"/>
+      <c r="A54" s="220"/>
+      <c r="B54" s="221"/>
       <c r="C54" s="123" t="s">
         <v>169</v>
       </c>
@@ -18772,10 +18538,10 @@
       </c>
     </row>
     <row r="58" spans="1:23">
-      <c r="A58" s="226" t="s">
+      <c r="A58" s="223" t="s">
         <v>176</v>
       </c>
-      <c r="B58" s="226"/>
+      <c r="B58" s="223"/>
       <c r="C58" s="19">
         <v>1995</v>
       </c>
@@ -19098,7 +18864,7 @@
       </c>
     </row>
     <row r="65" spans="1:14">
-      <c r="A65" s="198" t="s">
+      <c r="A65" s="217" t="s">
         <v>196</v>
       </c>
       <c r="B65" s="17" t="s">
@@ -19142,7 +18908,7 @@
       </c>
     </row>
     <row r="66" spans="1:14">
-      <c r="A66" s="199"/>
+      <c r="A66" s="218"/>
       <c r="B66" s="17" t="s">
         <v>194</v>
       </c>
@@ -19184,7 +18950,7 @@
       </c>
     </row>
     <row r="67" spans="1:14">
-      <c r="A67" s="205"/>
+      <c r="A67" s="222"/>
       <c r="B67" s="17" t="s">
         <v>195</v>
       </c>
@@ -19226,7 +18992,7 @@
       </c>
     </row>
     <row r="68" spans="1:14">
-      <c r="A68" s="198" t="s">
+      <c r="A68" s="217" t="s">
         <v>197</v>
       </c>
       <c r="B68" s="17" t="s">
@@ -19270,7 +19036,7 @@
       </c>
     </row>
     <row r="69" spans="1:14">
-      <c r="A69" s="199"/>
+      <c r="A69" s="218"/>
       <c r="B69" s="17" t="s">
         <v>194</v>
       </c>
@@ -19312,7 +19078,7 @@
       </c>
     </row>
     <row r="70" spans="1:14">
-      <c r="A70" s="205"/>
+      <c r="A70" s="222"/>
       <c r="B70" s="17" t="s">
         <v>195</v>
       </c>
@@ -19354,7 +19120,7 @@
       </c>
     </row>
     <row r="71" spans="1:14">
-      <c r="A71" s="198" t="s">
+      <c r="A71" s="217" t="s">
         <v>186</v>
       </c>
       <c r="B71" s="17" t="s">
@@ -19398,7 +19164,7 @@
       </c>
     </row>
     <row r="72" spans="1:14">
-      <c r="A72" s="199"/>
+      <c r="A72" s="218"/>
       <c r="B72" s="17" t="s">
         <v>194</v>
       </c>
@@ -19440,7 +19206,7 @@
       </c>
     </row>
     <row r="73" spans="1:14">
-      <c r="A73" s="205"/>
+      <c r="A73" s="222"/>
       <c r="B73" s="17" t="s">
         <v>195</v>
       </c>
@@ -19482,7 +19248,7 @@
       </c>
     </row>
     <row r="74" spans="1:14">
-      <c r="A74" s="198" t="s">
+      <c r="A74" s="217" t="s">
         <v>187</v>
       </c>
       <c r="B74" s="17" t="s">
@@ -19526,7 +19292,7 @@
       </c>
     </row>
     <row r="75" spans="1:14">
-      <c r="A75" s="199"/>
+      <c r="A75" s="218"/>
       <c r="B75" s="17" t="s">
         <v>194</v>
       </c>
@@ -19568,7 +19334,7 @@
       </c>
     </row>
     <row r="76" spans="1:14">
-      <c r="A76" s="205"/>
+      <c r="A76" s="222"/>
       <c r="B76" s="17" t="s">
         <v>195</v>
       </c>
@@ -19610,7 +19376,7 @@
       </c>
     </row>
     <row r="77" spans="1:14">
-      <c r="A77" s="198" t="s">
+      <c r="A77" s="217" t="s">
         <v>188</v>
       </c>
       <c r="B77" s="17" t="s">
@@ -19654,7 +19420,7 @@
       </c>
     </row>
     <row r="78" spans="1:14">
-      <c r="A78" s="199"/>
+      <c r="A78" s="218"/>
       <c r="B78" s="17" t="s">
         <v>194</v>
       </c>
@@ -19696,7 +19462,7 @@
       </c>
     </row>
     <row r="79" spans="1:14">
-      <c r="A79" s="205"/>
+      <c r="A79" s="222"/>
       <c r="B79" s="17" t="s">
         <v>195</v>
       </c>
@@ -19738,7 +19504,7 @@
       </c>
     </row>
     <row r="80" spans="1:14">
-      <c r="A80" s="198" t="s">
+      <c r="A80" s="217" t="s">
         <v>189</v>
       </c>
       <c r="B80" s="17" t="s">
@@ -19782,7 +19548,7 @@
       </c>
     </row>
     <row r="81" spans="1:14">
-      <c r="A81" s="199"/>
+      <c r="A81" s="218"/>
       <c r="B81" s="17" t="s">
         <v>194</v>
       </c>
@@ -19824,7 +19590,7 @@
       </c>
     </row>
     <row r="82" spans="1:14">
-      <c r="A82" s="205"/>
+      <c r="A82" s="222"/>
       <c r="B82" s="17" t="s">
         <v>195</v>
       </c>
@@ -19866,7 +19632,7 @@
       </c>
     </row>
     <row r="83" spans="1:14">
-      <c r="A83" s="198" t="s">
+      <c r="A83" s="217" t="s">
         <v>190</v>
       </c>
       <c r="B83" s="17" t="s">
@@ -19910,7 +19676,7 @@
       </c>
     </row>
     <row r="84" spans="1:14">
-      <c r="A84" s="199"/>
+      <c r="A84" s="218"/>
       <c r="B84" s="17" t="s">
         <v>194</v>
       </c>
@@ -19952,7 +19718,7 @@
       </c>
     </row>
     <row r="85" spans="1:14">
-      <c r="A85" s="205"/>
+      <c r="A85" s="222"/>
       <c r="B85" s="17" t="s">
         <v>195</v>
       </c>
@@ -19994,7 +19760,7 @@
       </c>
     </row>
     <row r="86" spans="1:14">
-      <c r="A86" s="198" t="s">
+      <c r="A86" s="217" t="s">
         <v>191</v>
       </c>
       <c r="B86" s="17" t="s">
@@ -20038,7 +19804,7 @@
       </c>
     </row>
     <row r="87" spans="1:14">
-      <c r="A87" s="199"/>
+      <c r="A87" s="218"/>
       <c r="B87" s="17" t="s">
         <v>194</v>
       </c>
@@ -20080,7 +19846,7 @@
       </c>
     </row>
     <row r="88" spans="1:14">
-      <c r="A88" s="205"/>
+      <c r="A88" s="222"/>
       <c r="B88" s="17" t="s">
         <v>195</v>
       </c>
@@ -20122,7 +19888,7 @@
       </c>
     </row>
     <row r="89" spans="1:14">
-      <c r="A89" s="198" t="s">
+      <c r="A89" s="217" t="s">
         <v>198</v>
       </c>
       <c r="B89" s="17" t="s">
@@ -20166,7 +19932,7 @@
       </c>
     </row>
     <row r="90" spans="1:14">
-      <c r="A90" s="199"/>
+      <c r="A90" s="218"/>
       <c r="B90" s="17" t="s">
         <v>194</v>
       </c>
@@ -20208,7 +19974,7 @@
       </c>
     </row>
     <row r="91" spans="1:14">
-      <c r="A91" s="205"/>
+      <c r="A91" s="222"/>
       <c r="B91" s="17" t="s">
         <v>195</v>
       </c>
@@ -20250,7 +20016,7 @@
       </c>
     </row>
     <row r="92" spans="1:14">
-      <c r="A92" s="198" t="s">
+      <c r="A92" s="217" t="s">
         <v>199</v>
       </c>
       <c r="B92" s="17" t="s">
@@ -20294,7 +20060,7 @@
       </c>
     </row>
     <row r="93" spans="1:14">
-      <c r="A93" s="199"/>
+      <c r="A93" s="218"/>
       <c r="B93" s="17" t="s">
         <v>194</v>
       </c>
@@ -20336,7 +20102,7 @@
       </c>
     </row>
     <row r="94" spans="1:14" ht="16.5" customHeight="1">
-      <c r="A94" s="205"/>
+      <c r="A94" s="222"/>
       <c r="B94" s="17" t="s">
         <v>195</v>
       </c>
@@ -20378,7 +20144,7 @@
       </c>
     </row>
     <row r="95" spans="1:14">
-      <c r="A95" s="198" t="s">
+      <c r="A95" s="217" t="s">
         <v>200</v>
       </c>
       <c r="B95" s="17" t="s">
@@ -20422,7 +20188,7 @@
       </c>
     </row>
     <row r="96" spans="1:14">
-      <c r="A96" s="199"/>
+      <c r="A96" s="218"/>
       <c r="B96" s="17" t="s">
         <v>194</v>
       </c>
@@ -20464,7 +20230,7 @@
       </c>
     </row>
     <row r="97" spans="1:14">
-      <c r="A97" s="205"/>
+      <c r="A97" s="222"/>
       <c r="B97" s="17" t="s">
         <v>195</v>
       </c>
@@ -20506,7 +20272,7 @@
       </c>
     </row>
     <row r="98" spans="1:14">
-      <c r="A98" s="198" t="s">
+      <c r="A98" s="217" t="s">
         <v>201</v>
       </c>
       <c r="B98" s="17" t="s">
@@ -20550,7 +20316,7 @@
       </c>
     </row>
     <row r="99" spans="1:14">
-      <c r="A99" s="199"/>
+      <c r="A99" s="218"/>
       <c r="B99" s="17" t="s">
         <v>194</v>
       </c>
@@ -20592,7 +20358,7 @@
       </c>
     </row>
     <row r="100" spans="1:14">
-      <c r="A100" s="205"/>
+      <c r="A100" s="222"/>
       <c r="B100" s="17" t="s">
         <v>195</v>
       </c>
@@ -20634,7 +20400,7 @@
       </c>
     </row>
     <row r="101" spans="1:14">
-      <c r="A101" s="198" t="s">
+      <c r="A101" s="217" t="s">
         <v>202</v>
       </c>
       <c r="B101" s="17" t="s">
@@ -20678,7 +20444,7 @@
       </c>
     </row>
     <row r="102" spans="1:14">
-      <c r="A102" s="199"/>
+      <c r="A102" s="218"/>
       <c r="B102" s="17" t="s">
         <v>194</v>
       </c>
@@ -20720,7 +20486,7 @@
       </c>
     </row>
     <row r="103" spans="1:14">
-      <c r="A103" s="205"/>
+      <c r="A103" s="222"/>
       <c r="B103" s="17" t="s">
         <v>195</v>
       </c>
@@ -20762,7 +20528,7 @@
       </c>
     </row>
     <row r="104" spans="1:14">
-      <c r="A104" s="198" t="s">
+      <c r="A104" s="217" t="s">
         <v>203</v>
       </c>
       <c r="B104" s="17" t="s">
@@ -20806,7 +20572,7 @@
       </c>
     </row>
     <row r="105" spans="1:14">
-      <c r="A105" s="199"/>
+      <c r="A105" s="218"/>
       <c r="B105" s="17" t="s">
         <v>194</v>
       </c>
@@ -20848,7 +20614,7 @@
       </c>
     </row>
     <row r="106" spans="1:14">
-      <c r="A106" s="205"/>
+      <c r="A106" s="222"/>
       <c r="B106" s="17" t="s">
         <v>195</v>
       </c>
@@ -20890,7 +20656,7 @@
       </c>
     </row>
     <row r="107" spans="1:14">
-      <c r="A107" s="198" t="s">
+      <c r="A107" s="217" t="s">
         <v>204</v>
       </c>
       <c r="B107" s="17" t="s">
@@ -20934,7 +20700,7 @@
       </c>
     </row>
     <row r="108" spans="1:14">
-      <c r="A108" s="199"/>
+      <c r="A108" s="218"/>
       <c r="B108" s="17" t="s">
         <v>194</v>
       </c>
@@ -20976,7 +20742,7 @@
       </c>
     </row>
     <row r="109" spans="1:14">
-      <c r="A109" s="205"/>
+      <c r="A109" s="222"/>
       <c r="B109" s="17" t="s">
         <v>195</v>
       </c>
@@ -21062,7 +20828,7 @@
       </c>
     </row>
     <row r="111" spans="1:14">
-      <c r="A111" s="198" t="s">
+      <c r="A111" s="217" t="s">
         <v>212</v>
       </c>
       <c r="B111" s="17" t="s">
@@ -21106,7 +20872,7 @@
       </c>
     </row>
     <row r="112" spans="1:14">
-      <c r="A112" s="199"/>
+      <c r="A112" s="218"/>
       <c r="B112" s="17" t="s">
         <v>214</v>
       </c>
@@ -21149,33 +20915,6 @@
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="A89:A91"/>
-    <mergeCell ref="A92:A94"/>
-    <mergeCell ref="A95:A97"/>
-    <mergeCell ref="A98:A100"/>
-    <mergeCell ref="A101:A103"/>
-    <mergeCell ref="A27:A30"/>
-    <mergeCell ref="B27:B30"/>
-    <mergeCell ref="A31:A34"/>
-    <mergeCell ref="A65:A67"/>
-    <mergeCell ref="A68:A70"/>
-    <mergeCell ref="B31:B34"/>
-    <mergeCell ref="A35:A38"/>
-    <mergeCell ref="B35:B38"/>
-    <mergeCell ref="A51:A54"/>
-    <mergeCell ref="B51:B54"/>
-    <mergeCell ref="A14:A17"/>
-    <mergeCell ref="B14:B17"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="A23:A26"/>
-    <mergeCell ref="B23:B26"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="B10:B13"/>
     <mergeCell ref="A111:A112"/>
     <mergeCell ref="A58:B58"/>
     <mergeCell ref="A39:A42"/>
@@ -21192,6 +20931,33 @@
     <mergeCell ref="A107:A109"/>
     <mergeCell ref="A83:A85"/>
     <mergeCell ref="A86:A88"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="A23:A26"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="A27:A30"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="A31:A34"/>
+    <mergeCell ref="A65:A67"/>
+    <mergeCell ref="A68:A70"/>
+    <mergeCell ref="B31:B34"/>
+    <mergeCell ref="A35:A38"/>
+    <mergeCell ref="B35:B38"/>
+    <mergeCell ref="A51:A54"/>
+    <mergeCell ref="B51:B54"/>
+    <mergeCell ref="A89:A91"/>
+    <mergeCell ref="A92:A94"/>
+    <mergeCell ref="A95:A97"/>
+    <mergeCell ref="A98:A100"/>
+    <mergeCell ref="A101:A103"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>